<commit_message>
did something about sights and the gun. Did not finished.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,14 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="bronbiala" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="granaty" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="lunety" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="celowniki" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="celowniki" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -89,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2773" uniqueCount="760">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2209,6 +2208,9 @@
     <t xml:space="preserve">Min</t>
   </si>
   <si>
+    <t xml:space="preserve">specjalne</t>
+  </si>
+  <si>
     <t xml:space="preserve">Waga</t>
   </si>
   <si>
@@ -2218,6 +2220,9 @@
     <t xml:space="preserve">ACOGx1,5</t>
   </si>
   <si>
+    <t xml:space="preserve">siatka dyfrakcyjna, 2xtaniej, negowanie</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACOGx3</t>
   </si>
   <si>
@@ -2236,6 +2241,9 @@
     <t xml:space="preserve">x3</t>
   </si>
   <si>
+    <t xml:space="preserve">negowanie, Do Złącznienia</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.4</t>
   </si>
   <si>
@@ -2332,9 +2340,6 @@
     <t xml:space="preserve">Tani I stabilny</t>
   </si>
   <si>
-    <t xml:space="preserve">x2</t>
-  </si>
-  <si>
     <t xml:space="preserve">taniAdobry</t>
   </si>
   <si>
@@ -2360,6 +2365,9 @@
   </si>
   <si>
     <t xml:space="preserve">pistolety mają ten modyfikator zawsze, dla muszki i szczerbinki.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wszystkie półlunety i holografy, posiadają od razu siatkę dyfrakcyjną, oraz są profesjonalne i bardzo ciężko jest je zniszczyć (jak na lunety). Do tego wszystkie ACOGi mają dodatki do celowników w momencie zakupu za pół ceny. Dodatkowo przed pierwszym przyrostem znajduje się pole, w którym jest za blisko aby skorzystać z danego celownika. Jest to Min( wyrażany w metrach). Jednocześnie ten zasięg możesz ignorować i dopiero stosujesz przyrosty zasięgu. Musisz poświęcić fazę, za każdy przyrost zasięgu celownika ignorowanego w ten sposób zasięgu. Np. strzelając ze SCARa –L do wroga oddalonego o 41m z celownikiem ACOGx3, strzelasz jakbyś był w pierwszym zasięgu (jeśli odczekasz dodatkową fazę). Działa tylko w trybie pojedyncze. Strzelając serią nie ignorujesz tego dystansu. Czyli ten sam strzelec strzelając od razu, albo odczekując moment i strzelając serią tego bonusu się nie aplikuje. </t>
   </si>
 </sst>
 </file>
@@ -2372,7 +2380,7 @@
     <numFmt numFmtId="166" formatCode="d/mmm"/>
     <numFmt numFmtId="167" formatCode="mm/dd"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2483,6 +2491,21 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -2783,7 +2806,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="119">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3244,8 +3267,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3327,11 +3362,11 @@
   </sheetPr>
   <dimension ref="A1:P300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.01"/>
@@ -3346,7 +3381,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15851,7 +15886,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
@@ -16855,7 +16890,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="103" t="s">
@@ -17161,13 +17196,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="81.01"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="102" t="s">
@@ -17182,16 +17222,19 @@
       <c r="D1" s="102" t="s">
         <v>705</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="0" t="s">
         <v>706</v>
       </c>
       <c r="F1" s="102" t="s">
         <v>707</v>
       </c>
+      <c r="G1" s="102" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="102" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B2" s="102" t="n">
         <v>3</v>
@@ -17202,16 +17245,19 @@
       <c r="D2" s="102" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="102" t="n">
+      <c r="E2" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="F2" s="102" t="n">
         <v>0.4</v>
       </c>
-      <c r="F2" s="102" t="n">
+      <c r="G2" s="102" t="n">
         <v>1300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="102" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B3" s="102" t="n">
         <v>3</v>
@@ -17222,16 +17268,19 @@
       <c r="D3" s="102" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="102" t="n">
+      <c r="E3" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="F3" s="102" t="n">
         <v>0.4</v>
       </c>
-      <c r="F3" s="102" t="n">
+      <c r="G3" s="102" t="n">
         <v>1600</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="102" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B4" s="102" t="n">
         <v>3</v>
@@ -17242,16 +17291,19 @@
       <c r="D4" s="102" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="102" t="n">
+      <c r="E4" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="F4" s="102" t="n">
         <v>0.4</v>
       </c>
-      <c r="F4" s="102" t="n">
+      <c r="G4" s="102" t="n">
         <v>1700</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="102" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B5" s="102" t="n">
         <v>3</v>
@@ -17262,16 +17314,19 @@
       <c r="D5" s="102" t="n">
         <v>30</v>
       </c>
-      <c r="E5" s="102" t="n">
+      <c r="E5" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="F5" s="102" t="n">
         <v>0.4</v>
       </c>
-      <c r="F5" s="102" t="n">
+      <c r="G5" s="102" t="n">
         <v>2800</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="102" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B6" s="102" t="n">
         <v>2</v>
@@ -17282,16 +17337,19 @@
       <c r="D6" s="102" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="102" t="n">
+      <c r="E6" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="F6" s="102" t="n">
         <v>0.4</v>
       </c>
-      <c r="F6" s="102" t="n">
+      <c r="G6" s="102" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="102" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B7" s="102" t="n">
         <v>3</v>
@@ -17302,16 +17360,19 @@
       <c r="D7" s="102" t="n">
         <v>18</v>
       </c>
-      <c r="E7" s="102" t="n">
+      <c r="E7" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="F7" s="102" t="n">
         <v>0.4</v>
       </c>
-      <c r="F7" s="102" t="n">
+      <c r="G7" s="102" t="n">
         <v>1500</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="102" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B8" s="102" t="n">
         <v>3</v>
@@ -17322,16 +17383,19 @@
       <c r="D8" s="102" t="n">
         <v>15</v>
       </c>
-      <c r="E8" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="F8" s="102" t="n">
+      <c r="E8" s="115" t="s">
+        <v>717</v>
+      </c>
+      <c r="F8" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G8" s="102" t="n">
         <v>600</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="102" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="B9" s="102" t="n">
         <v>3</v>
@@ -17342,16 +17406,19 @@
       <c r="D9" s="102" t="n">
         <v>40</v>
       </c>
-      <c r="E9" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="F9" s="102" t="n">
+      <c r="E9" s="115" t="s">
+        <v>717</v>
+      </c>
+      <c r="F9" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G9" s="102" t="n">
         <v>800</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="102" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B10" s="102" t="n">
         <v>3</v>
@@ -17362,16 +17429,19 @@
       <c r="D10" s="102" t="n">
         <v>80</v>
       </c>
-      <c r="E10" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="F10" s="102" t="n">
+      <c r="E10" s="115" t="s">
+        <v>717</v>
+      </c>
+      <c r="F10" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G10" s="102" t="n">
         <v>900</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="102" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="B11" s="102" t="n">
         <v>3</v>
@@ -17382,16 +17452,19 @@
       <c r="D11" s="102" t="n">
         <v>100</v>
       </c>
-      <c r="E11" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="F11" s="102" t="n">
+      <c r="E11" s="115" t="s">
+        <v>717</v>
+      </c>
+      <c r="F11" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G11" s="102" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="102" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B12" s="102" t="n">
         <v>3</v>
@@ -17402,16 +17475,19 @@
       <c r="D12" s="102" t="n">
         <v>200</v>
       </c>
-      <c r="E12" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="F12" s="102" t="n">
+      <c r="E12" s="115" t="s">
+        <v>717</v>
+      </c>
+      <c r="F12" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G12" s="102" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="102" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="B13" s="102" t="n">
         <v>3</v>
@@ -17422,350 +17498,331 @@
       <c r="D13" s="102" t="n">
         <v>400</v>
       </c>
-      <c r="E13" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="F13" s="102" t="n">
+      <c r="E13" s="115" t="s">
+        <v>717</v>
+      </c>
+      <c r="F13" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G13" s="102" t="n">
         <v>1500</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="102" t="s">
+        <v>724</v>
+      </c>
+      <c r="B14" s="102" t="s">
+        <v>703</v>
+      </c>
+      <c r="C14" s="102" t="s">
+        <v>704</v>
+      </c>
+      <c r="D14" s="102" t="s">
+        <v>725</v>
+      </c>
+      <c r="E14" s="102" t="s">
+        <v>726</v>
+      </c>
+      <c r="F14" s="102" t="s">
+        <v>727</v>
+      </c>
+      <c r="G14" s="102" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="102" t="s">
+        <v>728</v>
+      </c>
+      <c r="B15" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="102" t="n">
+        <v>20</v>
+      </c>
+      <c r="D15" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="102" t="s">
+        <v>729</v>
+      </c>
+      <c r="F15" s="102" t="s">
+        <v>730</v>
+      </c>
+      <c r="G15" s="102" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="102" t="s">
+        <v>732</v>
+      </c>
+      <c r="B16" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="102" t="n">
+        <v>25</v>
+      </c>
+      <c r="D16" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="102" t="s">
+        <v>733</v>
+      </c>
+      <c r="F16" s="102" t="s">
+        <v>734</v>
+      </c>
+      <c r="G16" s="102" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="102" t="s">
+        <v>736</v>
+      </c>
+      <c r="B17" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="102" t="n">
+        <v>30</v>
+      </c>
+      <c r="D17" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="102" t="s">
+        <v>733</v>
+      </c>
+      <c r="F17" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G17" s="102" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="102" t="s">
+        <v>738</v>
+      </c>
+      <c r="B18" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="102" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="102" t="s">
+        <v>570</v>
+      </c>
+      <c r="F18" s="102" t="s">
+        <v>734</v>
+      </c>
+      <c r="G18" s="102" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="102" t="s">
+        <v>740</v>
+      </c>
+      <c r="B19" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="102" t="n">
+        <v>30</v>
+      </c>
+      <c r="D19" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="102" t="s">
+        <v>741</v>
+      </c>
+      <c r="F19" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G19" s="102" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="102" t="s">
+        <v>743</v>
+      </c>
+      <c r="B20" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="102" t="n">
+        <v>15</v>
+      </c>
+      <c r="D20" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="102" t="s">
+        <v>744</v>
+      </c>
+      <c r="F20" s="102" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G20" s="102" t="s">
+        <v>693</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="115"/>
+      <c r="A21" s="102" t="s">
+        <v>745</v>
+      </c>
+      <c r="B21" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="102" t="n">
+        <v>30</v>
+      </c>
+      <c r="D21" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" s="102" t="s">
+        <v>746</v>
+      </c>
+      <c r="F21" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G21" s="102" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="115"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="102" t="s">
-        <v>721</v>
-      </c>
-      <c r="B1" s="102" t="s">
-        <v>703</v>
-      </c>
-      <c r="C1" s="102" t="s">
-        <v>704</v>
-      </c>
-      <c r="D1" s="102" t="s">
-        <v>722</v>
-      </c>
-      <c r="E1" s="102" t="s">
-        <v>723</v>
-      </c>
-      <c r="F1" s="102" t="s">
-        <v>724</v>
-      </c>
-      <c r="G1" s="102" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="102" t="s">
-        <v>725</v>
-      </c>
-      <c r="B2" s="102" t="n">
+      <c r="A22" s="102" t="s">
+        <v>747</v>
+      </c>
+      <c r="B22" s="102" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="102" t="n">
-        <v>20</v>
-      </c>
-      <c r="D2" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="102" t="s">
-        <v>726</v>
-      </c>
-      <c r="F2" s="102" t="s">
-        <v>727</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="102" t="s">
-        <v>729</v>
-      </c>
-      <c r="B3" s="102" t="n">
+      <c r="C22" s="102" t="n">
+        <v>25</v>
+      </c>
+      <c r="D22" s="102" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="102" t="n">
+      <c r="E22" s="102" t="s">
+        <v>748</v>
+      </c>
+      <c r="F22" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G22" s="102" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="102" t="s">
+        <v>749</v>
+      </c>
+      <c r="B23" s="102" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="102" t="n">
         <v>25</v>
       </c>
-      <c r="D3" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="102" t="s">
-        <v>730</v>
-      </c>
-      <c r="F3" s="102" t="s">
-        <v>731</v>
-      </c>
-      <c r="G3" s="102" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="102" t="s">
-        <v>733</v>
-      </c>
-      <c r="B4" s="102" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="102" t="n">
+      <c r="D23" s="102" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="102" t="s">
+        <v>750</v>
+      </c>
+      <c r="F23" s="102" t="s">
+        <v>718</v>
+      </c>
+      <c r="G23" s="102" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="102" t="s">
+        <v>752</v>
+      </c>
+      <c r="B24" s="102" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="102" t="n">
+        <v>25</v>
+      </c>
+      <c r="E24" s="102" t="s">
+        <v>753</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="102" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="102" t="s">
+        <v>754</v>
+      </c>
+      <c r="B25" s="102" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="102" t="n">
+        <v>25</v>
+      </c>
+      <c r="E25" s="116"/>
+      <c r="F25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="102" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="102" t="s">
+        <v>755</v>
+      </c>
+      <c r="B26" s="102" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="102" t="n">
         <v>30</v>
       </c>
-      <c r="D4" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="102" t="s">
-        <v>730</v>
-      </c>
-      <c r="F4" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="G4" s="102" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="102" t="s">
+      <c r="E26" s="102" t="s">
+        <v>756</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="102" t="s">
         <v>735</v>
       </c>
-      <c r="B5" s="102" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="102" t="n">
-        <v>25</v>
-      </c>
-      <c r="D5" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="102" t="s">
-        <v>570</v>
-      </c>
-      <c r="F5" s="102" t="s">
-        <v>731</v>
-      </c>
-      <c r="G5" s="102" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="102" t="s">
-        <v>737</v>
-      </c>
-      <c r="B6" s="102" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="102" t="n">
-        <v>30</v>
-      </c>
-      <c r="D6" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="102" t="s">
-        <v>738</v>
-      </c>
-      <c r="F6" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="G6" s="102" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="102" t="s">
-        <v>740</v>
-      </c>
-      <c r="B7" s="102" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="102" t="n">
-        <v>15</v>
-      </c>
-      <c r="D7" s="102" t="s">
-        <v>714</v>
-      </c>
-      <c r="E7" s="102" t="s">
-        <v>741</v>
-      </c>
-      <c r="F7" s="102" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="G7" s="102" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="102" t="s">
-        <v>742</v>
-      </c>
-      <c r="B8" s="102" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="102" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="102" t="s">
-        <v>714</v>
-      </c>
-      <c r="E8" s="102" t="s">
-        <v>743</v>
-      </c>
-      <c r="F8" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="G8" s="102" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="102" t="s">
-        <v>744</v>
-      </c>
-      <c r="B9" s="102" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="102" t="n">
-        <v>25</v>
-      </c>
-      <c r="D9" s="102" t="s">
-        <v>714</v>
-      </c>
-      <c r="E9" s="102" t="s">
-        <v>745</v>
-      </c>
-      <c r="F9" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="G9" s="102" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="102" t="s">
-        <v>746</v>
-      </c>
-      <c r="B10" s="102" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="102" t="n">
-        <v>25</v>
-      </c>
-      <c r="D10" s="102" t="s">
-        <v>747</v>
-      </c>
-      <c r="E10" s="102" t="s">
-        <v>748</v>
-      </c>
-      <c r="F10" s="102" t="s">
-        <v>715</v>
-      </c>
-      <c r="G10" s="102" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="102" t="s">
-        <v>750</v>
-      </c>
-      <c r="B11" s="102" t="n">
+    </row>
+    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="102" t="s">
+        <v>757</v>
+      </c>
+      <c r="B27" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="102" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E27" s="102" t="s">
+        <v>758</v>
+      </c>
+      <c r="F27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="102" t="n">
-        <v>25</v>
-      </c>
-      <c r="E11" s="102" t="s">
-        <v>751</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="G27" s="102" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="102" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="102" t="s">
-        <v>752</v>
-      </c>
-      <c r="B12" s="102" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="102" t="n">
-        <v>25</v>
-      </c>
-      <c r="E12" s="115"/>
-      <c r="F12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="102" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="102" t="s">
-        <v>753</v>
-      </c>
-      <c r="B13" s="102" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="102" t="n">
-        <v>30</v>
-      </c>
-      <c r="E13" s="102" t="s">
-        <v>754</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="102" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="102" t="s">
-        <v>755</v>
-      </c>
-      <c r="B14" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="102" t="n">
-        <v>-5</v>
-      </c>
-      <c r="E14" s="102" t="s">
-        <v>756</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="102" t="n">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="28" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H28" s="117" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="118"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
spore zmiany, magazynki zaczynaja działać, ale wciąż da się wystrzelić bez naboju w komorze.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2974" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="817">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -2460,6 +2460,9 @@
     <t xml:space="preserve">6,5 Creedmoor</t>
   </si>
   <si>
+    <t xml:space="preserve">wyborowe</t>
+  </si>
+  <si>
     <t xml:space="preserve">18$</t>
   </si>
   <si>
@@ -2475,15 +2478,9 @@
     <t xml:space="preserve">Beowolf '50</t>
   </si>
   <si>
-    <t xml:space="preserve">10?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wielkokalibrowe</t>
   </si>
   <si>
-    <t xml:space="preserve">wyborowe</t>
-  </si>
-  <si>
     <t xml:space="preserve">‘50 BMG</t>
   </si>
   <si>
@@ -2503,12 +2500,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bełty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?50$</t>
   </si>
 </sst>
 </file>
@@ -3151,8 +3142,8 @@
   </sheetPr>
   <dimension ref="A1:P300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A244" activeCellId="0" sqref="A244"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A247" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H251" activeCellId="0" sqref="H251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17712,8 +17703,8 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17807,13 +17798,13 @@
       <c r="D4" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -18148,7 +18139,7 @@
         <v>802</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
@@ -18177,7 +18168,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>-7</v>
@@ -18191,7 +18182,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>800</v>
@@ -18200,7 +18191,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>-7</v>
@@ -18212,9 +18203,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>800</v>
@@ -18232,10 +18223,10 @@
         <v>116</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>435</v>
       </c>
@@ -18246,7 +18237,7 @@
         <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>-7</v>
@@ -18255,18 +18246,18 @@
         <v>116</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>170</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>800</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>808</v>
+      <c r="C25" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>801</v>
@@ -18300,7 +18291,7 @@
         <v>413</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>15</v>
@@ -18323,7 +18314,7 @@
         <v>439</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>10</v>
@@ -18343,10 +18334,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>10</v>
@@ -18369,7 +18360,7 @@
         <v>430</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
@@ -18389,7 +18380,7 @@
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="51" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B31" s="51" t="s">
         <v>770</v>
@@ -18426,7 +18417,7 @@
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="51" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B33" s="51" t="s">
         <v>770</v>
@@ -18449,7 +18440,7 @@
         <v>75</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>-1</v>
@@ -18472,7 +18463,7 @@
         <v>75</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>-1</v>
@@ -18509,13 +18500,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>815</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>816</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>808</v>
+      <c r="C37" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>703</v>
@@ -18523,16 +18514,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>816</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>818</v>
+        <v>815</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>819</v>
+        <v>703</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18579,6 +18570,9 @@
       </c>
       <c r="G40" s="2" t="s">
         <v>147</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
przerobione zuzycie - w końcu na prawdziwe. plus poprawa testów.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="816">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -1465,9 +1465,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bezawaryjna, Celna, Pośrednia, Snajperka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.56 Nato</t>
   </si>
   <si>
     <t xml:space="preserve">Tłumik dźwięku [50m]</t>
@@ -3142,22 +3139,22 @@
   </sheetPr>
   <dimension ref="A1:P300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A247" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H251" activeCellId="0" sqref="H251"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I172" activeCellId="0" sqref="I172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="16" style="0" width="14.46"/>
   </cols>
@@ -11525,7 +11522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
         <v>470</v>
       </c>
@@ -11551,13 +11548,13 @@
         <v>471</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>472</v>
+        <v>172</v>
       </c>
       <c r="J172" s="2" t="n">
         <v>10</v>
       </c>
       <c r="K172" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L172" s="2" t="n">
         <v>2</v>
@@ -11578,7 +11575,7 @@
     </row>
     <row r="173" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B173" s="2" t="n">
         <v>750</v>
@@ -11599,7 +11596,7 @@
         <v>170</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I173" s="2" t="s">
         <v>466</v>
@@ -11611,7 +11608,7 @@
         <v>425</v>
       </c>
       <c r="L173" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M173" s="2" t="s">
         <v>24</v>
@@ -11629,7 +11626,7 @@
     </row>
     <row r="174" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B174" s="2" t="n">
         <v>2200</v>
@@ -11650,7 +11647,7 @@
         <v>21</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I174" s="2" t="s">
         <v>451</v>
@@ -11671,7 +11668,7 @@
         <v>11</v>
       </c>
       <c r="O174" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P174" s="3" t="n">
         <f aca="false">D174 + 1</f>
@@ -11680,7 +11677,7 @@
     </row>
     <row r="175" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B175" s="2" t="n">
         <v>2100</v>
@@ -11701,7 +11698,7 @@
         <v>21</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I175" s="2" t="s">
         <v>451</v>
@@ -11710,7 +11707,7 @@
         <v>5</v>
       </c>
       <c r="K175" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L175" s="2" t="s">
         <v>432</v>
@@ -11780,7 +11777,7 @@
     </row>
     <row r="177" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>15</v>
@@ -11831,7 +11828,7 @@
     </row>
     <row r="178" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B178" s="2" t="n">
         <v>2500</v>
@@ -11852,7 +11849,7 @@
         <v>21</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I178" s="2" t="s">
         <v>451</v>
@@ -11861,7 +11858,7 @@
         <v>5</v>
       </c>
       <c r="K178" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L178" s="2" t="s">
         <v>126</v>
@@ -11873,7 +11870,7 @@
         <v>12.5</v>
       </c>
       <c r="O178" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P178" s="3" t="n">
         <f aca="false">D178 + 1</f>
@@ -11882,7 +11879,7 @@
     </row>
     <row r="179" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B179" s="2" t="n">
         <v>1500</v>
@@ -11903,7 +11900,7 @@
         <v>21</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I179" s="2" t="s">
         <v>451</v>
@@ -11912,7 +11909,7 @@
         <v>10</v>
       </c>
       <c r="K179" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L179" s="2" t="s">
         <v>126</v>
@@ -11933,7 +11930,7 @@
     </row>
     <row r="180" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B180" s="2" t="n">
         <v>1400</v>
@@ -11954,7 +11951,7 @@
         <v>21</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I180" s="2" t="s">
         <v>451</v>
@@ -11963,7 +11960,7 @@
         <v>10</v>
       </c>
       <c r="K180" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L180" s="2" t="s">
         <v>126</v>
@@ -11975,7 +11972,7 @@
         <v>12</v>
       </c>
       <c r="O180" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="P180" s="3" t="n">
         <f aca="false">D180 + 1</f>
@@ -11984,7 +11981,7 @@
     </row>
     <row r="181" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B181" s="2" t="n">
         <v>400</v>
@@ -12026,7 +12023,7 @@
         <v>4</v>
       </c>
       <c r="O181" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="P181" s="3" t="n">
         <f aca="false">D181 + 1</f>
@@ -12035,7 +12032,7 @@
     </row>
     <row r="182" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B182" s="2" t="n">
         <v>600</v>
@@ -12056,7 +12053,7 @@
         <v>170</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I182" s="2" t="s">
         <v>365</v>
@@ -12077,7 +12074,7 @@
         <v>4.2</v>
       </c>
       <c r="O182" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="P182" s="3" t="n">
         <f aca="false">D182 + 1</f>
@@ -12086,7 +12083,7 @@
     </row>
     <row r="183" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B183" s="2" t="n">
         <v>750</v>
@@ -12107,7 +12104,7 @@
         <v>170</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I183" s="2" t="s">
         <v>365</v>
@@ -12137,7 +12134,7 @@
     </row>
     <row r="184" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B184" s="2" t="n">
         <v>750</v>
@@ -12158,7 +12155,7 @@
         <v>170</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I184" s="2" t="s">
         <v>365</v>
@@ -12167,7 +12164,7 @@
         <v>20</v>
       </c>
       <c r="K184" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L184" s="2" t="s">
         <v>184</v>
@@ -12179,7 +12176,7 @@
         <v>5</v>
       </c>
       <c r="O184" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="P184" s="3" t="n">
         <f aca="false">D184 + 1</f>
@@ -12188,7 +12185,7 @@
     </row>
     <row r="185" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B185" s="2" t="n">
         <v>750</v>
@@ -12209,7 +12206,7 @@
         <v>170</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I185" s="2" t="s">
         <v>365</v>
@@ -12230,7 +12227,7 @@
         <v>5</v>
       </c>
       <c r="O185" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="P185" s="3" t="n">
         <f aca="false">D185 + 1</f>
@@ -12239,7 +12236,7 @@
     </row>
     <row r="186" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B186" s="2" t="n">
         <v>1200</v>
@@ -12260,7 +12257,7 @@
         <v>21</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I186" s="2" t="s">
         <v>451</v>
@@ -12269,7 +12266,7 @@
         <v>10</v>
       </c>
       <c r="K186" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L186" s="2" t="s">
         <v>126</v>
@@ -12281,7 +12278,7 @@
         <v>14</v>
       </c>
       <c r="O186" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P186" s="3" t="n">
         <f aca="false">D186 + 1</f>
@@ -12290,7 +12287,7 @@
     </row>
     <row r="187" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B187" s="2" t="n">
         <v>1400</v>
@@ -12311,7 +12308,7 @@
         <v>21</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I187" s="2" t="s">
         <v>439</v>
@@ -12320,7 +12317,7 @@
         <v>5</v>
       </c>
       <c r="K187" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L187" s="2" t="s">
         <v>126</v>
@@ -12332,7 +12329,7 @@
         <v>14</v>
       </c>
       <c r="O187" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="P187" s="3" t="n">
         <f aca="false">D187 + 1</f>
@@ -12341,7 +12338,7 @@
     </row>
     <row r="188" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B188" s="2" t="n">
         <v>600</v>
@@ -12362,7 +12359,7 @@
         <v>170</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I188" s="2" t="s">
         <v>365</v>
@@ -12383,7 +12380,7 @@
         <v>7.2</v>
       </c>
       <c r="O188" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P188" s="3" t="n">
         <f aca="false">D188 + 1</f>
@@ -12392,7 +12389,7 @@
     </row>
     <row r="189" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B189" s="2" t="n">
         <v>750</v>
@@ -12413,7 +12410,7 @@
         <v>170</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I189" s="2" t="s">
         <v>324</v>
@@ -12422,10 +12419,10 @@
         <v>10</v>
       </c>
       <c r="K189" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="L189" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="L189" s="2" t="s">
-        <v>517</v>
       </c>
       <c r="M189" s="2" t="s">
         <v>24</v>
@@ -12434,7 +12431,7 @@
         <v>4.1</v>
       </c>
       <c r="O189" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P189" s="3" t="n">
         <f aca="false">D189 + 1</f>
@@ -12443,7 +12440,7 @@
     </row>
     <row r="190" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B190" s="2" t="n">
         <v>800</v>
@@ -12464,7 +12461,7 @@
         <v>170</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I190" s="2" t="s">
         <v>365</v>
@@ -12485,7 +12482,7 @@
         <v>4.9</v>
       </c>
       <c r="O190" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="P190" s="3" t="n">
         <f aca="false">D190 + 1</f>
@@ -12587,7 +12584,7 @@
         <v>4</v>
       </c>
       <c r="O192" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="P192" s="3" t="n">
         <f aca="false">D192 + 1</f>
@@ -12596,7 +12593,7 @@
     </row>
     <row r="193" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B193" s="2" t="n">
         <v>750</v>
@@ -12617,7 +12614,7 @@
         <v>170</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I193" s="2" t="s">
         <v>365</v>
@@ -12629,7 +12626,7 @@
         <v>179</v>
       </c>
       <c r="L193" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="M193" s="2" t="s">
         <v>220</v>
@@ -12638,7 +12635,7 @@
         <v>4.3</v>
       </c>
       <c r="O193" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P193" s="3" t="n">
         <f aca="false">D193 + 1</f>
@@ -12647,7 +12644,7 @@
     </row>
     <row r="194" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B194" s="2" t="n">
         <v>600</v>
@@ -12668,10 +12665,10 @@
         <v>170</v>
       </c>
       <c r="H194" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J194" s="2" t="n">
         <v>10</v>
@@ -12749,7 +12746,7 @@
     </row>
     <row r="196" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B196" s="2" t="n">
         <v>600</v>
@@ -12770,7 +12767,7 @@
         <v>170</v>
       </c>
       <c r="H196" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I196" s="2" t="s">
         <v>324</v>
@@ -12779,7 +12776,7 @@
         <v>20</v>
       </c>
       <c r="K196" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L196" s="2" t="s">
         <v>342</v>
@@ -12791,7 +12788,7 @@
         <v>4.2</v>
       </c>
       <c r="O196" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="P196" s="3" t="n">
         <f aca="false">D196 + 1</f>
@@ -12800,7 +12797,7 @@
     </row>
     <row r="197" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B197" s="2" t="n">
         <v>450</v>
@@ -12821,16 +12818,16 @@
         <v>147</v>
       </c>
       <c r="H197" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="I197" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="I197" s="2" t="s">
-        <v>530</v>
       </c>
       <c r="J197" s="2" t="n">
         <v>20</v>
       </c>
       <c r="K197" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L197" s="2" t="s">
         <v>141</v>
@@ -12900,7 +12897,7 @@
     </row>
     <row r="199" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>15</v>
@@ -12951,7 +12948,7 @@
     </row>
     <row r="200" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B200" s="2" t="n">
         <v>700</v>
@@ -12972,7 +12969,7 @@
         <v>65</v>
       </c>
       <c r="H200" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I200" s="2" t="s">
         <v>334</v>
@@ -12981,7 +12978,7 @@
         <v>100</v>
       </c>
       <c r="K200" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L200" s="2" t="s">
         <v>126</v>
@@ -12993,7 +12990,7 @@
         <v>6.3</v>
       </c>
       <c r="O200" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="P200" s="3" t="n">
         <f aca="false">D200 + 1</f>
@@ -13002,7 +12999,7 @@
     </row>
     <row r="201" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B201" s="2" t="n">
         <v>400</v>
@@ -13023,7 +13020,7 @@
         <v>65</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I201" s="2" t="s">
         <v>334</v>
@@ -13032,10 +13029,10 @@
         <v>30</v>
       </c>
       <c r="K201" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L201" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M201" s="2" t="s">
         <v>84</v>
@@ -13053,7 +13050,7 @@
     </row>
     <row r="202" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B202" s="2" t="n">
         <v>500</v>
@@ -13074,7 +13071,7 @@
         <v>65</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I202" s="2" t="s">
         <v>334</v>
@@ -13083,10 +13080,10 @@
         <v>100</v>
       </c>
       <c r="K202" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L202" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M202" s="2" t="s">
         <v>84</v>
@@ -13104,7 +13101,7 @@
     </row>
     <row r="203" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B203" s="2" t="n">
         <v>800</v>
@@ -13125,7 +13122,7 @@
         <v>65</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I203" s="2" t="s">
         <v>334</v>
@@ -13134,7 +13131,7 @@
         <v>100</v>
       </c>
       <c r="K203" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L203" s="2" t="s">
         <v>318</v>
@@ -13146,7 +13143,7 @@
         <v>12</v>
       </c>
       <c r="O203" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P203" s="3" t="n">
         <f aca="false">D203 + 1</f>
@@ -13155,7 +13152,7 @@
     </row>
     <row r="204" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B204" s="2" t="n">
         <v>400</v>
@@ -13176,7 +13173,7 @@
         <v>65</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I204" s="2" t="s">
         <v>172</v>
@@ -13185,7 +13182,7 @@
         <v>100</v>
       </c>
       <c r="K204" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L204" s="2" t="s">
         <v>126</v>
@@ -13197,7 +13194,7 @@
         <v>7.8</v>
       </c>
       <c r="O204" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P204" s="3" t="n">
         <f aca="false">D204 + 1</f>
@@ -13206,7 +13203,7 @@
     </row>
     <row r="205" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B205" s="2" t="n">
         <v>500</v>
@@ -13227,7 +13224,7 @@
         <v>65</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I205" s="2" t="s">
         <v>172</v>
@@ -13236,7 +13233,7 @@
         <v>100</v>
       </c>
       <c r="K205" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L205" s="2" t="s">
         <v>126</v>
@@ -13248,7 +13245,7 @@
         <v>5.1</v>
       </c>
       <c r="O205" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="P205" s="3" t="n">
         <f aca="false">D205 + 1</f>
@@ -13257,7 +13254,7 @@
     </row>
     <row r="206" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B206" s="2" t="n">
         <v>980</v>
@@ -13278,7 +13275,7 @@
         <v>65</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I206" s="2" t="s">
         <v>334</v>
@@ -13287,7 +13284,7 @@
         <v>100</v>
       </c>
       <c r="K206" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L206" s="2" t="s">
         <v>126</v>
@@ -13299,7 +13296,7 @@
         <v>11</v>
       </c>
       <c r="O206" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="P206" s="3" t="n">
         <f aca="false">D206 + 1</f>
@@ -13308,7 +13305,7 @@
     </row>
     <row r="207" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B207" s="2" t="n">
         <v>500</v>
@@ -13329,7 +13326,7 @@
         <v>65</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I207" s="2" t="s">
         <v>172</v>
@@ -13338,7 +13335,7 @@
         <v>100</v>
       </c>
       <c r="K207" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L207" s="2" t="s">
         <v>126</v>
@@ -13359,7 +13356,7 @@
     </row>
     <row r="208" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B208" s="2" t="n">
         <v>500</v>
@@ -13380,7 +13377,7 @@
         <v>65</v>
       </c>
       <c r="H208" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I208" s="2" t="s">
         <v>334</v>
@@ -13389,10 +13386,10 @@
         <v>100</v>
       </c>
       <c r="K208" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L208" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M208" s="2" t="s">
         <v>84</v>
@@ -13401,7 +13398,7 @@
         <v>10.5</v>
       </c>
       <c r="O208" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="P208" s="3" t="n">
         <f aca="false">D208 + 1</f>
@@ -13410,7 +13407,7 @@
     </row>
     <row r="209" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B209" s="2" t="n">
         <v>500</v>
@@ -13431,7 +13428,7 @@
         <v>65</v>
       </c>
       <c r="H209" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I209" s="2" t="s">
         <v>334</v>
@@ -13440,10 +13437,10 @@
         <v>100</v>
       </c>
       <c r="K209" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L209" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M209" s="2" t="s">
         <v>84</v>
@@ -13452,7 +13449,7 @@
         <v>10.5</v>
       </c>
       <c r="O209" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="P209" s="3" t="n">
         <f aca="false">D209 + 1</f>
@@ -13461,7 +13458,7 @@
     </row>
     <row r="210" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B210" s="2" t="n">
         <v>500</v>
@@ -13482,7 +13479,7 @@
         <v>65</v>
       </c>
       <c r="H210" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I210" s="2" t="s">
         <v>368</v>
@@ -13491,7 +13488,7 @@
         <v>100</v>
       </c>
       <c r="K210" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L210" s="2" t="s">
         <v>191</v>
@@ -13503,12 +13500,12 @@
         <v>12</v>
       </c>
       <c r="O210" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B211" s="2" t="n">
         <v>400</v>
@@ -13529,7 +13526,7 @@
         <v>65</v>
       </c>
       <c r="H211" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I211" s="2" t="s">
         <v>172</v>
@@ -13538,7 +13535,7 @@
         <v>100</v>
       </c>
       <c r="K211" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L211" s="2" t="s">
         <v>126</v>
@@ -13559,7 +13556,7 @@
     </row>
     <row r="212" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B212" s="2" t="n">
         <v>600</v>
@@ -13580,7 +13577,7 @@
         <v>65</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I212" s="2" t="s">
         <v>368</v>
@@ -13589,7 +13586,7 @@
         <v>100</v>
       </c>
       <c r="K212" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L212" s="2" t="s">
         <v>191</v>
@@ -13610,7 +13607,7 @@
     </row>
     <row r="213" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B213" s="2" t="n">
         <v>300</v>
@@ -13631,7 +13628,7 @@
         <v>65</v>
       </c>
       <c r="H213" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I213" s="2" t="s">
         <v>435</v>
@@ -13682,7 +13679,7 @@
     </row>
     <row r="215" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B215" s="2" t="n">
         <v>600</v>
@@ -13703,7 +13700,7 @@
         <v>65</v>
       </c>
       <c r="H215" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I215" s="2" t="s">
         <v>334</v>
@@ -13712,7 +13709,7 @@
         <v>100</v>
       </c>
       <c r="K215" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L215" s="2" t="s">
         <v>126</v>
@@ -13733,7 +13730,7 @@
     </row>
     <row r="216" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B216" s="2" t="n">
         <v>500</v>
@@ -13754,7 +13751,7 @@
         <v>65</v>
       </c>
       <c r="H216" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I216" s="2" t="s">
         <v>188</v>
@@ -13763,10 +13760,10 @@
         <v>100</v>
       </c>
       <c r="K216" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L216" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="M216" s="2" t="s">
         <v>24</v>
@@ -13784,7 +13781,7 @@
     </row>
     <row r="217" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B217" s="2" t="n">
         <v>900</v>
@@ -13805,7 +13802,7 @@
         <v>65</v>
       </c>
       <c r="H217" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I217" s="2" t="s">
         <v>188</v>
@@ -13814,10 +13811,10 @@
         <v>100</v>
       </c>
       <c r="K217" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L217" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="M217" s="2" t="s">
         <v>24</v>
@@ -13826,7 +13823,7 @@
         <v>8.2</v>
       </c>
       <c r="O217" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P217" s="3" t="n">
         <f aca="false">D217 + 1</f>
@@ -13835,7 +13832,7 @@
     </row>
     <row r="218" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B218" s="2" t="n">
         <v>400</v>
@@ -13856,7 +13853,7 @@
         <v>65</v>
       </c>
       <c r="H218" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I218" s="2" t="s">
         <v>188</v>
@@ -13865,10 +13862,10 @@
         <v>45</v>
       </c>
       <c r="K218" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L218" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="M218" s="2" t="s">
         <v>84</v>
@@ -13877,7 +13874,7 @@
         <v>6.2</v>
       </c>
       <c r="O218" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P218" s="3" t="n">
         <f aca="false">D218 + 1</f>
@@ -13886,7 +13883,7 @@
     </row>
     <row r="219" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B219" s="2" t="n">
         <v>450</v>
@@ -13907,7 +13904,7 @@
         <v>65</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I219" s="2" t="s">
         <v>324</v>
@@ -13916,7 +13913,7 @@
         <v>100</v>
       </c>
       <c r="K219" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L219" s="2" t="s">
         <v>126</v>
@@ -13928,7 +13925,7 @@
         <v>10</v>
       </c>
       <c r="O219" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P219" s="3" t="n">
         <f aca="false">D219 + 1</f>
@@ -13958,7 +13955,7 @@
         <v>65</v>
       </c>
       <c r="H220" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I220" s="2" t="s">
         <v>324</v>
@@ -13967,7 +13964,7 @@
         <v>50</v>
       </c>
       <c r="K220" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L220" s="2" t="s">
         <v>184</v>
@@ -13979,7 +13976,7 @@
         <v>4</v>
       </c>
       <c r="O220" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="P220" s="3" t="n">
         <f aca="false">D220 + 1</f>
@@ -13988,7 +13985,7 @@
     </row>
     <row r="221" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B221" s="2" t="n">
         <v>900</v>
@@ -14009,7 +14006,7 @@
         <v>65</v>
       </c>
       <c r="H221" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I221" s="2" t="s">
         <v>334</v>
@@ -14018,10 +14015,10 @@
         <v>100</v>
       </c>
       <c r="K221" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L221" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="M221" s="2" t="s">
         <v>24</v>
@@ -14030,7 +14027,7 @@
         <v>8.4</v>
       </c>
       <c r="O221" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P221" s="3" t="n">
         <f aca="false">D221 + 1</f>
@@ -14088,7 +14085,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>15</v>
@@ -14139,13 +14136,13 @@
     </row>
     <row r="224" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B224" s="2" t="n">
         <v>120</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D224" s="2" t="n">
         <v>6</v>
@@ -14157,10 +14154,10 @@
         <v>61</v>
       </c>
       <c r="G224" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H224" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="H224" s="2" t="s">
-        <v>585</v>
       </c>
       <c r="I224" s="2" t="s">
         <v>378</v>
@@ -14172,7 +14169,7 @@
         <v>15</v>
       </c>
       <c r="L224" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="M224" s="2" t="s">
         <v>24</v>
@@ -14190,7 +14187,7 @@
     </row>
     <row r="225" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B225" s="2" t="n">
         <v>120</v>
@@ -14208,10 +14205,10 @@
         <v>61</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I225" s="2" t="s">
         <v>378</v>
@@ -14223,7 +14220,7 @@
         <v>15</v>
       </c>
       <c r="L225" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="M225" s="2" t="s">
         <v>24</v>
@@ -14292,7 +14289,7 @@
     </row>
     <row r="227" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B227" s="2" t="n">
         <v>150</v>
@@ -14310,10 +14307,10 @@
         <v>61</v>
       </c>
       <c r="G227" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H227" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I227" s="2" t="s">
         <v>378</v>
@@ -14325,7 +14322,7 @@
         <v>15</v>
       </c>
       <c r="L227" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M227" s="2" t="s">
         <v>84</v>
@@ -14343,13 +14340,13 @@
     </row>
     <row r="228" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B228" s="2" t="n">
         <v>100</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D228" s="2" t="n">
         <v>6</v>
@@ -14364,7 +14361,7 @@
         <v>29</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I228" s="2" t="s">
         <v>378</v>
@@ -14376,7 +14373,7 @@
         <v>15</v>
       </c>
       <c r="L228" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="M228" s="2" t="s">
         <v>84</v>
@@ -14394,13 +14391,13 @@
     </row>
     <row r="229" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B229" s="2" t="n">
         <v>120</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D229" s="2" t="n">
         <v>6</v>
@@ -14412,10 +14409,10 @@
         <v>61</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I229" s="2" t="s">
         <v>378</v>
@@ -14427,7 +14424,7 @@
         <v>15</v>
       </c>
       <c r="L229" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M229" s="2" t="s">
         <v>24</v>
@@ -14445,7 +14442,7 @@
     </row>
     <row r="230" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B230" s="2" t="n">
         <v>70</v>
@@ -14463,10 +14460,10 @@
         <v>61</v>
       </c>
       <c r="G230" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I230" s="2" t="s">
         <v>378</v>
@@ -14478,7 +14475,7 @@
         <v>15</v>
       </c>
       <c r="L230" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M230" s="2" t="s">
         <v>24</v>
@@ -14496,13 +14493,13 @@
     </row>
     <row r="231" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B231" s="2" t="n">
         <v>30</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D231" s="2" t="n">
         <v>5</v>
@@ -14514,10 +14511,10 @@
         <v>61</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I231" s="2" t="s">
         <v>378</v>
@@ -14547,7 +14544,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B232" s="2" t="n">
         <v>120</v>
@@ -14565,10 +14562,10 @@
         <v>61</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I232" s="2" t="s">
         <v>378</v>
@@ -14598,7 +14595,7 @@
     </row>
     <row r="233" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B233" s="2" t="n">
         <v>120</v>
@@ -14616,10 +14613,10 @@
         <v>61</v>
       </c>
       <c r="G233" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H233" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="H233" s="2" t="s">
-        <v>585</v>
       </c>
       <c r="I233" s="2" t="s">
         <v>378</v>
@@ -14631,7 +14628,7 @@
         <v>15</v>
       </c>
       <c r="L233" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M233" s="2" t="s">
         <v>24</v>
@@ -14698,7 +14695,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>15</v>
@@ -14749,13 +14746,13 @@
     </row>
     <row r="236" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B236" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D236" s="2" t="n">
         <v>2</v>
@@ -14770,10 +14767,10 @@
         <v>147</v>
       </c>
       <c r="H236" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="I236" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="I236" s="2" t="s">
-        <v>608</v>
       </c>
       <c r="J236" s="2" t="n">
         <v>1</v>
@@ -14800,13 +14797,13 @@
     </row>
     <row r="237" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B237" s="2" t="n">
         <v>300</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D237" s="2" t="n">
         <v>2</v>
@@ -14821,10 +14818,10 @@
         <v>147</v>
       </c>
       <c r="H237" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I237" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="J237" s="2" t="n">
         <v>1</v>
@@ -14851,13 +14848,13 @@
     </row>
     <row r="238" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B238" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D238" s="2" t="n">
         <v>0</v>
@@ -14866,16 +14863,16 @@
         <v>-4</v>
       </c>
       <c r="F238" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G238" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H238" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="I238" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="I238" s="2" t="s">
-        <v>608</v>
       </c>
       <c r="J238" s="2" t="n">
         <v>1</v>
@@ -14902,13 +14899,13 @@
     </row>
     <row r="239" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B239" s="2" t="n">
         <v>125</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D239" s="2" t="n">
         <v>1</v>
@@ -14923,10 +14920,10 @@
         <v>147</v>
       </c>
       <c r="H239" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="I239" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="I239" s="2" t="s">
-        <v>608</v>
       </c>
       <c r="J239" s="2" t="n">
         <v>1</v>
@@ -14953,13 +14950,13 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B240" s="2" t="n">
         <v>300</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D240" s="2" t="n">
         <v>2</v>
@@ -14974,10 +14971,10 @@
         <v>147</v>
       </c>
       <c r="H240" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I240" s="2" t="s">
         <v>615</v>
-      </c>
-      <c r="I240" s="2" t="s">
-        <v>616</v>
       </c>
       <c r="J240" s="2" t="n">
         <v>1</v>
@@ -15004,13 +15001,13 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B241" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D241" s="2" t="n">
         <v>2</v>
@@ -15025,10 +15022,10 @@
         <v>147</v>
       </c>
       <c r="H241" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I241" s="2" t="s">
         <v>615</v>
-      </c>
-      <c r="I241" s="2" t="s">
-        <v>616</v>
       </c>
       <c r="J241" s="2" t="n">
         <v>1</v>
@@ -15037,7 +15034,7 @@
         <v>15</v>
       </c>
       <c r="L241" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="M241" s="2" t="s">
         <v>15</v>
@@ -15055,13 +15052,13 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B242" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D242" s="2" t="n">
         <v>2</v>
@@ -15076,10 +15073,10 @@
         <v>147</v>
       </c>
       <c r="H242" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I242" s="2" t="s">
         <v>615</v>
-      </c>
-      <c r="I242" s="2" t="s">
-        <v>616</v>
       </c>
       <c r="J242" s="2" t="n">
         <v>1</v>
@@ -15106,13 +15103,13 @@
     </row>
     <row r="243" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B243" s="2" t="n">
         <v>100</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D243" s="2" t="n">
         <v>2</v>
@@ -15121,16 +15118,16 @@
         <v>-1</v>
       </c>
       <c r="F243" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G243" s="2" t="s">
         <v>147</v>
       </c>
       <c r="H243" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I243" s="2" t="s">
         <v>615</v>
-      </c>
-      <c r="I243" s="2" t="s">
-        <v>616</v>
       </c>
       <c r="J243" s="2" t="n">
         <v>1</v>
@@ -15157,7 +15154,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>15</v>
@@ -15208,13 +15205,13 @@
     </row>
     <row r="245" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B245" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D245" s="2" t="n">
         <v>2</v>
@@ -15229,10 +15226,10 @@
         <v>65</v>
       </c>
       <c r="H245" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="I245" s="2" t="s">
         <v>624</v>
-      </c>
-      <c r="I245" s="2" t="s">
-        <v>625</v>
       </c>
       <c r="J245" s="2" t="n">
         <v>1</v>
@@ -15259,13 +15256,13 @@
     </row>
     <row r="246" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B246" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D246" s="2" t="n">
         <v>2</v>
@@ -15280,10 +15277,10 @@
         <v>65</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I246" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J246" s="2" t="n">
         <v>1</v>
@@ -15310,13 +15307,13 @@
     </row>
     <row r="247" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B247" s="2" t="n">
         <v>400</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D247" s="2" t="n">
         <v>4</v>
@@ -15331,10 +15328,10 @@
         <v>65</v>
       </c>
       <c r="H247" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I247" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J247" s="2" t="n">
         <v>6</v>
@@ -15343,7 +15340,7 @@
         <v>15</v>
       </c>
       <c r="L247" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="M247" s="2" t="n">
         <v>2</v>
@@ -15352,7 +15349,7 @@
         <v>5.3</v>
       </c>
       <c r="O247" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P247" s="3" t="n">
         <f aca="false">bronbiala!D7 + 1</f>
@@ -15361,13 +15358,13 @@
     </row>
     <row r="248" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B248" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D248" s="2" t="n">
         <v>3</v>
@@ -15382,10 +15379,10 @@
         <v>65</v>
       </c>
       <c r="H248" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I248" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J248" s="2" t="n">
         <v>1</v>
@@ -15412,13 +15409,13 @@
     </row>
     <row r="249" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B249" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D249" s="2" t="n">
         <v>3</v>
@@ -15433,10 +15430,10 @@
         <v>65</v>
       </c>
       <c r="H249" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I249" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J249" s="2" t="n">
         <v>1</v>
@@ -15463,13 +15460,13 @@
     </row>
     <row r="250" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B250" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D250" s="2" t="n">
         <v>1</v>
@@ -15484,10 +15481,10 @@
         <v>21</v>
       </c>
       <c r="H250" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I250" s="2" t="s">
         <v>636</v>
-      </c>
-      <c r="I250" s="2" t="s">
-        <v>637</v>
       </c>
       <c r="J250" s="2" t="n">
         <v>1</v>
@@ -15514,13 +15511,13 @@
     </row>
     <row r="251" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B251" s="2" t="n">
         <v>72</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D251" s="2" t="n">
         <v>0</v>
@@ -15535,10 +15532,10 @@
         <v>21</v>
       </c>
       <c r="H251" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I251" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J251" s="2" t="n">
         <v>1</v>
@@ -15565,13 +15562,13 @@
     </row>
     <row r="252" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B252" s="2" t="n">
         <v>500</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D252" s="2" t="n">
         <v>1</v>
@@ -15586,10 +15583,10 @@
         <v>21</v>
       </c>
       <c r="H252" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I252" s="2" t="s">
         <v>636</v>
-      </c>
-      <c r="I252" s="2" t="s">
-        <v>637</v>
       </c>
       <c r="J252" s="2" t="n">
         <v>1</v>
@@ -15607,7 +15604,7 @@
         <v>15</v>
       </c>
       <c r="O252" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P252" s="3" t="n">
         <f aca="false">bronbiala!D12 + 1</f>
@@ -15616,13 +15613,13 @@
     </row>
     <row r="253" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B253" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D253" s="2" t="n">
         <v>3</v>
@@ -15637,10 +15634,10 @@
         <v>65</v>
       </c>
       <c r="H253" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I253" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J253" s="2" t="n">
         <v>4</v>
@@ -15780,7 +15777,7 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O300" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -15805,11 +15802,11 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>15</v>
@@ -15856,7 +15853,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>0</v>
@@ -15871,13 +15868,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>645</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>646</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>16</v>
@@ -15903,7 +15900,7 @@
     </row>
     <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B3" s="21" t="n">
         <v>1.5</v>
@@ -15924,10 +15921,10 @@
         <v>65</v>
       </c>
       <c r="H3" s="27" t="s">
+        <v>647</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>648</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>649</v>
       </c>
       <c r="J3" s="28" t="s">
         <v>15</v>
@@ -15945,12 +15942,12 @@
         <v>0.5</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>1</v>
@@ -15969,10 +15966,10 @@
         <v>65</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>15</v>
@@ -15990,12 +15987,12 @@
         <v>0.4</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>0</v>
@@ -16016,10 +16013,10 @@
         <v>65</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>15</v>
@@ -16037,12 +16034,12 @@
         <v>0.4</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>0.5</v>
@@ -16063,10 +16060,10 @@
         <v>15</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>15</v>
@@ -16084,12 +16081,12 @@
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>1</v>
@@ -16110,10 +16107,10 @@
         <v>15</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>15</v>
@@ -16131,12 +16128,12 @@
         <v>1.5</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0</v>
@@ -16157,10 +16154,10 @@
         <v>15</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>15</v>
@@ -16178,12 +16175,12 @@
         <v>0.1</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0</v>
@@ -16198,16 +16195,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>15</v>
@@ -16225,12 +16222,12 @@
         <v>0.4</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>1</v>
@@ -16275,7 +16272,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.5</v>
@@ -16296,10 +16293,10 @@
         <v>65</v>
       </c>
       <c r="H11" s="19" t="s">
+        <v>661</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>662</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>15</v>
@@ -16317,12 +16314,12 @@
         <v>1</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="34" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>1.5</v>
@@ -16367,7 +16364,7 @@
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>2</v>
@@ -16388,7 +16385,7 @@
         <v>65</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>127</v>
@@ -16414,7 +16411,7 @@
     </row>
     <row r="14" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="34" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0</v>
@@ -16435,10 +16432,10 @@
         <v>65</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>15</v>
@@ -16456,12 +16453,12 @@
         <v>0.3</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0</v>
@@ -16482,10 +16479,10 @@
         <v>65</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>15</v>
@@ -16503,12 +16500,12 @@
         <v>0.4</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0.5</v>
@@ -16529,10 +16526,10 @@
         <v>15</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>15</v>
@@ -16550,12 +16547,12 @@
         <v>0.5</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>1</v>
@@ -16576,7 +16573,7 @@
         <v>65</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>134</v>
@@ -16602,7 +16599,7 @@
     </row>
     <row r="18" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="34" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>0</v>
@@ -16617,16 +16614,16 @@
         <v>0</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J18" s="12" t="s">
         <v>15</v>
@@ -16644,12 +16641,12 @@
         <v>0.2</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="34" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0.5</v>
@@ -16670,10 +16667,10 @@
         <v>65</v>
       </c>
       <c r="H19" s="11" t="s">
+        <v>674</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>675</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>676</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>15</v>
@@ -16691,7 +16688,7 @@
         <v>1</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16751,40 +16748,40 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="37" t="s">
+        <v>676</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>677</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C1" s="38" t="s">
         <v>678</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>679</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="38" t="s">
+        <v>679</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>680</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="G1" s="39" t="s">
         <v>681</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>682</v>
       </c>
       <c r="H1" s="38" t="s">
         <v>36</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="40" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B2" s="41" t="n">
         <v>6</v>
@@ -16796,24 +16793,24 @@
         <v>15</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F2" s="44" t="n">
         <v>5</v>
       </c>
       <c r="G2" s="45" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H2" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B3" s="41" t="n">
         <v>5</v>
@@ -16822,27 +16819,27 @@
         <v>336</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F3" s="44" t="n">
         <v>5</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H3" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B4" s="41" t="n">
         <v>5</v>
@@ -16854,24 +16851,24 @@
         <v>15</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F4" s="44" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="45" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="H4" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I4" s="47" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="40" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B5" s="41" t="n">
         <v>5</v>
@@ -16883,24 +16880,24 @@
         <v>15</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F5" s="44" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="45" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H5" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I5" s="47" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B6" s="41" t="n">
         <v>6</v>
@@ -16912,24 +16909,24 @@
         <v>15</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F6" s="44" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H6" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I6" s="47" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B7" s="41" t="n">
         <v>2</v>
@@ -16938,10 +16935,10 @@
         <v>336</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F7" s="44" t="n">
         <v>5</v>
@@ -16951,12 +16948,12 @@
         <v>0.4</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="40" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B8" s="41" t="n">
         <v>5</v>
@@ -16968,24 +16965,24 @@
         <v>15</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F8" s="44" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H8" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="40" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B9" s="41" t="n">
         <v>3</v>
@@ -16997,24 +16994,24 @@
         <v>15</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F9" s="44" t="n">
         <v>4</v>
       </c>
       <c r="G9" s="45" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H9" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="40" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B10" s="41" t="n">
         <v>5</v>
@@ -17023,22 +17020,22 @@
         <v>20</v>
       </c>
       <c r="D10" s="42" t="s">
+        <v>709</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="45" t="s">
         <v>710</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>711</v>
       </c>
       <c r="H10" s="46" t="n">
         <v>0.4</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>
@@ -17063,7 +17060,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17072,30 +17069,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="0" t="s">
         <v>715</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>3</v>
@@ -17107,7 +17104,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.4</v>
@@ -17118,7 +17115,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>3</v>
@@ -17130,7 +17127,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.4</v>
@@ -17141,7 +17138,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>3</v>
@@ -17153,7 +17150,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.4</v>
@@ -17164,7 +17161,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>3</v>
@@ -17176,7 +17173,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.4</v>
@@ -17187,7 +17184,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
@@ -17199,7 +17196,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
@@ -17210,7 +17207,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>3</v>
@@ -17222,7 +17219,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
@@ -17233,7 +17230,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>3</v>
@@ -17245,10 +17242,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>728</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>600</v>
@@ -17256,7 +17253,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>3</v>
@@ -17268,10 +17265,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>728</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>800</v>
@@ -17279,7 +17276,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>3</v>
@@ -17291,10 +17288,10 @@
         <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>728</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>900</v>
@@ -17302,7 +17299,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>3</v>
@@ -17314,10 +17311,10 @@
         <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>728</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1000</v>
@@ -17325,7 +17322,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>3</v>
@@ -17337,10 +17334,10 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>728</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>1000</v>
@@ -17348,7 +17345,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>3</v>
@@ -17360,10 +17357,10 @@
         <v>400</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>728</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>1500</v>
@@ -17371,30 +17368,30 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>734</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>713</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>714</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>737</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>3</v>
@@ -17406,18 +17403,18 @@
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>740</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>3</v>
@@ -17429,18 +17426,18 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>744</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>3</v>
@@ -17452,18 +17449,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>3</v>
@@ -17475,18 +17472,18 @@
         <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>3</v>
@@ -17498,18 +17495,18 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>751</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>3</v>
@@ -17521,18 +17518,18 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0.3</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>3</v>
@@ -17544,18 +17541,18 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>3</v>
@@ -17567,18 +17564,18 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2</v>
@@ -17590,18 +17587,18 @@
         <v>2</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>760</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>0</v>
@@ -17610,7 +17607,7 @@
         <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>0</v>
@@ -17621,7 +17618,7 @@
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>0</v>
@@ -17634,12 +17631,12 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>1</v>
@@ -17648,18 +17645,18 @@
         <v>30</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>15</v>
@@ -17668,7 +17665,7 @@
         <v>-5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>0</v>
@@ -17679,7 +17676,7 @@
     </row>
     <row r="28" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="49" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17703,11 +17700,11 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -17715,42 +17712,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>769</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>770</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>771</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="E1" s="0" t="s">
         <v>772</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>773</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>774</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>775</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>776</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>777</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>-3</v>
@@ -17767,13 +17764,13 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>90</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>-1</v>
@@ -17790,13 +17787,13 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>-1</v>
@@ -17813,13 +17810,13 @@
         <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>-1</v>
@@ -17833,16 +17830,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>-2</v>
@@ -17854,21 +17851,21 @@
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B7" s="51" t="s">
+        <v>769</v>
+      </c>
+      <c r="C7" s="51" t="s">
         <v>770</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="D7" s="51" t="s">
         <v>771</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>772</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="52"/>
@@ -17878,13 +17875,13 @@
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>-3</v>
@@ -17898,16 +17895,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>-5</v>
@@ -17921,16 +17918,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>-4</v>
@@ -17944,16 +17941,16 @@
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="51" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B11" s="51" t="s">
+        <v>769</v>
+      </c>
+      <c r="C11" s="51" t="s">
         <v>770</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="D11" s="51" t="s">
         <v>771</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17961,13 +17958,13 @@
         <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>-5</v>
@@ -17981,16 +17978,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>-5</v>
@@ -18002,7 +17999,7 @@
         <v>65</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18010,13 +18007,13 @@
         <v>178</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>-6</v>
@@ -18030,16 +18027,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>-5</v>
@@ -18053,16 +18050,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>90</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>-5</v>
@@ -18076,30 +18073,30 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B17" s="51" t="s">
+        <v>769</v>
+      </c>
+      <c r="C17" s="51" t="s">
         <v>770</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="D17" s="51" t="s">
         <v>771</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>799</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>800</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>-7</v>
@@ -18116,13 +18113,13 @@
         <v>469</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>-7</v>
@@ -18136,16 +18133,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>802</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>803</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>-7</v>
@@ -18162,13 +18159,13 @@
         <v>334</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>-7</v>
@@ -18182,16 +18179,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>-7</v>
@@ -18205,16 +18202,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>-7</v>
@@ -18231,13 +18228,13 @@
         <v>435</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>-7</v>
@@ -18251,16 +18248,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>-10</v>
@@ -18274,16 +18271,16 @@
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="51" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B26" s="51" t="s">
+        <v>769</v>
+      </c>
+      <c r="C26" s="51" t="s">
         <v>770</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="D26" s="51" t="s">
         <v>771</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18291,13 +18288,13 @@
         <v>413</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>-9</v>
@@ -18314,13 +18311,13 @@
         <v>439</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>-16</v>
@@ -18334,16 +18331,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>-16</v>
@@ -18360,13 +18357,13 @@
         <v>430</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>-12</v>
@@ -18380,16 +18377,16 @@
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="51" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B31" s="51" t="s">
+        <v>769</v>
+      </c>
+      <c r="C31" s="51" t="s">
         <v>770</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="D31" s="51" t="s">
         <v>771</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18397,13 +18394,13 @@
         <v>378</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>23</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>-5</v>
@@ -18412,21 +18409,21 @@
         <v>61</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="51" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B33" s="51" t="s">
+        <v>769</v>
+      </c>
+      <c r="C33" s="51" t="s">
         <v>770</v>
       </c>
-      <c r="C33" s="51" t="s">
+      <c r="D33" s="51" t="s">
         <v>771</v>
-      </c>
-      <c r="D33" s="51" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18434,13 +18431,13 @@
         <v>149</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>-1</v>
@@ -18457,13 +18454,13 @@
         <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>-1</v>
@@ -18480,13 +18477,13 @@
         <v>464</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>16</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>-6</v>
@@ -18500,44 +18497,44 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>814</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>815</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>30</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>-6</v>
@@ -18554,13 +18551,13 @@
         <v>211</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>30</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>-6</v>
@@ -18572,7 +18569,7 @@
         <v>147</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did default magazine for the gun at init, also did good testing of gun. Also you can't unload ammo to any package. and tests. quite a lot of them.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -3139,8 +3139,8 @@
   </sheetPr>
   <dimension ref="A1:P300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I172" activeCellId="0" sqref="I172"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E172" activeCellId="0" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3150,6 +3150,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.45"/>
@@ -11522,7 +11523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
         <v>470</v>
       </c>

</xml_diff>

<commit_message>
Naprawiono buga z umiejętnościami, oraz walka wręcz, podstawowe klepanie isę działa.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="817">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -1980,7 +1980,7 @@
     <t xml:space="preserve">Broń biała</t>
   </si>
   <si>
-    <t xml:space="preserve">Kolba/Pięść</t>
+    <t xml:space="preserve">Kolba</t>
   </si>
   <si>
     <t xml:space="preserve">D2</t>
@@ -1989,21 +1989,24 @@
     <t xml:space="preserve">Obuchowa</t>
   </si>
   <si>
+    <t xml:space="preserve">Pięść</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$50,00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bagnet (od Mosina, założony)/ włócznia</t>
   </si>
   <si>
     <t xml:space="preserve">Zdejmowalny</t>
   </si>
   <si>
-    <t xml:space="preserve">$50,00</t>
+    <t xml:space="preserve">$100,00</t>
   </si>
   <si>
     <t xml:space="preserve">Bagnet (założony)</t>
   </si>
   <si>
-    <t xml:space="preserve">$100,00</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bagnet (zdjęty)</t>
   </si>
   <si>
@@ -2031,15 +2034,15 @@
     <t xml:space="preserve">Katana</t>
   </si>
   <si>
+    <t xml:space="preserve">$200,00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maczeta</t>
   </si>
   <si>
     <t xml:space="preserve">Szybka</t>
   </si>
   <si>
-    <t xml:space="preserve">$200,00</t>
-  </si>
-  <si>
     <t xml:space="preserve">Miecz długi</t>
   </si>
   <si>
@@ -2070,13 +2073,13 @@
     <t xml:space="preserve">Rękawice szturmowe</t>
   </si>
   <si>
+    <t xml:space="preserve">$150,00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Toporek</t>
   </si>
   <si>
     <t xml:space="preserve">Rzut (3m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$150,00</t>
   </si>
   <si>
     <t xml:space="preserve">Granaty I miny</t>
@@ -2783,13 +2786,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top style="thin">
@@ -2804,6 +2800,13 @@
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -2847,7 +2850,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2928,39 +2931,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2972,15 +2947,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2988,15 +2991,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3139,11 +3138,11 @@
   </sheetPr>
   <dimension ref="A1:P300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E172" activeCellId="0" sqref="E172"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B98" activeCellId="0" sqref="B98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -3155,7 +3154,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="16" style="0" width="14.46"/>
   </cols>
@@ -15046,9 +15045,9 @@
       <c r="O241" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="P241" s="3" t="e">
+      <c r="P241" s="3" t="n">
         <f aca="false">bronbiala!D1 + 1</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15097,9 +15096,9 @@
       <c r="O242" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="P242" s="3" t="e">
+      <c r="P242" s="3" t="n">
         <f aca="false">bronbiala!D2 + 1</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15149,7 +15148,7 @@
         <v>101</v>
       </c>
       <c r="P243" s="3" t="n">
-        <f aca="false">bronbiala!D3 + 1</f>
+        <f aca="false">bronbiala!D4 + 1</f>
         <v>7</v>
       </c>
     </row>
@@ -15200,7 +15199,7 @@
         <v>16</v>
       </c>
       <c r="P244" s="3" t="n">
-        <f aca="false">bronbiala!D4 + 1</f>
+        <f aca="false">bronbiala!D5 + 1</f>
         <v>5</v>
       </c>
     </row>
@@ -15251,7 +15250,7 @@
         <v>394</v>
       </c>
       <c r="P245" s="3" t="n">
-        <f aca="false">bronbiala!D5 + 1</f>
+        <f aca="false">bronbiala!D6 + 1</f>
         <v>4</v>
       </c>
     </row>
@@ -15302,7 +15301,7 @@
         <v>127</v>
       </c>
       <c r="P246" s="3" t="n">
-        <f aca="false">bronbiala!D6 + 1</f>
+        <f aca="false">bronbiala!D7 + 1</f>
         <v>6</v>
       </c>
     </row>
@@ -15353,7 +15352,7 @@
         <v>630</v>
       </c>
       <c r="P247" s="3" t="n">
-        <f aca="false">bronbiala!D7 + 1</f>
+        <f aca="false">bronbiala!D8 + 1</f>
         <v>6</v>
       </c>
     </row>
@@ -15404,7 +15403,7 @@
         <v>104</v>
       </c>
       <c r="P248" s="3" t="n">
-        <f aca="false">bronbiala!D8 + 1</f>
+        <f aca="false">bronbiala!D9 + 1</f>
         <v>2</v>
       </c>
     </row>
@@ -15455,7 +15454,7 @@
         <v>101</v>
       </c>
       <c r="P249" s="3" t="n">
-        <f aca="false">bronbiala!D9 + 1</f>
+        <f aca="false">bronbiala!D10 + 1</f>
         <v>2</v>
       </c>
     </row>
@@ -15506,7 +15505,7 @@
         <v>127</v>
       </c>
       <c r="P250" s="3" t="n">
-        <f aca="false">bronbiala!D10 + 1</f>
+        <f aca="false">bronbiala!D11 + 1</f>
         <v>7</v>
       </c>
     </row>
@@ -15557,7 +15556,7 @@
         <v>101</v>
       </c>
       <c r="P251" s="3" t="n">
-        <f aca="false">bronbiala!D11 + 1</f>
+        <f aca="false">bronbiala!D12 + 1</f>
         <v>5</v>
       </c>
     </row>
@@ -15608,7 +15607,7 @@
         <v>630</v>
       </c>
       <c r="P252" s="3" t="n">
-        <f aca="false">bronbiala!D12 + 1</f>
+        <f aca="false">bronbiala!D13 + 1</f>
         <v>7</v>
       </c>
     </row>
@@ -15659,50 +15658,50 @@
         <v>389</v>
       </c>
       <c r="P253" s="3" t="n">
-        <f aca="false">bronbiala!D13 + 1</f>
+        <f aca="false">bronbiala!D14 + 1</f>
         <v>9</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P254" s="3" t="n">
-        <f aca="false">bronbiala!D14 + 1</f>
+        <f aca="false">bronbiala!D15 + 1</f>
         <v>4</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P255" s="3" t="n">
-        <f aca="false">bronbiala!D15 + 1</f>
+        <f aca="false">bronbiala!D16 + 1</f>
         <v>4</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P256" s="3" t="n">
-        <f aca="false">bronbiala!D16 + 1</f>
+        <f aca="false">bronbiala!D17 + 1</f>
         <v>6</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P257" s="3" t="n">
-        <f aca="false">bronbiala!D17 + 1</f>
+        <f aca="false">bronbiala!D18 + 1</f>
         <v>7</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P258" s="3" t="n">
-        <f aca="false">bronbiala!D18 + 1</f>
+        <f aca="false">bronbiala!D19 + 1</f>
         <v>2</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P259" s="3" t="n">
-        <f aca="false">bronbiala!D19 + 1</f>
+        <f aca="false">bronbiala!D20 + 1</f>
         <v>6</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P260" s="3" t="n">
         <f aca="false">bronbiala!D20 + 1</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15799,11 +15798,11 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -15815,8 +15814,8 @@
       <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>15</v>
+      <c r="D1" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>15</v>
@@ -15862,8 +15861,8 @@
       <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>15</v>
+      <c r="D2" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>0</v>
@@ -15872,7 +15871,7 @@
         <v>644</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>15</v>
+        <v>583</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>645</v>
@@ -15899,78 +15898,80 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
         <v>646</v>
       </c>
-      <c r="B3" s="21" t="n">
+      <c r="B3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>645</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="25" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26" t="s">
+        <v>648</v>
+      </c>
+      <c r="B4" s="27" t="n">
         <v>1.5</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="23" t="n">
+      <c r="C4" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E4" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F4" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G4" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H4" s="33" t="s">
+        <v>649</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>647</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="32" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>649</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>647</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>650</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>15</v>
@@ -15991,18 +15992,16 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+    <row r="5" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
         <v>651</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>0</v>
@@ -16013,8 +16012,8 @@
       <c r="G5" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>652</v>
+      <c r="H5" s="19" t="s">
+        <v>649</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>650</v>
@@ -16038,33 +16037,33 @@
         <v>650</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="8" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>15</v>
@@ -16082,15 +16081,15 @@
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34" t="s">
         <v>654</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>15</v>
@@ -16099,19 +16098,19 @@
         <v>5</v>
       </c>
       <c r="E7" s="8" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>645</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>15</v>
@@ -16132,30 +16131,30 @@
         <v>650</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34" t="s">
+    <row r="8" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18" t="s">
         <v>655</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8" s="8" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>656</v>
+        <v>583</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>645</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>650</v>
@@ -16180,8 +16179,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
-        <v>657</v>
+      <c r="A9" s="34" t="s">
+        <v>656</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0</v>
@@ -16196,13 +16195,13 @@
         <v>0</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>658</v>
+        <v>15</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>645</v>
+        <v>583</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>657</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>650</v>
@@ -16227,30 +16226,32 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>659</v>
       </c>
-      <c r="B10" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" s="8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="G10" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="11"/>
+        <v>583</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>645</v>
+      </c>
       <c r="I10" s="2" t="s">
-        <v>127</v>
+        <v>650</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>15</v>
@@ -16271,33 +16272,31 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="34" t="s">
         <v>660</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E11" s="8" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>661</v>
-      </c>
+      <c r="H11" s="11"/>
       <c r="I11" s="2" t="s">
-        <v>662</v>
+        <v>127</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>15</v>
@@ -16315,24 +16314,24 @@
         <v>1</v>
       </c>
       <c r="O11" s="17" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="s">
-        <v>663</v>
-      </c>
       <c r="B12" s="5" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12" s="8" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>116</v>
@@ -16340,9 +16339,11 @@
       <c r="G12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="19" t="s">
+        <v>663</v>
+      </c>
       <c r="I12" s="2" t="s">
-        <v>283</v>
+        <v>661</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>15</v>
@@ -16363,33 +16364,31 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="34" t="s">
         <v>664</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E13" s="8" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="19" t="s">
-        <v>665</v>
-      </c>
+      <c r="H13" s="11"/>
       <c r="I13" s="2" t="s">
-        <v>127</v>
+        <v>283</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>15</v>
@@ -16410,33 +16409,33 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="34" t="s">
-        <v>666</v>
+    <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
+        <v>665</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="7" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E14" s="8" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>667</v>
+      <c r="H14" s="19" t="s">
+        <v>666</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>648</v>
+        <v>127</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>15</v>
@@ -16454,12 +16453,12 @@
         <v>0.3</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
-        <v>668</v>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="34" t="s">
+        <v>667</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0</v>
@@ -16474,16 +16473,16 @@
         <v>0</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>667</v>
+      <c r="H15" s="11" t="s">
+        <v>668</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>15</v>
@@ -16504,33 +16503,33 @@
         <v>650</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
         <v>669</v>
       </c>
       <c r="B16" s="5" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" s="8" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>645</v>
+        <v>668</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>15</v>
@@ -16548,36 +16547,36 @@
         <v>0.5</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
         <v>670</v>
       </c>
       <c r="B17" s="5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="8" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>65</v>
+        <v>583</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>671</v>
+        <v>645</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>134</v>
+        <v>647</v>
       </c>
       <c r="J17" s="12" t="s">
         <v>15</v>
@@ -16598,33 +16597,33 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
-        <v>672</v>
+    <row r="18" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
+        <v>671</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>658</v>
+        <v>35</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>645</v>
+        <v>65</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>672</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>650</v>
+        <v>134</v>
       </c>
       <c r="J18" s="12" t="s">
         <v>15</v>
@@ -16645,33 +16644,33 @@
         <v>650</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="34" t="s">
         <v>673</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E19" s="8" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>116</v>
+        <v>659</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>65</v>
+        <v>583</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>674</v>
+        <v>645</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>675</v>
+        <v>650</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>15</v>
@@ -16689,19 +16688,37 @@
         <v>1</v>
       </c>
       <c r="O19" s="17" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="34" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="12"/>
+      <c r="B20" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>676</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>674</v>
+      </c>
       <c r="J20" s="12"/>
       <c r="K20" s="13"/>
       <c r="L20" s="14"/>
@@ -16710,7 +16727,7 @@
       <c r="O20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
@@ -16749,294 +16766,294 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>676</v>
-      </c>
-      <c r="B1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>677</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>678</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="37" t="s">
+        <v>679</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="38" t="s">
-        <v>679</v>
-      </c>
-      <c r="F1" s="38" t="s">
+      <c r="E1" s="37" t="s">
         <v>680</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>681</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="G1" s="38" t="s">
+        <v>682</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="38" t="s">
-        <v>682</v>
+      <c r="I1" s="37" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
-        <v>683</v>
-      </c>
-      <c r="B2" s="41" t="n">
+      <c r="A2" s="39" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2" s="40" t="n">
         <v>6</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F2" s="44" t="n">
+      <c r="C2" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="F2" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="44" t="s">
+        <v>686</v>
+      </c>
+      <c r="H2" s="45" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="39" t="s">
+        <v>688</v>
+      </c>
+      <c r="B3" s="40" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>689</v>
+      </c>
+      <c r="E3" s="42" t="s">
         <v>685</v>
       </c>
-      <c r="H2" s="46" t="n">
+      <c r="F3" s="43" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>690</v>
+      </c>
+      <c r="H3" s="45" t="n">
         <v>0.4</v>
       </c>
-      <c r="I2" s="47" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="s">
-        <v>687</v>
-      </c>
-      <c r="B3" s="41" t="n">
+      <c r="I3" s="46" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="39" t="s">
+        <v>692</v>
+      </c>
+      <c r="B4" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C4" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="F4" s="43" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="H4" s="45" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="39" t="s">
+        <v>695</v>
+      </c>
+      <c r="B5" s="40" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="F5" s="43" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>696</v>
+      </c>
+      <c r="H5" s="45" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="39" t="s">
+        <v>698</v>
+      </c>
+      <c r="B6" s="40" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="F6" s="43" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>699</v>
+      </c>
+      <c r="H6" s="45" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I6" s="46" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="39" t="s">
+        <v>701</v>
+      </c>
+      <c r="B7" s="40" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="41" t="s">
         <v>336</v>
       </c>
-      <c r="D3" s="42" t="s">
-        <v>688</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F3" s="44" t="n">
+      <c r="D7" s="41" t="s">
+        <v>702</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="F7" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>689</v>
-      </c>
-      <c r="H3" s="46" t="n">
+      <c r="G7" s="47"/>
+      <c r="H7" s="45" t="n">
         <v>0.4</v>
       </c>
-      <c r="I3" s="47" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
-        <v>691</v>
-      </c>
-      <c r="B4" s="41" t="n">
+      <c r="I7" s="46" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="39" t="s">
+        <v>704</v>
+      </c>
+      <c r="B8" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F4" s="44" t="n">
+      <c r="C8" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="F8" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="G4" s="45" t="s">
-        <v>692</v>
-      </c>
-      <c r="H4" s="46" t="n">
+      <c r="G8" s="44" t="s">
+        <v>705</v>
+      </c>
+      <c r="H8" s="45" t="n">
         <v>0.4</v>
       </c>
-      <c r="I4" s="47" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
-        <v>694</v>
-      </c>
-      <c r="B5" s="41" t="n">
+      <c r="I8" s="46" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="39" t="s">
+        <v>706</v>
+      </c>
+      <c r="B9" s="40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="F9" s="43" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>707</v>
+      </c>
+      <c r="H9" s="45" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="39" t="s">
+        <v>709</v>
+      </c>
+      <c r="B10" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F5" s="44" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>695</v>
-      </c>
-      <c r="H5" s="46" t="n">
+      <c r="C10" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>710</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>711</v>
+      </c>
+      <c r="H10" s="45" t="n">
         <v>0.4</v>
       </c>
-      <c r="I5" s="47" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
-        <v>697</v>
-      </c>
-      <c r="B6" s="41" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F6" s="44" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" s="45" t="s">
-        <v>698</v>
-      </c>
-      <c r="H6" s="46" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="s">
-        <v>700</v>
-      </c>
-      <c r="B7" s="41" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>336</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>701</v>
-      </c>
-      <c r="E7" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F7" s="44" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="46" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I7" s="47" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="s">
+      <c r="I10" s="46" t="s">
         <v>703</v>
-      </c>
-      <c r="B8" s="41" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>336</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F8" s="44" t="n">
-        <v>5</v>
-      </c>
-      <c r="G8" s="45" t="s">
-        <v>704</v>
-      </c>
-      <c r="H8" s="46" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I8" s="47" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="s">
-        <v>705</v>
-      </c>
-      <c r="B9" s="41" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="F9" s="44" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>706</v>
-      </c>
-      <c r="H9" s="46" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I9" s="47" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="40" t="s">
-        <v>708</v>
-      </c>
-      <c r="B10" s="41" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>709</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>710</v>
-      </c>
-      <c r="H10" s="46" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I10" s="47" t="s">
-        <v>702</v>
       </c>
     </row>
   </sheetData>
@@ -17061,7 +17078,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17070,30 +17087,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>3</v>
@@ -17105,7 +17122,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.4</v>
@@ -17116,7 +17133,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>3</v>
@@ -17128,7 +17145,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.4</v>
@@ -17139,7 +17156,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>3</v>
@@ -17151,7 +17168,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.4</v>
@@ -17162,7 +17179,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>3</v>
@@ -17174,7 +17191,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.4</v>
@@ -17185,7 +17202,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
@@ -17197,7 +17214,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
@@ -17208,7 +17225,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>3</v>
@@ -17220,7 +17237,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
@@ -17231,7 +17248,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>3</v>
@@ -17243,10 +17260,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>600</v>
@@ -17254,7 +17271,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>3</v>
@@ -17266,10 +17283,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>800</v>
@@ -17277,7 +17294,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>3</v>
@@ -17289,10 +17306,10 @@
         <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>900</v>
@@ -17300,7 +17317,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>3</v>
@@ -17312,10 +17329,10 @@
         <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1000</v>
@@ -17323,7 +17340,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>3</v>
@@ -17335,10 +17352,10 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>1000</v>
@@ -17346,7 +17363,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>3</v>
@@ -17358,10 +17375,10 @@
         <v>400</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>1500</v>
@@ -17369,30 +17386,30 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>3</v>
@@ -17404,18 +17421,18 @@
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>3</v>
@@ -17427,18 +17444,18 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>3</v>
@@ -17450,18 +17467,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>3</v>
@@ -17476,15 +17493,15 @@
         <v>580</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>3</v>
@@ -17496,18 +17513,18 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>3</v>
@@ -17519,18 +17536,18 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0.3</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>3</v>
@@ -17542,18 +17559,18 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>3</v>
@@ -17565,18 +17582,18 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2</v>
@@ -17588,18 +17605,18 @@
         <v>2</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>0</v>
@@ -17608,7 +17625,7 @@
         <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>0</v>
@@ -17619,7 +17636,7 @@
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>0</v>
@@ -17632,12 +17649,12 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>1</v>
@@ -17646,18 +17663,18 @@
         <v>30</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>15</v>
@@ -17666,7 +17683,7 @@
         <v>-5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>0</v>
@@ -17676,12 +17693,12 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="49" t="s">
-        <v>768</v>
+      <c r="H28" s="48" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="50"/>
+      <c r="E32" s="49"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -17701,54 +17718,54 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
-        <v>766</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>769</v>
-      </c>
-      <c r="C1" s="51" t="s">
+      <c r="A1" s="50" t="s">
+        <v>767</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>770</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>771</v>
       </c>
+      <c r="D1" s="50" t="s">
+        <v>772</v>
+      </c>
       <c r="E1" s="0" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>-3</v>
@@ -17765,13 +17782,13 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>90</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>-1</v>
@@ -17788,13 +17805,13 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>-1</v>
@@ -17811,13 +17828,13 @@
         <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>-1</v>
@@ -17831,16 +17848,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>-2</v>
@@ -17852,37 +17869,37 @@
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="s">
-        <v>781</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>769</v>
-      </c>
-      <c r="C7" s="51" t="s">
+      <c r="A7" s="50" t="s">
+        <v>782</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>770</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="C7" s="50" t="s">
         <v>771</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
+      <c r="D7" s="50" t="s">
+        <v>772</v>
+      </c>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>-3</v>
@@ -17896,16 +17913,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>-5</v>
@@ -17919,16 +17936,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>-4</v>
@@ -17941,17 +17958,17 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="51" t="s">
-        <v>786</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>769</v>
-      </c>
-      <c r="C11" s="51" t="s">
+      <c r="A11" s="50" t="s">
+        <v>787</v>
+      </c>
+      <c r="B11" s="50" t="s">
         <v>770</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="C11" s="50" t="s">
         <v>771</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17959,13 +17976,13 @@
         <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>-5</v>
@@ -17979,16 +17996,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>-5</v>
@@ -18000,7 +18017,7 @@
         <v>65</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18008,13 +18025,13 @@
         <v>178</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>-6</v>
@@ -18028,16 +18045,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>-5</v>
@@ -18051,16 +18068,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>90</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>-5</v>
@@ -18073,31 +18090,31 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="51" t="s">
-        <v>797</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>769</v>
-      </c>
-      <c r="C17" s="51" t="s">
+      <c r="A17" s="50" t="s">
+        <v>798</v>
+      </c>
+      <c r="B17" s="50" t="s">
         <v>770</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="C17" s="50" t="s">
         <v>771</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>-7</v>
@@ -18114,13 +18131,13 @@
         <v>469</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>-7</v>
@@ -18134,16 +18151,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>-7</v>
@@ -18160,13 +18177,13 @@
         <v>334</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>-7</v>
@@ -18180,16 +18197,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>-7</v>
@@ -18203,16 +18220,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>-7</v>
@@ -18229,13 +18246,13 @@
         <v>435</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>-7</v>
@@ -18249,16 +18266,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>-10</v>
@@ -18271,17 +18288,17 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="51" t="s">
-        <v>808</v>
-      </c>
-      <c r="B26" s="51" t="s">
-        <v>769</v>
-      </c>
-      <c r="C26" s="51" t="s">
+      <c r="A26" s="50" t="s">
+        <v>809</v>
+      </c>
+      <c r="B26" s="50" t="s">
         <v>770</v>
       </c>
-      <c r="D26" s="51" t="s">
+      <c r="C26" s="50" t="s">
         <v>771</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18289,13 +18306,13 @@
         <v>413</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>-9</v>
@@ -18312,13 +18329,13 @@
         <v>439</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>-16</v>
@@ -18332,16 +18349,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>-16</v>
@@ -18358,13 +18375,13 @@
         <v>430</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>-12</v>
@@ -18377,17 +18394,17 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="51" t="s">
-        <v>810</v>
-      </c>
-      <c r="B31" s="51" t="s">
-        <v>769</v>
-      </c>
-      <c r="C31" s="51" t="s">
+      <c r="A31" s="50" t="s">
+        <v>811</v>
+      </c>
+      <c r="B31" s="50" t="s">
         <v>770</v>
       </c>
-      <c r="D31" s="51" t="s">
+      <c r="C31" s="50" t="s">
         <v>771</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18395,13 +18412,13 @@
         <v>378</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>23</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>-5</v>
@@ -18414,17 +18431,17 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="51" t="s">
-        <v>811</v>
-      </c>
-      <c r="B33" s="51" t="s">
-        <v>769</v>
-      </c>
-      <c r="C33" s="51" t="s">
+      <c r="A33" s="50" t="s">
+        <v>812</v>
+      </c>
+      <c r="B33" s="50" t="s">
         <v>770</v>
       </c>
-      <c r="D33" s="51" t="s">
+      <c r="C33" s="50" t="s">
         <v>771</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18432,13 +18449,13 @@
         <v>149</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>-1</v>
@@ -18455,13 +18472,13 @@
         <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>-1</v>
@@ -18478,13 +18495,13 @@
         <v>464</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>16</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>-6</v>
@@ -18498,30 +18515,30 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>815</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>814</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18529,13 +18546,13 @@
         <v>529</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>30</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>-6</v>
@@ -18552,13 +18569,13 @@
         <v>211</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>30</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>-6</v>
@@ -18570,7 +18587,7 @@
         <v>147</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stały magazynek wymaga wciąż popraw. jakimś cudem nie ładuje naboi poprawnie...
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="818">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -1449,33 +1449,36 @@
     <t xml:space="preserve">Mosin Nagant</t>
   </si>
   <si>
+    <t xml:space="preserve">7,62 x 54 R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spriengfield M1903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezawaryjna, Łódeczki, Snajperka, Stary typ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steyr Scout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezawaryjna, Celna, Pośrednia, Snajperka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tłumik dźwięku [50m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezawaryjna, Celna, Niezniszczalna, Potężna, Snajperka, Ciężka</t>
+  </si>
+  <si>
     <t xml:space="preserve">7,62 × 54 R</t>
   </si>
   <si>
-    <t xml:space="preserve">Spriengfield M1903</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bezawaryjna, Łódeczki, Snajperka, Stary typ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30-06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steyr Scout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bezawaryjna, Celna, Pośrednia, Snajperka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tłumik dźwięku [50m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW 98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bezawaryjna, Celna, Niezniszczalna, Potężna, Snajperka, Ciężka</t>
-  </si>
-  <si>
     <t xml:space="preserve">02/04</t>
   </si>
   <si>
@@ -2466,10 +2469,10 @@
     <t xml:space="preserve">18$</t>
   </si>
   <si>
+    <t xml:space="preserve">7,62 x 54 r</t>
+  </si>
+  <si>
     <t xml:space="preserve">7,62 wz 43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,62 x 54 R</t>
   </si>
   <si>
     <t xml:space="preserve">22$</t>
@@ -3138,11 +3141,11 @@
   </sheetPr>
   <dimension ref="A1:P300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B98" activeCellId="0" sqref="B98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I170" activeCellId="0" sqref="I170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -11599,7 +11602,7 @@
         <v>474</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="J173" s="2" t="n">
         <v>10</v>
@@ -11608,7 +11611,7 @@
         <v>425</v>
       </c>
       <c r="L173" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="M173" s="2" t="s">
         <v>24</v>
@@ -11626,7 +11629,7 @@
     </row>
     <row r="174" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B174" s="2" t="n">
         <v>2200</v>
@@ -11647,7 +11650,7 @@
         <v>21</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="I174" s="2" t="s">
         <v>451</v>
@@ -11668,7 +11671,7 @@
         <v>11</v>
       </c>
       <c r="O174" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="P174" s="3" t="n">
         <f aca="false">D174 + 1</f>
@@ -11677,7 +11680,7 @@
     </row>
     <row r="175" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B175" s="2" t="n">
         <v>2100</v>
@@ -11698,7 +11701,7 @@
         <v>21</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="I175" s="2" t="s">
         <v>451</v>
@@ -11707,7 +11710,7 @@
         <v>5</v>
       </c>
       <c r="K175" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="L175" s="2" t="s">
         <v>432</v>
@@ -11777,7 +11780,7 @@
     </row>
     <row r="177" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>15</v>
@@ -11828,7 +11831,7 @@
     </row>
     <row r="178" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B178" s="2" t="n">
         <v>2500</v>
@@ -11849,7 +11852,7 @@
         <v>21</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="I178" s="2" t="s">
         <v>451</v>
@@ -11858,7 +11861,7 @@
         <v>5</v>
       </c>
       <c r="K178" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L178" s="2" t="s">
         <v>126</v>
@@ -11870,7 +11873,7 @@
         <v>12.5</v>
       </c>
       <c r="O178" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="P178" s="3" t="n">
         <f aca="false">D178 + 1</f>
@@ -11879,7 +11882,7 @@
     </row>
     <row r="179" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B179" s="2" t="n">
         <v>1500</v>
@@ -11900,7 +11903,7 @@
         <v>21</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="I179" s="2" t="s">
         <v>451</v>
@@ -11909,7 +11912,7 @@
         <v>10</v>
       </c>
       <c r="K179" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L179" s="2" t="s">
         <v>126</v>
@@ -11930,7 +11933,7 @@
     </row>
     <row r="180" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B180" s="2" t="n">
         <v>1400</v>
@@ -11951,7 +11954,7 @@
         <v>21</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="I180" s="2" t="s">
         <v>451</v>
@@ -11960,7 +11963,7 @@
         <v>10</v>
       </c>
       <c r="K180" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L180" s="2" t="s">
         <v>126</v>
@@ -11972,7 +11975,7 @@
         <v>12</v>
       </c>
       <c r="O180" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="P180" s="3" t="n">
         <f aca="false">D180 + 1</f>
@@ -11981,7 +11984,7 @@
     </row>
     <row r="181" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B181" s="2" t="n">
         <v>400</v>
@@ -12023,7 +12026,7 @@
         <v>4</v>
       </c>
       <c r="O181" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="P181" s="3" t="n">
         <f aca="false">D181 + 1</f>
@@ -12032,7 +12035,7 @@
     </row>
     <row r="182" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B182" s="2" t="n">
         <v>600</v>
@@ -12053,7 +12056,7 @@
         <v>170</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="I182" s="2" t="s">
         <v>365</v>
@@ -12074,7 +12077,7 @@
         <v>4.2</v>
       </c>
       <c r="O182" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="P182" s="3" t="n">
         <f aca="false">D182 + 1</f>
@@ -12083,7 +12086,7 @@
     </row>
     <row r="183" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B183" s="2" t="n">
         <v>750</v>
@@ -12104,7 +12107,7 @@
         <v>170</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I183" s="2" t="s">
         <v>365</v>
@@ -12134,7 +12137,7 @@
     </row>
     <row r="184" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B184" s="2" t="n">
         <v>750</v>
@@ -12155,7 +12158,7 @@
         <v>170</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="I184" s="2" t="s">
         <v>365</v>
@@ -12164,7 +12167,7 @@
         <v>20</v>
       </c>
       <c r="K184" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="L184" s="2" t="s">
         <v>184</v>
@@ -12176,7 +12179,7 @@
         <v>5</v>
       </c>
       <c r="O184" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="P184" s="3" t="n">
         <f aca="false">D184 + 1</f>
@@ -12185,7 +12188,7 @@
     </row>
     <row r="185" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B185" s="2" t="n">
         <v>750</v>
@@ -12206,7 +12209,7 @@
         <v>170</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="I185" s="2" t="s">
         <v>365</v>
@@ -12227,7 +12230,7 @@
         <v>5</v>
       </c>
       <c r="O185" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="P185" s="3" t="n">
         <f aca="false">D185 + 1</f>
@@ -12236,7 +12239,7 @@
     </row>
     <row r="186" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B186" s="2" t="n">
         <v>1200</v>
@@ -12257,7 +12260,7 @@
         <v>21</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="I186" s="2" t="s">
         <v>451</v>
@@ -12266,7 +12269,7 @@
         <v>10</v>
       </c>
       <c r="K186" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L186" s="2" t="s">
         <v>126</v>
@@ -12278,7 +12281,7 @@
         <v>14</v>
       </c>
       <c r="O186" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="P186" s="3" t="n">
         <f aca="false">D186 + 1</f>
@@ -12287,7 +12290,7 @@
     </row>
     <row r="187" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B187" s="2" t="n">
         <v>1400</v>
@@ -12308,7 +12311,7 @@
         <v>21</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="I187" s="2" t="s">
         <v>439</v>
@@ -12317,7 +12320,7 @@
         <v>5</v>
       </c>
       <c r="K187" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L187" s="2" t="s">
         <v>126</v>
@@ -12329,7 +12332,7 @@
         <v>14</v>
       </c>
       <c r="O187" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="P187" s="3" t="n">
         <f aca="false">D187 + 1</f>
@@ -12338,7 +12341,7 @@
     </row>
     <row r="188" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B188" s="2" t="n">
         <v>600</v>
@@ -12359,7 +12362,7 @@
         <v>170</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="I188" s="2" t="s">
         <v>365</v>
@@ -12380,7 +12383,7 @@
         <v>7.2</v>
       </c>
       <c r="O188" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="P188" s="3" t="n">
         <f aca="false">D188 + 1</f>
@@ -12389,7 +12392,7 @@
     </row>
     <row r="189" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B189" s="2" t="n">
         <v>750</v>
@@ -12410,7 +12413,7 @@
         <v>170</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I189" s="2" t="s">
         <v>324</v>
@@ -12419,10 +12422,10 @@
         <v>10</v>
       </c>
       <c r="K189" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="L189" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="M189" s="2" t="s">
         <v>24</v>
@@ -12431,7 +12434,7 @@
         <v>4.1</v>
       </c>
       <c r="O189" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="P189" s="3" t="n">
         <f aca="false">D189 + 1</f>
@@ -12440,7 +12443,7 @@
     </row>
     <row r="190" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B190" s="2" t="n">
         <v>800</v>
@@ -12461,7 +12464,7 @@
         <v>170</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I190" s="2" t="s">
         <v>365</v>
@@ -12482,7 +12485,7 @@
         <v>4.9</v>
       </c>
       <c r="O190" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="P190" s="3" t="n">
         <f aca="false">D190 + 1</f>
@@ -12584,7 +12587,7 @@
         <v>4</v>
       </c>
       <c r="O192" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="P192" s="3" t="n">
         <f aca="false">D192 + 1</f>
@@ -12593,7 +12596,7 @@
     </row>
     <row r="193" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B193" s="2" t="n">
         <v>750</v>
@@ -12614,7 +12617,7 @@
         <v>170</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="I193" s="2" t="s">
         <v>365</v>
@@ -12626,7 +12629,7 @@
         <v>179</v>
       </c>
       <c r="L193" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="M193" s="2" t="s">
         <v>220</v>
@@ -12635,7 +12638,7 @@
         <v>4.3</v>
       </c>
       <c r="O193" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P193" s="3" t="n">
         <f aca="false">D193 + 1</f>
@@ -12644,7 +12647,7 @@
     </row>
     <row r="194" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B194" s="2" t="n">
         <v>600</v>
@@ -12665,10 +12668,10 @@
         <v>170</v>
       </c>
       <c r="H194" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="J194" s="2" t="n">
         <v>10</v>
@@ -12746,7 +12749,7 @@
     </row>
     <row r="196" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B196" s="2" t="n">
         <v>600</v>
@@ -12767,7 +12770,7 @@
         <v>170</v>
       </c>
       <c r="H196" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I196" s="2" t="s">
         <v>324</v>
@@ -12776,7 +12779,7 @@
         <v>20</v>
       </c>
       <c r="K196" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="L196" s="2" t="s">
         <v>342</v>
@@ -12788,7 +12791,7 @@
         <v>4.2</v>
       </c>
       <c r="O196" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="P196" s="3" t="n">
         <f aca="false">D196 + 1</f>
@@ -12797,7 +12800,7 @@
     </row>
     <row r="197" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B197" s="2" t="n">
         <v>450</v>
@@ -12818,16 +12821,16 @@
         <v>147</v>
       </c>
       <c r="H197" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="J197" s="2" t="n">
         <v>20</v>
       </c>
       <c r="K197" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="L197" s="2" t="s">
         <v>141</v>
@@ -12897,7 +12900,7 @@
     </row>
     <row r="199" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>15</v>
@@ -12948,7 +12951,7 @@
     </row>
     <row r="200" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B200" s="2" t="n">
         <v>700</v>
@@ -12969,7 +12972,7 @@
         <v>65</v>
       </c>
       <c r="H200" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="I200" s="2" t="s">
         <v>334</v>
@@ -12978,7 +12981,7 @@
         <v>100</v>
       </c>
       <c r="K200" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L200" s="2" t="s">
         <v>126</v>
@@ -12990,7 +12993,7 @@
         <v>6.3</v>
       </c>
       <c r="O200" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="P200" s="3" t="n">
         <f aca="false">D200 + 1</f>
@@ -12999,7 +13002,7 @@
     </row>
     <row r="201" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B201" s="2" t="n">
         <v>400</v>
@@ -13020,7 +13023,7 @@
         <v>65</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="I201" s="2" t="s">
         <v>334</v>
@@ -13029,10 +13032,10 @@
         <v>30</v>
       </c>
       <c r="K201" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L201" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M201" s="2" t="s">
         <v>84</v>
@@ -13050,7 +13053,7 @@
     </row>
     <row r="202" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B202" s="2" t="n">
         <v>500</v>
@@ -13071,7 +13074,7 @@
         <v>65</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="I202" s="2" t="s">
         <v>334</v>
@@ -13080,10 +13083,10 @@
         <v>100</v>
       </c>
       <c r="K202" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L202" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M202" s="2" t="s">
         <v>84</v>
@@ -13101,7 +13104,7 @@
     </row>
     <row r="203" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B203" s="2" t="n">
         <v>800</v>
@@ -13122,7 +13125,7 @@
         <v>65</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="I203" s="2" t="s">
         <v>334</v>
@@ -13131,7 +13134,7 @@
         <v>100</v>
       </c>
       <c r="K203" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L203" s="2" t="s">
         <v>318</v>
@@ -13143,7 +13146,7 @@
         <v>12</v>
       </c>
       <c r="O203" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P203" s="3" t="n">
         <f aca="false">D203 + 1</f>
@@ -13152,7 +13155,7 @@
     </row>
     <row r="204" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B204" s="2" t="n">
         <v>400</v>
@@ -13173,7 +13176,7 @@
         <v>65</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="I204" s="2" t="s">
         <v>172</v>
@@ -13182,7 +13185,7 @@
         <v>100</v>
       </c>
       <c r="K204" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L204" s="2" t="s">
         <v>126</v>
@@ -13194,7 +13197,7 @@
         <v>7.8</v>
       </c>
       <c r="O204" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P204" s="3" t="n">
         <f aca="false">D204 + 1</f>
@@ -13203,7 +13206,7 @@
     </row>
     <row r="205" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B205" s="2" t="n">
         <v>500</v>
@@ -13224,7 +13227,7 @@
         <v>65</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="I205" s="2" t="s">
         <v>172</v>
@@ -13233,7 +13236,7 @@
         <v>100</v>
       </c>
       <c r="K205" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L205" s="2" t="s">
         <v>126</v>
@@ -13245,7 +13248,7 @@
         <v>5.1</v>
       </c>
       <c r="O205" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="P205" s="3" t="n">
         <f aca="false">D205 + 1</f>
@@ -13254,7 +13257,7 @@
     </row>
     <row r="206" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B206" s="2" t="n">
         <v>980</v>
@@ -13275,7 +13278,7 @@
         <v>65</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="I206" s="2" t="s">
         <v>334</v>
@@ -13284,7 +13287,7 @@
         <v>100</v>
       </c>
       <c r="K206" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L206" s="2" t="s">
         <v>126</v>
@@ -13296,7 +13299,7 @@
         <v>11</v>
       </c>
       <c r="O206" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="P206" s="3" t="n">
         <f aca="false">D206 + 1</f>
@@ -13305,7 +13308,7 @@
     </row>
     <row r="207" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B207" s="2" t="n">
         <v>500</v>
@@ -13326,7 +13329,7 @@
         <v>65</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="I207" s="2" t="s">
         <v>172</v>
@@ -13335,7 +13338,7 @@
         <v>100</v>
       </c>
       <c r="K207" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L207" s="2" t="s">
         <v>126</v>
@@ -13356,7 +13359,7 @@
     </row>
     <row r="208" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B208" s="2" t="n">
         <v>500</v>
@@ -13377,7 +13380,7 @@
         <v>65</v>
       </c>
       <c r="H208" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="I208" s="2" t="s">
         <v>334</v>
@@ -13386,10 +13389,10 @@
         <v>100</v>
       </c>
       <c r="K208" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L208" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="M208" s="2" t="s">
         <v>84</v>
@@ -13398,7 +13401,7 @@
         <v>10.5</v>
       </c>
       <c r="O208" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="P208" s="3" t="n">
         <f aca="false">D208 + 1</f>
@@ -13407,7 +13410,7 @@
     </row>
     <row r="209" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B209" s="2" t="n">
         <v>500</v>
@@ -13428,7 +13431,7 @@
         <v>65</v>
       </c>
       <c r="H209" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I209" s="2" t="s">
         <v>334</v>
@@ -13437,10 +13440,10 @@
         <v>100</v>
       </c>
       <c r="K209" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L209" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="M209" s="2" t="s">
         <v>84</v>
@@ -13449,7 +13452,7 @@
         <v>10.5</v>
       </c>
       <c r="O209" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="P209" s="3" t="n">
         <f aca="false">D209 + 1</f>
@@ -13458,7 +13461,7 @@
     </row>
     <row r="210" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B210" s="2" t="n">
         <v>500</v>
@@ -13479,7 +13482,7 @@
         <v>65</v>
       </c>
       <c r="H210" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="I210" s="2" t="s">
         <v>368</v>
@@ -13488,7 +13491,7 @@
         <v>100</v>
       </c>
       <c r="K210" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L210" s="2" t="s">
         <v>191</v>
@@ -13500,12 +13503,12 @@
         <v>12</v>
       </c>
       <c r="O210" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B211" s="2" t="n">
         <v>400</v>
@@ -13526,7 +13529,7 @@
         <v>65</v>
       </c>
       <c r="H211" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="I211" s="2" t="s">
         <v>172</v>
@@ -13535,7 +13538,7 @@
         <v>100</v>
       </c>
       <c r="K211" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L211" s="2" t="s">
         <v>126</v>
@@ -13556,7 +13559,7 @@
     </row>
     <row r="212" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B212" s="2" t="n">
         <v>600</v>
@@ -13577,7 +13580,7 @@
         <v>65</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="I212" s="2" t="s">
         <v>368</v>
@@ -13586,7 +13589,7 @@
         <v>100</v>
       </c>
       <c r="K212" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L212" s="2" t="s">
         <v>191</v>
@@ -13607,7 +13610,7 @@
     </row>
     <row r="213" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B213" s="2" t="n">
         <v>300</v>
@@ -13628,7 +13631,7 @@
         <v>65</v>
       </c>
       <c r="H213" s="2" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="I213" s="2" t="s">
         <v>435</v>
@@ -13679,7 +13682,7 @@
     </row>
     <row r="215" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B215" s="2" t="n">
         <v>600</v>
@@ -13700,7 +13703,7 @@
         <v>65</v>
       </c>
       <c r="H215" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="I215" s="2" t="s">
         <v>334</v>
@@ -13709,7 +13712,7 @@
         <v>100</v>
       </c>
       <c r="K215" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L215" s="2" t="s">
         <v>126</v>
@@ -13730,7 +13733,7 @@
     </row>
     <row r="216" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B216" s="2" t="n">
         <v>500</v>
@@ -13751,7 +13754,7 @@
         <v>65</v>
       </c>
       <c r="H216" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I216" s="2" t="s">
         <v>188</v>
@@ -13760,10 +13763,10 @@
         <v>100</v>
       </c>
       <c r="K216" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L216" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M216" s="2" t="s">
         <v>24</v>
@@ -13781,7 +13784,7 @@
     </row>
     <row r="217" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B217" s="2" t="n">
         <v>900</v>
@@ -13802,7 +13805,7 @@
         <v>65</v>
       </c>
       <c r="H217" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I217" s="2" t="s">
         <v>188</v>
@@ -13811,10 +13814,10 @@
         <v>100</v>
       </c>
       <c r="K217" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L217" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M217" s="2" t="s">
         <v>24</v>
@@ -13823,7 +13826,7 @@
         <v>8.2</v>
       </c>
       <c r="O217" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P217" s="3" t="n">
         <f aca="false">D217 + 1</f>
@@ -13832,7 +13835,7 @@
     </row>
     <row r="218" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B218" s="2" t="n">
         <v>400</v>
@@ -13853,7 +13856,7 @@
         <v>65</v>
       </c>
       <c r="H218" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="I218" s="2" t="s">
         <v>188</v>
@@ -13862,10 +13865,10 @@
         <v>45</v>
       </c>
       <c r="K218" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L218" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M218" s="2" t="s">
         <v>84</v>
@@ -13874,7 +13877,7 @@
         <v>6.2</v>
       </c>
       <c r="O218" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P218" s="3" t="n">
         <f aca="false">D218 + 1</f>
@@ -13883,7 +13886,7 @@
     </row>
     <row r="219" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B219" s="2" t="n">
         <v>450</v>
@@ -13904,7 +13907,7 @@
         <v>65</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="I219" s="2" t="s">
         <v>324</v>
@@ -13913,7 +13916,7 @@
         <v>100</v>
       </c>
       <c r="K219" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L219" s="2" t="s">
         <v>126</v>
@@ -13925,7 +13928,7 @@
         <v>10</v>
       </c>
       <c r="O219" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="P219" s="3" t="n">
         <f aca="false">D219 + 1</f>
@@ -13955,7 +13958,7 @@
         <v>65</v>
       </c>
       <c r="H220" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="I220" s="2" t="s">
         <v>324</v>
@@ -13964,7 +13967,7 @@
         <v>50</v>
       </c>
       <c r="K220" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L220" s="2" t="s">
         <v>184</v>
@@ -13976,7 +13979,7 @@
         <v>4</v>
       </c>
       <c r="O220" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="P220" s="3" t="n">
         <f aca="false">D220 + 1</f>
@@ -13985,7 +13988,7 @@
     </row>
     <row r="221" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B221" s="2" t="n">
         <v>900</v>
@@ -14006,7 +14009,7 @@
         <v>65</v>
       </c>
       <c r="H221" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="I221" s="2" t="s">
         <v>334</v>
@@ -14015,10 +14018,10 @@
         <v>100</v>
       </c>
       <c r="K221" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="L221" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M221" s="2" t="s">
         <v>24</v>
@@ -14027,7 +14030,7 @@
         <v>8.4</v>
       </c>
       <c r="O221" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P221" s="3" t="n">
         <f aca="false">D221 + 1</f>
@@ -14085,7 +14088,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>15</v>
@@ -14136,13 +14139,13 @@
     </row>
     <row r="224" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B224" s="2" t="n">
         <v>120</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D224" s="2" t="n">
         <v>6</v>
@@ -14154,10 +14157,10 @@
         <v>61</v>
       </c>
       <c r="G224" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H224" s="2" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="I224" s="2" t="s">
         <v>378</v>
@@ -14169,7 +14172,7 @@
         <v>15</v>
       </c>
       <c r="L224" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="M224" s="2" t="s">
         <v>24</v>
@@ -14187,7 +14190,7 @@
     </row>
     <row r="225" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B225" s="2" t="n">
         <v>120</v>
@@ -14205,10 +14208,10 @@
         <v>61</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="I225" s="2" t="s">
         <v>378</v>
@@ -14220,7 +14223,7 @@
         <v>15</v>
       </c>
       <c r="L225" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="M225" s="2" t="s">
         <v>24</v>
@@ -14289,7 +14292,7 @@
     </row>
     <row r="227" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B227" s="2" t="n">
         <v>150</v>
@@ -14307,10 +14310,10 @@
         <v>61</v>
       </c>
       <c r="G227" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H227" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="I227" s="2" t="s">
         <v>378</v>
@@ -14322,7 +14325,7 @@
         <v>15</v>
       </c>
       <c r="L227" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M227" s="2" t="s">
         <v>84</v>
@@ -14340,13 +14343,13 @@
     </row>
     <row r="228" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B228" s="2" t="n">
         <v>100</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D228" s="2" t="n">
         <v>6</v>
@@ -14361,7 +14364,7 @@
         <v>29</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="I228" s="2" t="s">
         <v>378</v>
@@ -14373,7 +14376,7 @@
         <v>15</v>
       </c>
       <c r="L228" s="2" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="M228" s="2" t="s">
         <v>84</v>
@@ -14391,13 +14394,13 @@
     </row>
     <row r="229" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B229" s="2" t="n">
         <v>120</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D229" s="2" t="n">
         <v>6</v>
@@ -14409,10 +14412,10 @@
         <v>61</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="I229" s="2" t="s">
         <v>378</v>
@@ -14424,7 +14427,7 @@
         <v>15</v>
       </c>
       <c r="L229" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M229" s="2" t="s">
         <v>24</v>
@@ -14442,7 +14445,7 @@
     </row>
     <row r="230" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B230" s="2" t="n">
         <v>70</v>
@@ -14460,10 +14463,10 @@
         <v>61</v>
       </c>
       <c r="G230" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="I230" s="2" t="s">
         <v>378</v>
@@ -14475,7 +14478,7 @@
         <v>15</v>
       </c>
       <c r="L230" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M230" s="2" t="s">
         <v>24</v>
@@ -14493,13 +14496,13 @@
     </row>
     <row r="231" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B231" s="2" t="n">
         <v>30</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D231" s="2" t="n">
         <v>5</v>
@@ -14511,10 +14514,10 @@
         <v>61</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="I231" s="2" t="s">
         <v>378</v>
@@ -14544,7 +14547,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B232" s="2" t="n">
         <v>120</v>
@@ -14562,10 +14565,10 @@
         <v>61</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="I232" s="2" t="s">
         <v>378</v>
@@ -14595,7 +14598,7 @@
     </row>
     <row r="233" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B233" s="2" t="n">
         <v>120</v>
@@ -14613,10 +14616,10 @@
         <v>61</v>
       </c>
       <c r="G233" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H233" s="2" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="I233" s="2" t="s">
         <v>378</v>
@@ -14628,7 +14631,7 @@
         <v>15</v>
       </c>
       <c r="L233" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M233" s="2" t="s">
         <v>24</v>
@@ -14695,7 +14698,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>15</v>
@@ -14746,13 +14749,13 @@
     </row>
     <row r="236" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B236" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D236" s="2" t="n">
         <v>2</v>
@@ -14767,10 +14770,10 @@
         <v>147</v>
       </c>
       <c r="H236" s="2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="I236" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="J236" s="2" t="n">
         <v>1</v>
@@ -14797,13 +14800,13 @@
     </row>
     <row r="237" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B237" s="2" t="n">
         <v>300</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D237" s="2" t="n">
         <v>2</v>
@@ -14818,10 +14821,10 @@
         <v>147</v>
       </c>
       <c r="H237" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="I237" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="J237" s="2" t="n">
         <v>1</v>
@@ -14848,13 +14851,13 @@
     </row>
     <row r="238" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B238" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D238" s="2" t="n">
         <v>0</v>
@@ -14863,16 +14866,16 @@
         <v>-4</v>
       </c>
       <c r="F238" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G238" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H238" s="2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="I238" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="J238" s="2" t="n">
         <v>1</v>
@@ -14899,13 +14902,13 @@
     </row>
     <row r="239" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B239" s="2" t="n">
         <v>125</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D239" s="2" t="n">
         <v>1</v>
@@ -14920,10 +14923,10 @@
         <v>147</v>
       </c>
       <c r="H239" s="2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="I239" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="J239" s="2" t="n">
         <v>1</v>
@@ -14950,13 +14953,13 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B240" s="2" t="n">
         <v>300</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D240" s="2" t="n">
         <v>2</v>
@@ -14971,10 +14974,10 @@
         <v>147</v>
       </c>
       <c r="H240" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="I240" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="J240" s="2" t="n">
         <v>1</v>
@@ -15001,13 +15004,13 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B241" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D241" s="2" t="n">
         <v>2</v>
@@ -15022,10 +15025,10 @@
         <v>147</v>
       </c>
       <c r="H241" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="I241" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="J241" s="2" t="n">
         <v>1</v>
@@ -15034,7 +15037,7 @@
         <v>15</v>
       </c>
       <c r="L241" s="2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="M241" s="2" t="s">
         <v>15</v>
@@ -15052,13 +15055,13 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B242" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D242" s="2" t="n">
         <v>2</v>
@@ -15073,10 +15076,10 @@
         <v>147</v>
       </c>
       <c r="H242" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="I242" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="J242" s="2" t="n">
         <v>1</v>
@@ -15103,13 +15106,13 @@
     </row>
     <row r="243" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B243" s="2" t="n">
         <v>100</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D243" s="2" t="n">
         <v>2</v>
@@ -15118,16 +15121,16 @@
         <v>-1</v>
       </c>
       <c r="F243" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G243" s="2" t="s">
         <v>147</v>
       </c>
       <c r="H243" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="I243" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="J243" s="2" t="n">
         <v>1</v>
@@ -15154,7 +15157,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>15</v>
@@ -15205,13 +15208,13 @@
     </row>
     <row r="245" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B245" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D245" s="2" t="n">
         <v>2</v>
@@ -15226,10 +15229,10 @@
         <v>65</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="I245" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="J245" s="2" t="n">
         <v>1</v>
@@ -15256,13 +15259,13 @@
     </row>
     <row r="246" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B246" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D246" s="2" t="n">
         <v>2</v>
@@ -15277,10 +15280,10 @@
         <v>65</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="I246" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J246" s="2" t="n">
         <v>1</v>
@@ -15307,13 +15310,13 @@
     </row>
     <row r="247" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B247" s="2" t="n">
         <v>400</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D247" s="2" t="n">
         <v>4</v>
@@ -15328,10 +15331,10 @@
         <v>65</v>
       </c>
       <c r="H247" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="I247" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J247" s="2" t="n">
         <v>6</v>
@@ -15340,7 +15343,7 @@
         <v>15</v>
       </c>
       <c r="L247" s="2" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="M247" s="2" t="n">
         <v>2</v>
@@ -15349,7 +15352,7 @@
         <v>5.3</v>
       </c>
       <c r="O247" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="P247" s="3" t="n">
         <f aca="false">bronbiala!D8 + 1</f>
@@ -15358,13 +15361,13 @@
     </row>
     <row r="248" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B248" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D248" s="2" t="n">
         <v>3</v>
@@ -15379,10 +15382,10 @@
         <v>65</v>
       </c>
       <c r="H248" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="I248" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J248" s="2" t="n">
         <v>1</v>
@@ -15409,13 +15412,13 @@
     </row>
     <row r="249" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B249" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D249" s="2" t="n">
         <v>3</v>
@@ -15430,10 +15433,10 @@
         <v>65</v>
       </c>
       <c r="H249" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="I249" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J249" s="2" t="n">
         <v>1</v>
@@ -15460,13 +15463,13 @@
     </row>
     <row r="250" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B250" s="2" t="n">
         <v>150</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D250" s="2" t="n">
         <v>1</v>
@@ -15481,10 +15484,10 @@
         <v>21</v>
       </c>
       <c r="H250" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="I250" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="J250" s="2" t="n">
         <v>1</v>
@@ -15511,13 +15514,13 @@
     </row>
     <row r="251" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B251" s="2" t="n">
         <v>72</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D251" s="2" t="n">
         <v>0</v>
@@ -15532,10 +15535,10 @@
         <v>21</v>
       </c>
       <c r="H251" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="I251" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="J251" s="2" t="n">
         <v>1</v>
@@ -15562,13 +15565,13 @@
     </row>
     <row r="252" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B252" s="2" t="n">
         <v>500</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D252" s="2" t="n">
         <v>1</v>
@@ -15583,10 +15586,10 @@
         <v>21</v>
       </c>
       <c r="H252" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="I252" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="J252" s="2" t="n">
         <v>1</v>
@@ -15604,7 +15607,7 @@
         <v>15</v>
       </c>
       <c r="O252" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="P252" s="3" t="n">
         <f aca="false">bronbiala!D13 + 1</f>
@@ -15613,13 +15616,13 @@
     </row>
     <row r="253" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B253" s="2" t="n">
         <v>200</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D253" s="2" t="n">
         <v>3</v>
@@ -15634,10 +15637,10 @@
         <v>65</v>
       </c>
       <c r="H253" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="I253" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J253" s="2" t="n">
         <v>4</v>
@@ -15777,7 +15780,7 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O300" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -15798,15 +15801,15 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>15</v>
@@ -15853,7 +15856,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>0</v>
@@ -15868,13 +15871,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>16</v>
@@ -15900,7 +15903,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>0</v>
@@ -15915,13 +15918,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>16</v>
@@ -15942,12 +15945,12 @@
         <v>0.5</v>
       </c>
       <c r="O3" s="25" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="39.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B4" s="27" t="n">
         <v>1.5</v>
@@ -15968,10 +15971,10 @@
         <v>65</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>15</v>
@@ -15989,12 +15992,12 @@
         <v>0.4</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>1</v>
@@ -16013,10 +16016,10 @@
         <v>65</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>15</v>
@@ -16034,12 +16037,12 @@
         <v>0.4</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>0</v>
@@ -16060,10 +16063,10 @@
         <v>65</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>15</v>
@@ -16081,12 +16084,12 @@
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0.5</v>
@@ -16104,13 +16107,13 @@
         <v>64</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>15</v>
@@ -16128,12 +16131,12 @@
         <v>1.5</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>1</v>
@@ -16151,13 +16154,13 @@
         <v>35</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>15</v>
@@ -16175,12 +16178,12 @@
         <v>0.1</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0</v>
@@ -16198,13 +16201,13 @@
         <v>15</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>15</v>
@@ -16222,12 +16225,12 @@
         <v>0.4</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0</v>
@@ -16242,16 +16245,16 @@
         <v>0</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>15</v>
@@ -16274,7 +16277,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>1</v>
@@ -16314,12 +16317,12 @@
         <v>1</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0.5</v>
@@ -16340,10 +16343,10 @@
         <v>65</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>15</v>
@@ -16366,7 +16369,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="34" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>1.5</v>
@@ -16411,7 +16414,7 @@
     </row>
     <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>2</v>
@@ -16432,7 +16435,7 @@
         <v>65</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>127</v>
@@ -16453,12 +16456,12 @@
         <v>0.3</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="34" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0</v>
@@ -16479,10 +16482,10 @@
         <v>65</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>15</v>
@@ -16500,12 +16503,12 @@
         <v>0.4</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0</v>
@@ -16526,10 +16529,10 @@
         <v>65</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>15</v>
@@ -16547,12 +16550,12 @@
         <v>0.5</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0.5</v>
@@ -16570,13 +16573,13 @@
         <v>64</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J17" s="12" t="s">
         <v>15</v>
@@ -16599,7 +16602,7 @@
     </row>
     <row r="18" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>1</v>
@@ -16620,7 +16623,7 @@
         <v>65</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>134</v>
@@ -16641,12 +16644,12 @@
         <v>0.2</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="34" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0</v>
@@ -16661,16 +16664,16 @@
         <v>0</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>15</v>
@@ -16688,12 +16691,12 @@
         <v>1</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B20" s="5" t="n">
         <v>0.5</v>
@@ -16714,10 +16717,10 @@
         <v>65</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="13"/>
@@ -16766,40 +16769,40 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="H1" s="37" t="s">
         <v>36</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B2" s="40" t="n">
         <v>6</v>
@@ -16811,24 +16814,24 @@
         <v>15</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F2" s="43" t="n">
         <v>5</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="H2" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B3" s="40" t="n">
         <v>5</v>
@@ -16837,27 +16840,27 @@
         <v>336</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E3" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F3" s="43" t="n">
         <v>5</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I3" s="46" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="39" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B4" s="40" t="n">
         <v>5</v>
@@ -16869,24 +16872,24 @@
         <v>15</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F4" s="43" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H4" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B5" s="40" t="n">
         <v>5</v>
@@ -16898,24 +16901,24 @@
         <v>15</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F5" s="43" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="H5" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="39" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B6" s="40" t="n">
         <v>6</v>
@@ -16927,24 +16930,24 @@
         <v>15</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F6" s="43" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="H6" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="39" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B7" s="40" t="n">
         <v>2</v>
@@ -16953,10 +16956,10 @@
         <v>336</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F7" s="43" t="n">
         <v>5</v>
@@ -16966,12 +16969,12 @@
         <v>0.4</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="39" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B8" s="40" t="n">
         <v>5</v>
@@ -16983,24 +16986,24 @@
         <v>15</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F8" s="43" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="H8" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B9" s="40" t="n">
         <v>3</v>
@@ -17012,24 +17015,24 @@
         <v>15</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F9" s="43" t="n">
         <v>4</v>
       </c>
       <c r="G9" s="44" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H9" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I9" s="46" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B10" s="40" t="n">
         <v>5</v>
@@ -17038,7 +17041,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>15</v>
@@ -17047,13 +17050,13 @@
         <v>15</v>
       </c>
       <c r="G10" s="44" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="H10" s="45" t="n">
         <v>0.4</v>
       </c>
       <c r="I10" s="46" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -17078,7 +17081,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17087,30 +17090,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>3</v>
@@ -17122,7 +17125,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.4</v>
@@ -17133,7 +17136,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>3</v>
@@ -17145,7 +17148,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.4</v>
@@ -17156,7 +17159,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>3</v>
@@ -17168,7 +17171,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.4</v>
@@ -17179,7 +17182,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>3</v>
@@ -17191,7 +17194,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.4</v>
@@ -17202,7 +17205,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
@@ -17214,7 +17217,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
@@ -17225,7 +17228,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>3</v>
@@ -17237,7 +17240,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
@@ -17248,7 +17251,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>3</v>
@@ -17260,10 +17263,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>600</v>
@@ -17271,7 +17274,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>3</v>
@@ -17283,10 +17286,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>800</v>
@@ -17294,7 +17297,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>3</v>
@@ -17306,10 +17309,10 @@
         <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>900</v>
@@ -17317,7 +17320,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>3</v>
@@ -17329,10 +17332,10 @@
         <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1000</v>
@@ -17340,7 +17343,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>3</v>
@@ -17352,10 +17355,10 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>1000</v>
@@ -17363,7 +17366,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>3</v>
@@ -17375,10 +17378,10 @@
         <v>400</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>1500</v>
@@ -17386,30 +17389,30 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>3</v>
@@ -17421,18 +17424,18 @@
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>3</v>
@@ -17444,18 +17447,18 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>3</v>
@@ -17467,18 +17470,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>3</v>
@@ -17490,18 +17493,18 @@
         <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>3</v>
@@ -17513,18 +17516,18 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>3</v>
@@ -17536,18 +17539,18 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0.3</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>3</v>
@@ -17559,18 +17562,18 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>3</v>
@@ -17582,18 +17585,18 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2</v>
@@ -17605,18 +17608,18 @@
         <v>2</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>0</v>
@@ -17625,7 +17628,7 @@
         <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>0</v>
@@ -17636,7 +17639,7 @@
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>0</v>
@@ -17649,12 +17652,12 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>1</v>
@@ -17663,18 +17666,18 @@
         <v>30</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>15</v>
@@ -17683,7 +17686,7 @@
         <v>-5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>0</v>
@@ -17694,7 +17697,7 @@
     </row>
     <row r="28" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="48" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17716,13 +17719,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -17730,42 +17733,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="50" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>-3</v>
@@ -17782,13 +17785,13 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>90</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>-1</v>
@@ -17805,13 +17808,13 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>-1</v>
@@ -17828,13 +17831,13 @@
         <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>-1</v>
@@ -17848,16 +17851,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>-2</v>
@@ -17869,21 +17872,21 @@
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="50" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="H7" s="51"/>
       <c r="I7" s="51"/>
@@ -17893,13 +17896,13 @@
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>-3</v>
@@ -17913,16 +17916,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>-5</v>
@@ -17936,16 +17939,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>-4</v>
@@ -17959,16 +17962,16 @@
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="50" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17976,13 +17979,13 @@
         <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>-5</v>
@@ -17996,16 +17999,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>-5</v>
@@ -18017,7 +18020,7 @@
         <v>65</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18025,13 +18028,13 @@
         <v>178</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>-6</v>
@@ -18045,16 +18048,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>-5</v>
@@ -18068,16 +18071,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>90</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>-5</v>
@@ -18091,30 +18094,30 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="50" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>-7</v>
@@ -18131,13 +18134,13 @@
         <v>469</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>-7</v>
@@ -18151,16 +18154,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>-7</v>
@@ -18177,13 +18180,13 @@
         <v>334</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>-7</v>
@@ -18195,18 +18198,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>-7</v>
@@ -18218,18 +18221,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>694</v>
+        <v>805</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>-7</v>
@@ -18241,18 +18244,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>807</v>
+        <v>695</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>-7</v>
@@ -18264,101 +18267,101 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>808</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>800</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>801</v>
-      </c>
       <c r="E25" s="2" t="n">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>336</v>
+        <v>116</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="50" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>809</v>
       </c>
-      <c r="B26" s="50" t="s">
-        <v>770</v>
-      </c>
-      <c r="C26" s="50" t="s">
+      <c r="B26" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>-10</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="50" t="s">
+        <v>810</v>
+      </c>
+      <c r="B27" s="50" t="s">
         <v>771</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="C27" s="50" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>803</v>
-      </c>
-      <c r="C27" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>-9</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>147</v>
+      <c r="D27" s="50" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>703</v>
+        <v>790</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>-16</v>
+        <v>-9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>21</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>810</v>
+        <v>439</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>-16</v>
@@ -18372,19 +18375,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>430</v>
+        <v>811</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>428</v>
@@ -18393,92 +18396,92 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="50" t="s">
-        <v>811</v>
-      </c>
-      <c r="B31" s="50" t="s">
-        <v>770</v>
-      </c>
-      <c r="C31" s="50" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>-12</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="50" t="s">
+        <v>812</v>
+      </c>
+      <c r="B32" s="50" t="s">
         <v>771</v>
       </c>
-      <c r="D31" s="50" t="s">
+      <c r="C32" s="50" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="D32" s="50" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="C32" s="2" t="n">
+      <c r="B33" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="C33" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>694</v>
-      </c>
-      <c r="E32" s="2" t="n">
+      <c r="D33" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="E33" s="2" t="n">
         <v>-5</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="50" t="s">
-        <v>812</v>
-      </c>
-      <c r="B33" s="50" t="s">
-        <v>770</v>
-      </c>
-      <c r="C33" s="50" t="s">
+      <c r="G33" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="50" t="s">
+        <v>813</v>
+      </c>
+      <c r="B34" s="50" t="s">
         <v>771</v>
       </c>
-      <c r="D33" s="50" t="s">
+      <c r="C34" s="50" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="C34" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>147</v>
+      <c r="D34" s="50" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>75</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>-1</v>
@@ -18490,92 +18493,92 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>464</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>788</v>
+        <v>778</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>801</v>
+        <v>814</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>-6</v>
+        <v>-1</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>814</v>
+        <v>464</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>815</v>
+        <v>789</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>703</v>
+        <v>802</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>816</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>815</v>
-      </c>
       <c r="C38" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="C39" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>788</v>
-      </c>
-      <c r="C39" s="2" t="n">
-        <v>30</v>
-      </c>
       <c r="D39" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>789</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>-6</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>788</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>30</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>-6</v>
@@ -18586,8 +18589,31 @@
       <c r="G40" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H40" s="0" t="s">
-        <v>781</v>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
przygotowane początek różnych amunicji.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="805">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -2388,15 +2388,9 @@
     <t xml:space="preserve">pistoletowe</t>
   </si>
   <si>
-    <t xml:space="preserve">25$</t>
-  </si>
-  <si>
     <t xml:space="preserve">ACP'45</t>
   </si>
   <si>
-    <t xml:space="preserve">17$</t>
-  </si>
-  <si>
     <t xml:space="preserve">wytłumiona</t>
   </si>
   <si>
@@ -2406,9 +2400,6 @@
     <t xml:space="preserve">rewolwerowe</t>
   </si>
   <si>
-    <t xml:space="preserve">105$</t>
-  </si>
-  <si>
     <t xml:space="preserve">AE'50</t>
   </si>
   <si>
@@ -2421,33 +2412,18 @@
     <t xml:space="preserve">pośrednie</t>
   </si>
   <si>
-    <t xml:space="preserve">45$</t>
-  </si>
-  <si>
     <t xml:space="preserve">‘300 AAC Blackout</t>
   </si>
   <si>
-    <t xml:space="preserve">47$</t>
-  </si>
-  <si>
     <t xml:space="preserve">zasieg skuteczny -100m, zasieg skuteczny &lt;500</t>
   </si>
   <si>
-    <t xml:space="preserve">75$</t>
-  </si>
-  <si>
     <t xml:space="preserve">5,8 x 42</t>
   </si>
   <si>
-    <t xml:space="preserve">36$</t>
-  </si>
-  <si>
     <t xml:space="preserve">5,45 x 39</t>
   </si>
   <si>
-    <t xml:space="preserve">54$</t>
-  </si>
-  <si>
     <t xml:space="preserve">Karabinowe</t>
   </si>
   <si>
@@ -2457,24 +2433,15 @@
     <t xml:space="preserve">karabinowe</t>
   </si>
   <si>
-    <t xml:space="preserve">15$</t>
-  </si>
-  <si>
     <t xml:space="preserve">6,5 Creedmoor</t>
   </si>
   <si>
     <t xml:space="preserve">wyborowe</t>
   </si>
   <si>
-    <t xml:space="preserve">18$</t>
-  </si>
-  <si>
     <t xml:space="preserve">7,62 wz 43</t>
   </si>
   <si>
-    <t xml:space="preserve">22$</t>
-  </si>
-  <si>
     <t xml:space="preserve">Beowolf '50</t>
   </si>
   <si>
@@ -2488,9 +2455,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nieulepszalne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70$</t>
   </si>
   <si>
     <t xml:space="preserve">Strzały</t>
@@ -3142,7 +3106,7 @@
       <selection pane="topLeft" activeCell="I170" activeCellId="0" sqref="I170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15802,7 +15766,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -16766,7 +16730,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -17078,7 +17042,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17719,10 +17683,10 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -17754,7 +17718,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>777</v>
       </c>
@@ -17764,8 +17728,8 @@
       <c r="C2" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>779</v>
+      <c r="D2" s="2" t="n">
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>-3</v>
@@ -17787,8 +17751,8 @@
       <c r="C3" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>695</v>
+      <c r="D3" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>-1</v>
@@ -17800,7 +17764,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -17810,8 +17774,8 @@
       <c r="C4" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>695</v>
+      <c r="D4" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>-1</v>
@@ -17833,8 +17797,8 @@
       <c r="C5" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>695</v>
+      <c r="D5" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>-1</v>
@@ -17848,7 +17812,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>778</v>
@@ -17856,8 +17820,8 @@
       <c r="C6" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>781</v>
+      <c r="D6" s="2" t="n">
+        <v>17</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>-2</v>
@@ -17869,12 +17833,12 @@
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="50" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>771</v>
@@ -17893,13 +17857,13 @@
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>785</v>
+      <c r="D8" s="2" t="n">
+        <v>105</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>-3</v>
@@ -17913,16 +17877,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>692</v>
+      <c r="D9" s="2" t="n">
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>-5</v>
@@ -17936,16 +17900,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>701</v>
+      <c r="D10" s="2" t="n">
+        <v>80</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>-4</v>
@@ -17959,7 +17923,7 @@
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="50" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B11" s="50" t="s">
         <v>771</v>
@@ -17976,13 +17940,13 @@
         <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>790</v>
+      <c r="D12" s="2" t="n">
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>-5</v>
@@ -17994,18 +17958,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>792</v>
+      <c r="D13" s="2" t="n">
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>-5</v>
@@ -18017,7 +17981,7 @@
         <v>65</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18025,13 +17989,13 @@
         <v>178</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>794</v>
+      <c r="D14" s="2" t="n">
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>-6</v>
@@ -18045,16 +18009,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>796</v>
+      <c r="D15" s="2" t="n">
+        <v>36</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>-5</v>
@@ -18068,16 +18032,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>797</v>
+        <v>790</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>798</v>
+      <c r="D16" s="2" t="n">
+        <v>54</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>-5</v>
@@ -18091,7 +18055,7 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="50" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="B17" s="50" t="s">
         <v>771</v>
@@ -18105,16 +18069,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>802</v>
+      <c r="D18" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>-7</v>
@@ -18131,13 +18095,13 @@
         <v>469</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>695</v>
+      <c r="D19" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>-7</v>
@@ -18151,16 +18115,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>695</v>
+      <c r="D20" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>-7</v>
@@ -18177,13 +18141,13 @@
         <v>334</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>805</v>
+      <c r="D21" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>-7</v>
@@ -18200,13 +18164,13 @@
         <v>466</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>805</v>
+      <c r="D22" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>-7</v>
@@ -18220,16 +18184,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>806</v>
+        <v>796</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>805</v>
+      <c r="D23" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>-7</v>
@@ -18246,13 +18210,13 @@
         <v>439</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>695</v>
+      <c r="D24" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>-7</v>
@@ -18264,18 +18228,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>435</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>807</v>
+      <c r="D25" s="2" t="n">
+        <v>22</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>-7</v>
@@ -18289,16 +18253,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>808</v>
+        <v>797</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>802</v>
+      <c r="D26" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>-10</v>
@@ -18312,7 +18276,7 @@
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="50" t="s">
-        <v>809</v>
+        <v>798</v>
       </c>
       <c r="B27" s="50" t="s">
         <v>771</v>
@@ -18329,13 +18293,13 @@
         <v>413</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>790</v>
+      <c r="D28" s="2" t="n">
+        <v>45</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>-9</v>
@@ -18352,13 +18316,13 @@
         <v>439</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>704</v>
+      <c r="D29" s="2" t="n">
+        <v>50</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>-16</v>
@@ -18372,16 +18336,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>810</v>
+        <v>799</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>704</v>
+      <c r="D30" s="2" t="n">
+        <v>50</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>-16</v>
@@ -18398,13 +18362,13 @@
         <v>430</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>704</v>
+      <c r="D31" s="2" t="n">
+        <v>50</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>-12</v>
@@ -18418,7 +18382,7 @@
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="50" t="s">
-        <v>811</v>
+        <v>800</v>
       </c>
       <c r="B32" s="50" t="s">
         <v>771</v>
@@ -18440,8 +18404,8 @@
       <c r="C33" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>695</v>
+      <c r="D33" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>-5</v>
@@ -18455,7 +18419,7 @@
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="50" t="s">
-        <v>812</v>
+        <v>801</v>
       </c>
       <c r="B34" s="50" t="s">
         <v>771</v>
@@ -18467,7 +18431,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>149</v>
       </c>
@@ -18477,8 +18441,8 @@
       <c r="C35" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>813</v>
+      <c r="D35" s="2" t="n">
+        <v>70</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>-1</v>
@@ -18490,7 +18454,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -18500,8 +18464,8 @@
       <c r="C36" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>813</v>
+      <c r="D36" s="2" t="n">
+        <v>70</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>-1</v>
@@ -18518,13 +18482,13 @@
         <v>464</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>802</v>
+      <c r="D37" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>-6</v>
@@ -18538,44 +18502,44 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>814</v>
+        <v>802</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>815</v>
+        <v>803</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>704</v>
+      <c r="D38" s="2" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>816</v>
+        <v>804</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>815</v>
+        <v>803</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>530</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>790</v>
+      <c r="D40" s="2" t="n">
+        <v>45</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>-6</v>
@@ -18592,13 +18556,13 @@
         <v>211</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>790</v>
+      <c r="D41" s="2" t="n">
+        <v>45</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>-6</v>
@@ -18610,7 +18574,7 @@
         <v>147</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zrobiona maksymalny zasięg amunicji.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2948" uniqueCount="806">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -2380,6 +2380,9 @@
   </si>
   <si>
     <t xml:space="preserve">penetracja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maksymalny zasięg</t>
   </si>
   <si>
     <t xml:space="preserve">'40 S&amp;W</t>
@@ -3106,7 +3109,7 @@
       <selection pane="topLeft" activeCell="I170" activeCellId="0" sqref="I170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15766,7 +15769,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -16730,7 +16733,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -17042,7 +17045,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17683,10 +17686,10 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -17717,13 +17720,16 @@
       <c r="H1" s="0" t="s">
         <v>717</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>60</v>
@@ -17739,6 +17745,9 @@
       </c>
       <c r="G2" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17746,7 +17755,7 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>90</v>
@@ -17762,6 +17771,9 @@
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17769,7 +17781,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>80</v>
@@ -17785,6 +17797,9 @@
       </c>
       <c r="G4" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17792,7 +17807,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80</v>
@@ -17809,13 +17824,16 @@
       <c r="G5" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>779</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>778</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>50</v>
@@ -17833,12 +17851,15 @@
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="50" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>771</v>
@@ -17857,7 +17878,7 @@
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
@@ -17874,13 +17895,16 @@
       <c r="G8" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>783</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>782</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>20</v>
@@ -17897,13 +17921,16 @@
       <c r="G9" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>20</v>
@@ -17920,10 +17947,13 @@
       <c r="G10" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="50" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B11" s="50" t="s">
         <v>771</v>
@@ -17940,7 +17970,7 @@
         <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>75</v>
@@ -17957,13 +17987,16 @@
       <c r="G12" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>60</v>
@@ -17981,7 +18014,10 @@
         <v>65</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>788</v>
+        <v>789</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17989,7 +18025,7 @@
         <v>178</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>50</v>
@@ -18006,13 +18042,16 @@
       <c r="G14" s="2" t="s">
         <v>170</v>
       </c>
+      <c r="I14" s="0" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>60</v>
@@ -18029,13 +18068,16 @@
       <c r="G15" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I15" s="0" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>90</v>
@@ -18052,10 +18094,13 @@
       <c r="G16" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I16" s="0" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="50" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B17" s="50" t="s">
         <v>771</v>
@@ -18069,10 +18114,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>20</v>
@@ -18089,13 +18134,16 @@
       <c r="G18" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>469</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
@@ -18112,13 +18160,16 @@
       <c r="G19" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="I19" s="0" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
@@ -18134,6 +18185,9 @@
       </c>
       <c r="G20" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>600</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18141,7 +18195,7 @@
         <v>334</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
@@ -18157,6 +18211,9 @@
       </c>
       <c r="G21" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18164,7 +18221,7 @@
         <v>466</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>20</v>
@@ -18181,13 +18238,16 @@
       <c r="G22" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I22" s="0" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
@@ -18203,6 +18263,9 @@
       </c>
       <c r="G23" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18210,7 +18273,7 @@
         <v>439</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>20</v>
@@ -18226,6 +18289,9 @@
       </c>
       <c r="G24" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18233,7 +18299,7 @@
         <v>435</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>20</v>
@@ -18250,13 +18316,16 @@
       <c r="G25" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I25" s="0" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>10</v>
@@ -18273,10 +18342,13 @@
       <c r="G26" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I26" s="0" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="50" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B27" s="50" t="s">
         <v>771</v>
@@ -18293,7 +18365,7 @@
         <v>413</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>15</v>
@@ -18309,6 +18381,9 @@
       </c>
       <c r="G28" s="2" t="s">
         <v>147</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18316,7 +18391,7 @@
         <v>439</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>10</v>
@@ -18333,13 +18408,16 @@
       <c r="G29" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="I29" s="0" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
@@ -18355,6 +18433,9 @@
       </c>
       <c r="G30" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18362,7 +18443,7 @@
         <v>430</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>10</v>
@@ -18379,10 +18460,13 @@
       <c r="G31" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="I31" s="0" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="50" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B32" s="50" t="s">
         <v>771</v>
@@ -18399,7 +18483,7 @@
         <v>378</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>23</v>
@@ -18416,10 +18500,13 @@
       <c r="G33" s="2" t="s">
         <v>584</v>
       </c>
+      <c r="I33" s="0" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="50" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B34" s="50" t="s">
         <v>771</v>
@@ -18436,7 +18523,7 @@
         <v>149</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>75</v>
@@ -18452,6 +18539,9 @@
       </c>
       <c r="G35" s="2" t="s">
         <v>147</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18459,7 +18549,7 @@
         <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>75</v>
@@ -18475,6 +18565,9 @@
       </c>
       <c r="G36" s="2" t="s">
         <v>147</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18482,7 +18575,7 @@
         <v>464</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>16</v>
@@ -18499,13 +18592,16 @@
       <c r="G37" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="I37" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>10</v>
@@ -18513,19 +18609,25 @@
       <c r="D38" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="I38" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>804</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>803</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>10000</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18533,7 +18635,7 @@
         <v>530</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>30</v>
@@ -18549,6 +18651,9 @@
       </c>
       <c r="G40" s="2" t="s">
         <v>147</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>10000</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18556,7 +18661,7 @@
         <v>211</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>30</v>
@@ -18574,7 +18679,10 @@
         <v>147</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duży kaliber uwzględniony, bez interakcji z celownikiem.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -3109,7 +3109,7 @@
       <selection pane="topLeft" activeCell="I170" activeCellId="0" sqref="I170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15769,7 +15769,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -16733,7 +16733,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -17045,7 +17045,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17685,11 +17685,11 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -18541,7 +18541,7 @@
         <v>147</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18567,7 +18567,7 @@
         <v>147</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18593,7 +18593,7 @@
         <v>81</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>10000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18610,7 +18610,7 @@
         <v>50</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>10000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18627,7 +18627,7 @@
         <v>50</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>10000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18653,7 +18653,7 @@
         <v>147</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>10000</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18682,7 +18682,7 @@
         <v>781</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>10000</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
złożenie do strzału io zrywanie zrobione, i strzelanie z biodra, tylko że strzelanie z scouta nie działa....
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3199" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3200" uniqueCount="808">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -2212,6 +2212,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czas do złożenia się</t>
   </si>
   <si>
     <t xml:space="preserve">ACOGx1,5</t>
@@ -2820,7 +2823,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3018,6 +3021,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3108,11 +3115,11 @@
   </sheetPr>
   <dimension ref="A1:P300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I169" activeCellId="0" sqref="I169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -16681,7 +16688,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -18013,7 +18020,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -18321,15 +18328,15 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="81.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18354,10 +18361,13 @@
       <c r="G1" s="2" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="0" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B2" s="48" t="n">
         <v>3</v>
@@ -18369,7 +18379,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.4</v>
@@ -18377,10 +18387,13 @@
       <c r="G2" s="2" t="n">
         <v>1300</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>3</v>
@@ -18392,7 +18405,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.4</v>
@@ -18400,10 +18413,13 @@
       <c r="G3" s="2" t="n">
         <v>1600</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>3</v>
@@ -18415,7 +18431,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.4</v>
@@ -18423,10 +18439,13 @@
       <c r="G4" s="2" t="n">
         <v>1700</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>3</v>
@@ -18438,7 +18457,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.4</v>
@@ -18446,10 +18465,13 @@
       <c r="G5" s="2" t="n">
         <v>2800</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
@@ -18461,7 +18483,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
@@ -18469,10 +18491,13 @@
       <c r="G6" s="2" t="n">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>3</v>
@@ -18484,7 +18509,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
@@ -18492,10 +18517,13 @@
       <c r="G7" s="2" t="n">
         <v>1500</v>
       </c>
+      <c r="H7" s="49" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B8" s="48" t="n">
         <v>3</v>
@@ -18507,18 +18535,21 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>600</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>3</v>
@@ -18530,18 +18561,21 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>800</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>3</v>
@@ -18553,18 +18587,21 @@
         <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>900</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>3</v>
@@ -18576,18 +18613,21 @@
         <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1000</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>3</v>
@@ -18599,18 +18639,21 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>1000</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>3</v>
@@ -18622,18 +18665,21 @@
         <v>400</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>1500</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>715</v>
@@ -18642,21 +18688,22 @@
         <v>716</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="49"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B15" s="48" t="n">
         <v>3</v>
@@ -18668,18 +18715,21 @@
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>744</v>
+      </c>
+      <c r="H15" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>3</v>
@@ -18691,18 +18741,21 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>748</v>
+      </c>
+      <c r="H16" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>3</v>
@@ -18714,18 +18767,21 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>750</v>
+      </c>
+      <c r="H17" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>3</v>
@@ -18740,15 +18796,18 @@
         <v>580</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>752</v>
+      </c>
+      <c r="H18" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>3</v>
@@ -18760,18 +18819,21 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>755</v>
+      </c>
+      <c r="H19" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>3</v>
@@ -18783,7 +18845,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0.3</v>
@@ -18791,10 +18853,13 @@
       <c r="G20" s="2" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>3</v>
@@ -18806,18 +18871,21 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H21" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>3</v>
@@ -18829,18 +18897,21 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2</v>
@@ -18852,18 +18923,21 @@
         <v>2</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>764</v>
+      </c>
+      <c r="H23" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B24" s="48" t="n">
         <v>0</v>
@@ -18872,7 +18946,7 @@
         <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>0</v>
@@ -18880,10 +18954,13 @@
       <c r="G24" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>0</v>
@@ -18898,10 +18975,13 @@
       <c r="G25" s="2" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>1</v>
@@ -18910,18 +18990,21 @@
         <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>748</v>
+      </c>
+      <c r="H26" s="49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>15</v>
@@ -18930,7 +19013,7 @@
         <v>-5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>0</v>
@@ -18938,14 +19021,15 @@
       <c r="G27" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="H27" s="49"/>
     </row>
     <row r="28" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="48" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="49"/>
+      <c r="E32" s="50"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -18969,47 +19053,47 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="50" t="s">
-        <v>769</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>772</v>
-      </c>
-      <c r="C1" s="50" t="s">
+      <c r="A1" s="51" t="s">
+        <v>770</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>773</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="51" t="s">
         <v>774</v>
       </c>
+      <c r="D1" s="51" t="s">
+        <v>775</v>
+      </c>
       <c r="E1" s="0" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>718</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>60</v>
@@ -19035,7 +19119,7 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>90</v>
@@ -19061,7 +19145,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>80</v>
@@ -19087,7 +19171,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80</v>
@@ -19110,10 +19194,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>781</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>780</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>50</v>
@@ -19131,34 +19215,34 @@
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="50" t="s">
-        <v>783</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>772</v>
-      </c>
-      <c r="C7" s="50" t="s">
+      <c r="A7" s="51" t="s">
+        <v>784</v>
+      </c>
+      <c r="B7" s="51" t="s">
         <v>773</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="C7" s="51" t="s">
         <v>774</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
+      <c r="D7" s="51" t="s">
+        <v>775</v>
+      </c>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
@@ -19181,10 +19265,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>785</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>784</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>20</v>
@@ -19207,10 +19291,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>20</v>
@@ -19232,17 +19316,17 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="50" t="s">
-        <v>787</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>772</v>
-      </c>
-      <c r="C11" s="50" t="s">
+      <c r="A11" s="51" t="s">
+        <v>788</v>
+      </c>
+      <c r="B11" s="51" t="s">
         <v>773</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="C11" s="51" t="s">
         <v>774</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19250,7 +19334,7 @@
         <v>171</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>75</v>
@@ -19276,7 +19360,7 @@
         <v>312</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>75</v>
@@ -19299,10 +19383,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>60</v>
@@ -19320,7 +19404,7 @@
         <v>65</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>300</v>
@@ -19331,7 +19415,7 @@
         <v>176</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>50</v>
@@ -19354,10 +19438,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>60</v>
@@ -19380,10 +19464,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>90</v>
@@ -19405,25 +19489,25 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="50" t="s">
-        <v>793</v>
-      </c>
-      <c r="B18" s="50" t="s">
-        <v>772</v>
-      </c>
-      <c r="C18" s="50" t="s">
+      <c r="A18" s="51" t="s">
+        <v>794</v>
+      </c>
+      <c r="B18" s="51" t="s">
         <v>773</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="C18" s="51" t="s">
         <v>774</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
@@ -19449,7 +19533,7 @@
         <v>351</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
@@ -19472,10 +19556,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
@@ -19501,7 +19585,7 @@
         <v>332</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>20</v>
@@ -19527,7 +19611,7 @@
         <v>467</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
@@ -19550,10 +19634,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>20</v>
@@ -19579,7 +19663,7 @@
         <v>440</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>20</v>
@@ -19605,7 +19689,7 @@
         <v>436</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>20</v>
@@ -19628,10 +19712,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>10</v>
@@ -19653,17 +19737,17 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="50" t="s">
-        <v>800</v>
-      </c>
-      <c r="B28" s="50" t="s">
-        <v>772</v>
-      </c>
-      <c r="C28" s="50" t="s">
+      <c r="A28" s="51" t="s">
+        <v>801</v>
+      </c>
+      <c r="B28" s="51" t="s">
         <v>773</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="C28" s="51" t="s">
         <v>774</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19671,7 +19755,7 @@
         <v>414</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>15</v>
@@ -19697,7 +19781,7 @@
         <v>440</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
@@ -19720,10 +19804,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>10</v>
@@ -19749,7 +19833,7 @@
         <v>431</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>10</v>
@@ -19771,17 +19855,17 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="50" t="s">
-        <v>802</v>
-      </c>
-      <c r="B33" s="50" t="s">
-        <v>772</v>
-      </c>
-      <c r="C33" s="50" t="s">
+      <c r="A33" s="51" t="s">
+        <v>803</v>
+      </c>
+      <c r="B33" s="51" t="s">
         <v>773</v>
       </c>
-      <c r="D33" s="50" t="s">
+      <c r="C33" s="51" t="s">
         <v>774</v>
+      </c>
+      <c r="D33" s="51" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19789,7 +19873,7 @@
         <v>377</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>23</v>
@@ -19811,17 +19895,17 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="50" t="s">
-        <v>803</v>
-      </c>
-      <c r="B35" s="50" t="s">
-        <v>772</v>
-      </c>
-      <c r="C35" s="50" t="s">
+      <c r="A35" s="51" t="s">
+        <v>804</v>
+      </c>
+      <c r="B35" s="51" t="s">
         <v>773</v>
       </c>
-      <c r="D35" s="50" t="s">
+      <c r="C35" s="51" t="s">
         <v>774</v>
+      </c>
+      <c r="D35" s="51" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19829,7 +19913,7 @@
         <v>149</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>75</v>
@@ -19855,7 +19939,7 @@
         <v>66</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>75</v>
@@ -19881,7 +19965,7 @@
         <v>465</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>16</v>
@@ -19904,10 +19988,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>10</v>
@@ -19921,10 +20005,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>806</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>805</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>20</v>
@@ -19941,7 +20025,7 @@
         <v>529</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>30</v>
@@ -19967,7 +20051,7 @@
         <v>209</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>30</v>
@@ -19985,7 +20069,7 @@
         <v>147</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>400</v>

</xml_diff>

<commit_message>
naprawiono masę baboli. Jeszcze masa rzeczy do wytestowania... po zrobieniu wprawy czas na duże testowanie.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -18328,8 +18328,8 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Celowniki w toku (już jako dodatki
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3200" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3211" uniqueCount="809">
   <si>
     <t xml:space="preserve">Zasięg [m]</t>
   </si>
@@ -2208,21 +2208,27 @@
     <t xml:space="preserve">specjalne</t>
   </si>
   <si>
+    <t xml:space="preserve">typ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czas do złożenia się</t>
+  </si>
+  <si>
     <t xml:space="preserve">Waga</t>
   </si>
   <si>
     <t xml:space="preserve">Cena</t>
   </si>
   <si>
-    <t xml:space="preserve">czas do złożenia się</t>
-  </si>
-  <si>
     <t xml:space="preserve">ACOGx1,5</t>
   </si>
   <si>
     <t xml:space="preserve">siatka dyfrakcyjna, 2xtaniej, negowanie</t>
   </si>
   <si>
+    <t xml:space="preserve">półluneta</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACOGx3</t>
   </si>
   <si>
@@ -2244,7 +2250,7 @@
     <t xml:space="preserve">negowanie, Do Złącznienia</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4</t>
+    <t xml:space="preserve">luneta</t>
   </si>
   <si>
     <t xml:space="preserve">x6</t>
@@ -2280,7 +2286,7 @@
     <t xml:space="preserve">Pistolety</t>
   </si>
   <si>
-    <t xml:space="preserve">0.2</t>
+    <t xml:space="preserve">kolimator</t>
   </si>
   <si>
     <t xml:space="preserve">700$</t>
@@ -2292,9 +2298,6 @@
     <t xml:space="preserve">Magnificer</t>
   </si>
   <si>
-    <t xml:space="preserve">0.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">500$</t>
   </si>
   <si>
@@ -2350,6 +2353,9 @@
   </si>
   <si>
     <t xml:space="preserve">w nocy kara -4,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mechaniczne</t>
   </si>
   <si>
     <t xml:space="preserve">Fosforyzujące/ światłowodowe</t>
@@ -2820,7 +2826,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3021,10 +3027,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3113,10 +3115,10 @@
   <dimension ref="A1:P300"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I75" activeCellId="0" sqref="I75"/>
+      <selection pane="topLeft" activeCell="O72" activeCellId="0" sqref="O72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -16685,7 +16687,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -18017,7 +18019,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -18323,20 +18325,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>714</v>
       </c>
@@ -18352,19 +18354,22 @@
       <c r="E1" s="0" t="s">
         <v>718</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="0" t="s">
         <v>719</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="0" t="s">
         <v>720</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>721</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B2" s="48" t="n">
         <v>3</v>
@@ -18376,21 +18381,24 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="F2" s="2" t="n">
+        <v>724</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="G2" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="I2" s="2" t="n">
         <v>1300</v>
-      </c>
-      <c r="H2" s="49" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>3</v>
@@ -18402,21 +18410,24 @@
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="F3" s="2" t="n">
+        <v>724</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="G3" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="I3" s="2" t="n">
         <v>1600</v>
-      </c>
-      <c r="H3" s="49" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>3</v>
@@ -18428,21 +18439,24 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="F4" s="2" t="n">
+        <v>724</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="G4" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="I4" s="2" t="n">
         <v>1700</v>
-      </c>
-      <c r="H4" s="49" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>3</v>
@@ -18454,21 +18468,24 @@
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="F5" s="2" t="n">
+        <v>724</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="G5" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="I5" s="2" t="n">
         <v>2800</v>
-      </c>
-      <c r="H5" s="49" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
@@ -18480,21 +18497,24 @@
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="F6" s="2" t="n">
+        <v>724</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="G6" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="I6" s="2" t="n">
         <v>1000</v>
-      </c>
-      <c r="H6" s="49" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>3</v>
@@ -18506,21 +18526,24 @@
         <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="F7" s="2" t="n">
+        <v>724</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="G7" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="I7" s="2" t="n">
         <v>1500</v>
-      </c>
-      <c r="H7" s="49" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B8" s="48" t="n">
         <v>3</v>
@@ -18532,21 +18555,24 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G8" s="2" t="n">
+        <v>732</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="G8" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I8" s="2" t="n">
         <v>600</v>
-      </c>
-      <c r="H8" s="49" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>3</v>
@@ -18558,21 +18584,24 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G9" s="2" t="n">
+        <v>732</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="G9" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I9" s="2" t="n">
         <v>800</v>
-      </c>
-      <c r="H9" s="49" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>3</v>
@@ -18584,21 +18613,24 @@
         <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G10" s="2" t="n">
+        <v>732</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="G10" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I10" s="2" t="n">
         <v>900</v>
-      </c>
-      <c r="H10" s="49" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>3</v>
@@ -18610,21 +18642,24 @@
         <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G11" s="2" t="n">
+        <v>732</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="G11" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I11" s="2" t="n">
         <v>1000</v>
-      </c>
-      <c r="H11" s="49" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>3</v>
@@ -18636,21 +18671,24 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G12" s="2" t="n">
+        <v>732</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="G12" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I12" s="2" t="n">
         <v>1000</v>
-      </c>
-      <c r="H12" s="49" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>3</v>
@@ -18662,21 +18700,24 @@
         <v>400</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G13" s="2" t="n">
+        <v>732</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="G13" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I13" s="2" t="n">
         <v>1500</v>
-      </c>
-      <c r="H13" s="49" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>715</v>
@@ -18685,22 +18726,22 @@
         <v>716</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>739</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="G14" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="G14" s="49"/>
+      <c r="H14" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="H14" s="49"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B15" s="48" t="n">
         <v>3</v>
@@ -18712,21 +18753,24 @@
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>742</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="G15" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="H15" s="49" t="n">
+      <c r="F15" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G15" s="49" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>3</v>
@@ -18738,21 +18782,24 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="G16" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="H16" s="49" t="n">
+      <c r="F16" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G16" s="49" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H16" s="2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>3</v>
@@ -18764,21 +18811,24 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="H17" s="49" t="n">
+        <v>748</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G17" s="49" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H17" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>3</v>
@@ -18792,19 +18842,22 @@
       <c r="E18" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>752</v>
-      </c>
-      <c r="H18" s="49" t="n">
+      <c r="F18" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G18" s="49" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>3</v>
@@ -18816,21 +18869,24 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>754</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G19" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="H19" s="49" t="n">
+      <c r="F19" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G19" s="49" t="n">
         <v>1</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>3</v>
@@ -18842,21 +18898,24 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="F20" s="2" t="n">
+        <v>758</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G20" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2" t="n">
         <v>0.3</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="H20" s="49" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>3</v>
@@ -18868,21 +18927,24 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>759</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G21" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="H21" s="49" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>3</v>
@@ -18894,21 +18956,24 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G22" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G22" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="H22" s="49" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2</v>
@@ -18920,21 +18985,24 @@
         <v>2</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="G23" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="H23" s="49" t="n">
+      <c r="F23" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="G23" s="49" t="n">
         <v>1</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B24" s="48" t="n">
         <v>0</v>
@@ -18943,21 +19011,24 @@
         <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="F24" s="0" t="n">
+        <v>767</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="G24" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="49" t="n">
-        <v>2</v>
+      <c r="I24" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>0</v>
@@ -18966,19 +19037,22 @@
         <v>20</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="G25" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>699</v>
-      </c>
-      <c r="H25" s="49" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>1</v>
@@ -18987,21 +19061,24 @@
         <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>769</v>
-      </c>
-      <c r="F26" s="0" t="n">
+        <v>771</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="G26" s="49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="H26" s="49" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I26" s="2" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>15</v>
@@ -19010,23 +19087,20 @@
         <v>-5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>771</v>
-      </c>
-      <c r="F27" s="0" t="n">
+        <v>773</v>
+      </c>
+      <c r="H27" s="49"/>
+      <c r="I27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="J27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H27" s="49"/>
-    </row>
-    <row r="28" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="48" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="50"/>
+    </row>
+    <row r="32" customFormat="false" ht="312.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="48" t="s">
+        <v>774</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -19046,51 +19120,51 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
-        <v>770</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>773</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>774</v>
-      </c>
-      <c r="D1" s="51" t="s">
+      <c r="A1" s="50" t="s">
+        <v>772</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>775</v>
       </c>
+      <c r="C1" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>777</v>
+      </c>
       <c r="E1" s="0" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>718</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>60</v>
@@ -19116,7 +19190,7 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>90</v>
@@ -19142,7 +19216,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>80</v>
@@ -19168,7 +19242,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80</v>
@@ -19191,10 +19265,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>50</v>
@@ -19212,34 +19286,34 @@
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="s">
-        <v>784</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>773</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>774</v>
-      </c>
-      <c r="D7" s="51" t="s">
+      <c r="A7" s="50" t="s">
+        <v>786</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>775</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
+      <c r="C7" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>777</v>
+      </c>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
@@ -19262,10 +19336,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>20</v>
@@ -19288,10 +19362,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>787</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>785</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>20</v>
@@ -19313,17 +19387,17 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="51" t="s">
-        <v>788</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>773</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>774</v>
-      </c>
-      <c r="D11" s="51" t="s">
+      <c r="A11" s="50" t="s">
+        <v>790</v>
+      </c>
+      <c r="B11" s="50" t="s">
         <v>775</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19331,7 +19405,7 @@
         <v>171</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>75</v>
@@ -19357,7 +19431,7 @@
         <v>312</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>75</v>
@@ -19380,10 +19454,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>790</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>788</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>60</v>
@@ -19401,7 +19475,7 @@
         <v>65</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>300</v>
@@ -19412,7 +19486,7 @@
         <v>176</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>50</v>
@@ -19435,10 +19509,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>60</v>
@@ -19461,10 +19535,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>90</v>
@@ -19486,25 +19560,25 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="51" t="s">
-        <v>794</v>
-      </c>
-      <c r="B18" s="51" t="s">
-        <v>773</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>774</v>
-      </c>
-      <c r="D18" s="51" t="s">
+      <c r="A18" s="50" t="s">
+        <v>796</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>775</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
@@ -19530,7 +19604,7 @@
         <v>351</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
@@ -19553,10 +19627,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
@@ -19582,7 +19656,7 @@
         <v>332</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>20</v>
@@ -19608,7 +19682,7 @@
         <v>467</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
@@ -19634,7 +19708,7 @@
         <v>186</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>20</v>
@@ -19660,7 +19734,7 @@
         <v>440</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>20</v>
@@ -19686,7 +19760,7 @@
         <v>436</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>20</v>
@@ -19709,10 +19783,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>10</v>
@@ -19734,17 +19808,17 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="51" t="s">
-        <v>800</v>
-      </c>
-      <c r="B28" s="51" t="s">
-        <v>773</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>774</v>
-      </c>
-      <c r="D28" s="51" t="s">
+      <c r="A28" s="50" t="s">
+        <v>802</v>
+      </c>
+      <c r="B28" s="50" t="s">
         <v>775</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="D28" s="50" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19752,7 +19826,7 @@
         <v>414</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>15</v>
@@ -19778,7 +19852,7 @@
         <v>440</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
@@ -19801,10 +19875,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>10</v>
@@ -19830,7 +19904,7 @@
         <v>431</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>10</v>
@@ -19852,17 +19926,17 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="51" t="s">
-        <v>802</v>
-      </c>
-      <c r="B33" s="51" t="s">
-        <v>773</v>
-      </c>
-      <c r="C33" s="51" t="s">
-        <v>774</v>
-      </c>
-      <c r="D33" s="51" t="s">
+      <c r="A33" s="50" t="s">
+        <v>804</v>
+      </c>
+      <c r="B33" s="50" t="s">
         <v>775</v>
+      </c>
+      <c r="C33" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19870,7 +19944,7 @@
         <v>377</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>23</v>
@@ -19892,17 +19966,17 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="51" t="s">
-        <v>803</v>
-      </c>
-      <c r="B35" s="51" t="s">
-        <v>773</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>774</v>
-      </c>
-      <c r="D35" s="51" t="s">
+      <c r="A35" s="50" t="s">
+        <v>805</v>
+      </c>
+      <c r="B35" s="50" t="s">
         <v>775</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="D35" s="50" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19910,7 +19984,7 @@
         <v>149</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>75</v>
@@ -19936,7 +20010,7 @@
         <v>66</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>75</v>
@@ -19962,7 +20036,7 @@
         <v>465</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>16</v>
@@ -19985,10 +20059,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>10</v>
@@ -20002,10 +20076,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>20</v>
@@ -20022,7 +20096,7 @@
         <v>529</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>30</v>
@@ -20048,7 +20122,7 @@
         <v>209</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>30</v>
@@ -20066,7 +20140,7 @@
         <v>147</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>400</v>

</xml_diff>

<commit_message>
implementing,and getting data from SQL ready
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -3114,8 +3114,8 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
disasembly of addon added.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="805">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2455,13 +2455,16 @@
     <t xml:space="preserve">laser</t>
   </si>
   <si>
+    <t xml:space="preserve">świeci,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latarka</t>
+  </si>
+  <si>
     <t xml:space="preserve">świeci, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latarka</t>
   </si>
 </sst>
 </file>
@@ -3096,11 +3099,11 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -14686,7 +14689,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -16018,7 +16021,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -16330,7 +16333,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17111,7 +17114,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -18101,11 +18104,14 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -18225,7 +18231,7 @@
         <v>84</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0.2</v>

</xml_diff>

<commit_message>
Wprawa  has been fixed..
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="805">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2350,7 +2350,7 @@
     <t xml:space="preserve">'40 S&amp;W</t>
   </si>
   <si>
-    <t xml:space="preserve">pistoletowe</t>
+    <t xml:space="preserve">pistoletowa</t>
   </si>
   <si>
     <t xml:space="preserve">ACP'45</t>
@@ -2359,7 +2359,7 @@
     <t xml:space="preserve">wytłumiona</t>
   </si>
   <si>
-    <t xml:space="preserve">rewolwerowe</t>
+    <t xml:space="preserve">rewolwerowa</t>
   </si>
   <si>
     <t xml:space="preserve">AE'50</t>
@@ -2368,15 +2368,12 @@
     <t xml:space="preserve">Magnum '44</t>
   </si>
   <si>
-    <t xml:space="preserve">pośrednie</t>
+    <t xml:space="preserve">pośrednia</t>
   </si>
   <si>
     <t xml:space="preserve">‘300 AAC Blackout</t>
   </si>
   <si>
-    <t xml:space="preserve">Pośrednie</t>
-  </si>
-  <si>
     <t xml:space="preserve">zasieg skuteczny -100m, zasieg skuteczny &lt;500</t>
   </si>
   <si>
@@ -2389,10 +2386,13 @@
     <t xml:space="preserve">'303</t>
   </si>
   <si>
-    <t xml:space="preserve">karabinowe</t>
+    <t xml:space="preserve">karabinowa</t>
   </si>
   <si>
     <t xml:space="preserve">6,5 Creedmoor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wyborowa</t>
   </si>
   <si>
     <t xml:space="preserve">wyborowe</t>
@@ -3099,11 +3099,11 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D187" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L190" activeCellId="0" sqref="L190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -14689,7 +14689,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -16021,7 +16021,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -16333,7 +16333,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17108,13 +17108,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -17149,7 +17149,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>765</v>
       </c>
@@ -17175,7 +17175,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>117</v>
       </c>
@@ -17201,7 +17201,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -17227,7 +17227,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>93</v>
       </c>
@@ -17253,7 +17253,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>767</v>
       </c>
@@ -17282,7 +17282,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -17308,7 +17308,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>770</v>
       </c>
@@ -17334,7 +17334,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>771</v>
       </c>
@@ -17360,7 +17360,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>171</v>
       </c>
@@ -17386,7 +17386,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>312</v>
       </c>
@@ -17417,7 +17417,7 @@
         <v>773</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>60</v>
@@ -17435,7 +17435,7 @@
         <v>65</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>300</v>
@@ -17469,7 +17469,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>772</v>
@@ -17495,7 +17495,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>772</v>
@@ -17519,12 +17519,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>778</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>779</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>20</v>
@@ -17545,12 +17545,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>350</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>20</v>
@@ -17571,12 +17571,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>780</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>781</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>20</v>
@@ -17602,7 +17602,7 @@
         <v>331</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
@@ -17628,7 +17628,7 @@
         <v>465</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>20</v>
@@ -17654,7 +17654,7 @@
         <v>186</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
@@ -17706,7 +17706,7 @@
         <v>434</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>20</v>
@@ -17732,7 +17732,7 @@
         <v>782</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>10</v>
@@ -17758,7 +17758,7 @@
         <v>412</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>15</v>
@@ -17784,7 +17784,7 @@
         <v>438</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>10</v>
@@ -17805,12 +17805,12 @@
         <v>700</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>783</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>10</v>
@@ -17836,7 +17836,7 @@
         <v>429</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>10</v>
@@ -18084,6 +18084,11 @@
       </c>
       <c r="I36" s="0" t="n">
         <v>400</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="2" t="s">
+        <v>766</v>
       </c>
     </row>
   </sheetData>
@@ -18104,11 +18109,11 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
   </cols>

</xml_diff>

<commit_message>
added quite a lot of tests, and refactoring class Bron.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">$1 400,00</t>
   </si>
   <si>
-    <t xml:space="preserve">Glock 17 9mm</t>
+    <t xml:space="preserve">Glock 17</t>
   </si>
   <si>
     <t xml:space="preserve">Bezawaryjna, Glock, Nakładka, Pistolet</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">$600,00</t>
   </si>
   <si>
-    <t xml:space="preserve">Glock 19 9mm</t>
+    <t xml:space="preserve">Glock 19</t>
   </si>
   <si>
     <t xml:space="preserve">Glock, Mała, Pistolet</t>
@@ -3099,11 +3099,11 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D187" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L190" activeCellId="0" sqref="L190"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -14689,7 +14689,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -16021,7 +16021,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -16333,7 +16333,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17114,7 +17114,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -18109,11 +18109,11 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
   </cols>

</xml_diff>

<commit_message>
refactor, due to features in the future.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,10 @@
     <sheet name="celowniki" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="amunicja" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="dodatki" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Szpej" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="plyty_balistyczne" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Tarcze" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Apteczki" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -50,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="942">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2458,13 +2462,424 @@
     <t xml:space="preserve">świeci,</t>
   </si>
   <si>
-    <t xml:space="preserve">1$</t>
-  </si>
-  <si>
     <t xml:space="preserve">latarka</t>
   </si>
   <si>
     <t xml:space="preserve">świeci, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">200$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamizelki i kombinezony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zasady specjalne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Unik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemność</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zajmowane sloty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mnożnik ceny płyt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undershirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Łatwa do ukrycia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dedykowana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zintegrowana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1A, 4k, 2p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klata, Pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plate carrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wybitny plate carrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skarab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2 (L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pancerz szturmowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5 (XL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Przeciw wybuchom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Całość</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2(XXL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centurion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pancerz wspomagany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodatki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas PT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,6kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas PT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,4kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bandoliera na granaty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szelki taktyczne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szelki 2A  Undershirt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szelki na granaty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handler do Strzelby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Przyspiesza ładowanie nabojów do strzelby (2 krotnie).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 12’G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podwójny Handler do Strzelby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Przyspiesza ładowanie nabojów do strzelby (2 krotnie). Odejmij 1 od sprawności fizycznej.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 12’G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,8kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprzęt ochronny I specjalny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stopery do uszu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chronią słuch przed wszelkim hukiem (między innymi przed granatami hukowymi). -10 do spostrzegania, jeśli chodzi o rozpoznawanie dźwięku.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomijalna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aktywna ochrona słuchu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zwane również słuchawkami taktycznymi. Możesz je podpiąć do radia, aby słyszeć rozkazy z radia. Chronią słuch przed wszelkimi hukami (od broni, po granaty). -3 do wszystkich testów opartych na słuchu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,4 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maska przeciwgazowa MP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chroni przed wszelkimi toksycznymi gazami i oparami. Utrudnia oddychanie, oraz można celować tylko z kolimatorów na wysokim montażu (lub strzelać z biodra).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowoczesna maska przeciwgazowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chroni przed wszelkimi gazami bojowymi. uniemożliwia złożenie się do muszki i szczerbinki, (celowanie laserem, lunetą lub kolimatorem)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hełm stalowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redukuje obrażenia z odłamków (granaty itd.) o 3. W kontekście ochrony przed pociskami, nie ma większego sensu. Dodaj 1 do red, do penetracji minimalnej.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Głowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hełm kevlarowy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redukuje obrażenia z odłamków (granaty itd.) o 3. Opcjonalnie można założyć latarkę, oraz jest slot na noktowizor. Dodaj 1 do red, do penetracji średniej.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noktowizor 1 Generacji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia widzenie w nocy na pełny zasięg, z podświetleniem ludzkich sylwetek. Zabiera przeciwnikom premię z kamuflażu, oraz munduru. Oślepienie. Dodatkowo wszyscy inni posiadacze noktowizji bardzo wyraźnie Cię widzą. W zestawie po za samym noktowizorem masz lampę, która wszystko podświetla wszystkim w noktowizji, a Ty tylko te podświetlony rejon widzisz. Sama lampa jest bardzo duża. Ognisko, latarka lub laser całkowicie oślepia. Zasięg widzenia to 400m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noktowizor Generacji 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia widzenie w nocy na pełny zasięg, z podświetleniem ludzkich sylwetek. Zabiera przeciwnikom premię z kamuflażu, oraz munduru. Oślepienie Ognisko, latarka lub laser całkowicie oślepia. Zasięg widzenia to 400m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noktowizor (generacji 3+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia widzenie w nocy na pełny zasięg, z podświetleniem ludzkich sylwetek. Zabiera przeciwnikom premię z kamuflażu, oraz munduru. Latarka, lub laser zwrócony bezpośrednio w Twoją stronę całkowicie oślepia. Ognisko, czy inne źródło ognia w polu widzenia utrudnia (wymaga testu spostrzegania T5) rozpoznanie celu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ochraniacze łokci i kolan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w momencie gdy się czołgasz, dodaj premię +5 do testów poruszania się w ciężkim terenie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ochraniacze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ochraniacze rąk i nóg, z ochroną przed kulami lekkie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brak miejsca na kaburę udową, w cenie są rękawice szturmowe( broń do walki wręcz). Premia +1 do Uniku. Maksymalne bazowe uchylanie to 20. Nie można założyć, z kamizelką Pancerz i Saper.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ochraniacze rąk i nóg, z ochroną przed kulami ciężkie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brak miejsca na kaburę udową, W cenie są rękawice szturmowe. Premia +2 do Uniku. Maksymalne bazowe uchylanie to 15. Nie można założyć, z kamizelką Pancerz i Saper.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plecaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ilość slotów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koszt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zwykły Plecak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plecy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">średni plecak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duży plecak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marines assault pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabura</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pozwala na szybkie wyciągnięcie broni krótkiej, (możesz kupić również na 1 slot specjalny np. na radio, bagnet/nóż itd.). Zajmuje 1 slot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,2 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabura udowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pozwala na szybkie wyciągnięcie broni krótkiej, (możesz kupić również na 1 slot specjalny np. na radio, bagnet/nóż itd.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,3 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukryta kabura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabura którą możesz nosić pod ubraniem (ukryć swoją broń +5 do ukrywania)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas nośny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Możesz dzięki temu mieć wolne ręce a broń Ci wisi na boku i łatwo Ci ją szybko chwycić (1 faza). Dla broni o masie większej niż 7kg niedostępny. Zajmuje slot na plecach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas nośny dla broni ciężkiej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ten jest dla broni której masa jest większa niż 7Kg. Umożliwia wygodne (jak na taką kobyłę) przenoszenie broni. Możesz dzięki temu mieć wolne ręce a broń Ci wisi na boku i łatwo Ci ją szybko chwycić (1 faza). Zajmuje slot na plecach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wkłady</t>
+  </si>
+  <si>
+    <t xml:space="preserve">różne rozmiary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ochrona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wytrzymałość</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klasa 3 stalowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klasa 4 stalowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klasa 1 miękkie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimalna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klasa 2 miękkie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lekka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klasa 3 miękkie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wkładka Undershirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Płyty Centurion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miękka podkładka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zwiększa wytrzymałość o 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarcze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mod Unik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ochrona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policyjna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Militarna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Średni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciężka Militarna</t>
   </si>
 </sst>
 </file>
@@ -2815,7 +3230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3020,6 +3435,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3099,11 +3526,11 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -14678,6 +15105,29 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -14689,7 +15139,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -16021,7 +16471,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -16333,7 +16783,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -17114,7 +17564,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -18110,10 +18560,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
   </cols>
@@ -18219,12 +18669,12 @@
         <v>0.2</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>642</v>
@@ -18236,13 +18686,13 @@
         <v>84</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
   </sheetData>
@@ -18254,4 +18704,1109 @@
     <oddFooter>&amp;CStrona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I40"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="48" t="s">
+        <v>805</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="51" t="s">
+        <v>843</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>794</v>
+      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="H10" s="52" t="s">
+        <v>714</v>
+      </c>
+      <c r="I10" s="52" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="52" t="s">
+        <v>844</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>845</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>846</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>820</v>
+      </c>
+      <c r="H11" s="52" t="s">
+        <v>847</v>
+      </c>
+      <c r="I11" s="52" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="52" t="s">
+        <v>848</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="E12" s="53" t="s">
+        <v>846</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>849</v>
+      </c>
+      <c r="H12" s="52" t="s">
+        <v>850</v>
+      </c>
+      <c r="I12" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="52" t="s">
+        <v>851</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="E13" s="53" t="s">
+        <v>852</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>849</v>
+      </c>
+      <c r="H13" s="52" t="s">
+        <v>850</v>
+      </c>
+      <c r="I13" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="52" t="s">
+        <v>853</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>854</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>855</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>815</v>
+      </c>
+      <c r="H14" s="52" t="s">
+        <v>856</v>
+      </c>
+      <c r="I14" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="52" t="s">
+        <v>857</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>854</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>858</v>
+      </c>
+      <c r="F15" s="53" t="s">
+        <v>815</v>
+      </c>
+      <c r="H15" s="52" t="s">
+        <v>856</v>
+      </c>
+      <c r="I15" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="52" t="s">
+        <v>859</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>860</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>861</v>
+      </c>
+      <c r="F16" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="52" t="s">
+        <v>850</v>
+      </c>
+      <c r="I16" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="52" t="s">
+        <v>862</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>863</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>864</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="52" t="s">
+        <v>865</v>
+      </c>
+      <c r="I17" s="52" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="51" t="s">
+        <v>866</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>794</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>714</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="52" t="s">
+        <v>867</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>868</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>869</v>
+      </c>
+      <c r="I19" s="52" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="52" t="s">
+        <v>870</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="H20" s="52" t="s">
+        <v>872</v>
+      </c>
+      <c r="I20" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="52" t="s">
+        <v>873</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>874</v>
+      </c>
+      <c r="H21" s="52" t="s">
+        <v>875</v>
+      </c>
+      <c r="I21" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="52" t="s">
+        <v>876</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>877</v>
+      </c>
+      <c r="H22" s="52" t="s">
+        <v>827</v>
+      </c>
+      <c r="I22" s="52" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="52" t="s">
+        <v>878</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>879</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>880</v>
+      </c>
+      <c r="H23" s="52" t="s">
+        <v>822</v>
+      </c>
+      <c r="I23" s="52" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="52" t="s">
+        <v>881</v>
+      </c>
+      <c r="B24" s="52" t="s">
+        <v>882</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>880</v>
+      </c>
+      <c r="H24" s="52" t="s">
+        <v>822</v>
+      </c>
+      <c r="I24" s="52" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="52" t="s">
+        <v>883</v>
+      </c>
+      <c r="B25" s="52" t="s">
+        <v>884</v>
+      </c>
+      <c r="H25" s="52" t="s">
+        <v>834</v>
+      </c>
+      <c r="I25" s="52" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="52" t="s">
+        <v>885</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>886</v>
+      </c>
+      <c r="H26" s="52" t="s">
+        <v>822</v>
+      </c>
+      <c r="I26" s="52" t="n">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="52" t="s">
+        <v>887</v>
+      </c>
+      <c r="B27" s="52" t="s">
+        <v>888</v>
+      </c>
+      <c r="H27" s="52" t="s">
+        <v>817</v>
+      </c>
+      <c r="I27" s="52" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="52" t="s">
+        <v>889</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>890</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>891</v>
+      </c>
+      <c r="H28" s="52" t="s">
+        <v>817</v>
+      </c>
+      <c r="I28" s="52" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="52" t="s">
+        <v>892</v>
+      </c>
+      <c r="B29" s="52" t="s">
+        <v>893</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>891</v>
+      </c>
+      <c r="H29" s="52" t="s">
+        <v>822</v>
+      </c>
+      <c r="I29" s="52" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="52" t="s">
+        <v>894</v>
+      </c>
+      <c r="B30" s="52" t="s">
+        <v>895</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>891</v>
+      </c>
+      <c r="H30" s="52" t="s">
+        <v>834</v>
+      </c>
+      <c r="I30" s="52" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="48" t="s">
+        <v>896</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>901</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>901</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>901</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>901</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="51" t="s">
+        <v>906</v>
+      </c>
+      <c r="B36" s="52" t="s">
+        <v>907</v>
+      </c>
+      <c r="H36" s="52" t="s">
+        <v>908</v>
+      </c>
+      <c r="I36" s="52" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="52" t="s">
+        <v>909</v>
+      </c>
+      <c r="B37" s="52" t="s">
+        <v>910</v>
+      </c>
+      <c r="H37" s="52" t="s">
+        <v>911</v>
+      </c>
+      <c r="I37" s="52" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="52" t="s">
+        <v>912</v>
+      </c>
+      <c r="B38" s="52" t="s">
+        <v>913</v>
+      </c>
+      <c r="H38" s="52" t="s">
+        <v>911</v>
+      </c>
+      <c r="I38" s="52" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="52" t="s">
+        <v>914</v>
+      </c>
+      <c r="B39" s="52" t="s">
+        <v>915</v>
+      </c>
+      <c r="H39" s="52" t="s">
+        <v>916</v>
+      </c>
+      <c r="I39" s="52" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="52" t="s">
+        <v>917</v>
+      </c>
+      <c r="B40" s="52" t="s">
+        <v>918</v>
+      </c>
+      <c r="H40" s="52" t="s">
+        <v>908</v>
+      </c>
+      <c r="I40" s="52" t="n">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="48" t="s">
+        <v>919</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>933</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="48" t="s">
+        <v>934</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>-10</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>-15</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
prepared data, for futher development.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,10 +14,15 @@
     <sheet name="celowniki" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="amunicja" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="dodatki" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Szpej" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="szpej" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="plyty_balistyczne" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Tarcze" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Apteczki" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="tarcze" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="apteczki" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="radia_i_komunikacja" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="jedzenie" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="zestawy_dajace_premie" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="drobnica" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="gotowe_zestawy" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -54,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="1118">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2471,13 +2476,10 @@
     <t xml:space="preserve">200$</t>
   </si>
   <si>
-    <t xml:space="preserve">Kamizelki i kombinezony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zasady specjalne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max Unik</t>
+    <t xml:space="preserve">szpej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max_Unik</t>
   </si>
   <si>
     <t xml:space="preserve">Red</t>
@@ -2486,10 +2488,10 @@
     <t xml:space="preserve">Pojemność</t>
   </si>
   <si>
-    <t xml:space="preserve">zajmowane sloty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mnożnik ceny płyt</t>
+    <t xml:space="preserve">zajmowane_sloty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mnożnik_ceny_płyt</t>
   </si>
   <si>
     <t xml:space="preserve">Undershirt</t>
@@ -2816,7 +2818,7 @@
     <t xml:space="preserve">Wkłady</t>
   </si>
   <si>
-    <t xml:space="preserve">różne rozmiary</t>
+    <t xml:space="preserve">różne_rozmiary</t>
   </si>
   <si>
     <t xml:space="preserve">Ochrona</t>
@@ -2861,7 +2863,7 @@
     <t xml:space="preserve">Tarcze</t>
   </si>
   <si>
-    <t xml:space="preserve">Mod Unik</t>
+    <t xml:space="preserve">Mod_Unik</t>
   </si>
   <si>
     <t xml:space="preserve">ochrona</t>
@@ -2880,15 +2882,547 @@
   </si>
   <si>
     <t xml:space="preserve">Ciężka Militarna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apteczka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zajmowane_miejsce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilość_ładunków</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prosta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quikclot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 sztuka zmieści się w apteczce.(umożliwia zaleczenie rany lekkiej, poważnej, lub kończyny w 5 minut, bez testu).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apteczka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taktyczna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adrenalina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zastosowanie podnosi z out of action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samochodowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prawie w każdym samochodzie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plecak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krem z filtrem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chroni przed ostrym słońcem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pomijalne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leki przeciwbólowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redukuje kary z chorób o 1, oraz z ran o 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antybiotyk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia wyleczenie z chorób bakteryjnych, w czasie 2krotnie krótszym.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operatorska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mieści się w slocie „a” kamizelki. Skorzystanie wymaga 3 rang w Dyscyplinie Naukowej Medycyna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morfina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na 2 godziny redukuje kary z ran do 0 (nie same rany, ale tylko kary do testów z nich wynikające). Skorzystanie wymaga 2 rang w Dyscyplinie Naukowej Medycyna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szyfrowanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zasięg_przechwycenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Słabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taktyczne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Średnie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odporne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profesjonalne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zawansowane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operejtorskie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptopy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bonus do testów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odporny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profesjonalny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operejtorski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jedzenie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">higiena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sloty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">racja MRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Racja całodzienna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">przybory do mycia na cały tydzień</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camelbag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manierka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2L wody butelkowanej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waga_i_miejsce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw narzędzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia wykonanie napraw większości sprzętu (bez lutowania). Za każde 200$ dodaj premię +1, oraz dodatkowy kilogram masy, a za każde dodatkowe 4 kilogramy dodaj slot zajmowany. Maksymalna premia +10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (3kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200$-2000$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw Konserwujący do broni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia wykonanie drobnych napraw, i przygotowanie broni aby była w pełnej gotowości, nawet po kompletnym upapraniu jej.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (1kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprzęt do nurkowania z butlą.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia przetrwanie pod wodą do 1 godziny.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (8kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw wspinaczkowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umożliwia bezproblemową wspinaczkę, jak i po budynku, jak i w góry. Zapewnia premię +5 do wszystkich testów podczas wspinaczki.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (5kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw biwakowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zawiera śpiwór, menaszki, i wszystko czego potrzebujesz aby rozpalić ogień, i zrobić na nim żarcie, jeśli jakieś upolujesz, (pamiętaj nie masz tego wiele). Za każde 200$ dodaj premię +1 do przyrządzania jedzenia oraz rozbijanie obozu, oraz dodatkowy kilogram masy, a za każde dodatkowe 4 kilogramy dodaj slot zajmowany. Maksymalna premia +10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (6kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Użytkowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">objętość</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flaszka wódki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5L (0,5 slotu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flaszka wódki lepsza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">butelka wina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">butelka lepszego wina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stek świeżo usmażony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,4 slotu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chleb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">karty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomijalne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paczka Papierosów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zapalniczka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,05kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1L (1 slot)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piersiówka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slot A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brzytwa do golenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,05 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kondomy (10 pak)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,01kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szpadel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaczep plecaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okulary przeciwsłoneczne (cena rośnie wraz ze szpanem)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-300$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survivalove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menażka (Zestaw Garnek + kubek + sztućce)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 sloty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nieśmiertelnik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,01 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ręcznik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes + długopis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ładowarka słoneczna (ładuje urządzenia elektryczne, lub zasila laptopa przy dobrym słońcu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerBank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1slot K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparat analogowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 slot A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,7 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kajdanki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 slot k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lina/sznur (10m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lina/sznur (5m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slot A kamizelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moskitiera dla 1 osoby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Składana wędka i osprzęt wędkarski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lornetka(+3D6 do spostrzegania w oddali)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camelbag (2L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Śpiwór taktyczny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namiot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 slotów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saperka (po naostrzeniu toporek z karą -1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 slot,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gotowe_zestawy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw biwakowy + Namiot 3 osobowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw biwakowy plus namiot z moskitierą. Ciężki w cholerę, ale podczas deszczu chwalisz Pana iż się zdecydowałeś.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (10kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw biwakowy + Namiot 5 osobowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrz wyżej plus ciężej ale wygodniej. Zajmuje w cholerę miejsca, i nie mieści się w zwykłym plecaku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 (15kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw podróżnika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plecak duży, 4L wody w butelkach, manierka, 2 racje MRE, bagnet/nóż, zestaw biwakowy. Przybory do mycia na tydzień. Powerbank, notes i długopis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">485$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw podróżnika większego zasięgu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Średni plecak wojskowy. 6L wody w butelkach, cammelbag, 10 racji MRE, mundur na przebranie, bagnet/nóż, zestaw biwakowy, kajdanki, zestaw konserwujący do broni. Ładowarka solarna. Przybory do mycia na 2 tygodnie. Notes i długopis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1487$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zestaw obieżyświata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marines assault pack. 10L wody, 10 racji całodziennych, cammelbag, bagnet/nóż, zestaw biwakowy + namiot 3 osobowy., Lina (10m),Mundur na przebranie, Zestaw konserwujący do broni, powerbank, ładowarka solarna, przybory do mycia na 3 tygodnie. Notes i długopis. Pamiętaj o możliwości zrzutu całości w fazę.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2040$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -3230,7 +3764,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3447,6 +3981,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3526,7 +4064,7 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H226" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -15110,14 +15648,1671 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
+        <v>941</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>794</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>942</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>943</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>944</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>715</v>
+      </c>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="52" t="s">
+        <v>945</v>
+      </c>
+      <c r="B2" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="52" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>692</v>
+      </c>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>947</v>
+      </c>
+      <c r="B3" s="53"/>
+      <c r="C3" s="52" t="s">
+        <v>948</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>949</v>
+      </c>
+      <c r="E3" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>907</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>950</v>
+      </c>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>951</v>
+      </c>
+      <c r="B4" s="52" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>855</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>952</v>
+      </c>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>953</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52" t="s">
+        <v>954</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>949</v>
+      </c>
+      <c r="E5" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>915</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>952</v>
+      </c>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="52" t="s">
+        <v>955</v>
+      </c>
+      <c r="B6" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>956</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>957</v>
+      </c>
+      <c r="E6" s="52" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>816</v>
+      </c>
+      <c r="G6" s="52" t="s">
+        <v>958</v>
+      </c>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="52" t="s">
+        <v>959</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>960</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>961</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>962</v>
+      </c>
+      <c r="E7" s="52" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>910</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>952</v>
+      </c>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>960</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>962</v>
+      </c>
+      <c r="E8" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>907</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>965</v>
+      </c>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="52" t="s">
+        <v>966</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>960</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>967</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>962</v>
+      </c>
+      <c r="E9" s="52" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>915</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>692</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="52" t="s">
+        <v>968</v>
+      </c>
+      <c r="B10" s="52" t="n">
+        <v>15</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>969</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>698</v>
+      </c>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="52" t="s">
+        <v>970</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>960</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>971</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>949</v>
+      </c>
+      <c r="E11" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>910</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>685</v>
+      </c>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="53"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="48" t="s">
+        <v>972</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="G7" s="54" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>998</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="G9" s="54" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>998</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>992</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="51" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="51" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C5" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="52" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C6" s="52" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="52" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C7" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>794</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="52" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="52" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>804</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="52" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>855</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>855</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>855</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>855</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="52" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="52" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>915</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="52" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="52" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="52" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="52" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>910</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="52" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="52" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="52" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="52" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="51" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>714</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="52" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="52" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="52" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="52" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="52" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="52" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B24" s="52" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>910</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="52" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B25" s="52" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="52" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="52" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B27" s="52" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="52" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="52" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B29" s="52" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="52" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B30" s="52" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C30" s="52" t="s">
+        <v>910</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="52" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B31" s="52" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C31" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D31" s="52" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="52" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B32" s="52" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C32" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="52" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C33" s="52" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="52" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B34" s="52" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C34" s="52" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="52" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C35" s="52" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="52" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B36" s="52" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C36" s="52" t="s">
+        <v>826</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="52" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B37" s="52" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C37" s="52" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>944</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="52" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="52" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="53"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="53"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -15135,7 +17330,7 @@
   </sheetPr>
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -16467,7 +18662,7 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -16779,7 +18974,7 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -17560,8 +19755,8 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18713,8 +20908,8 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18727,22 +20922,22 @@
         <v>805</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>806</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>807</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>808</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>809</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>810</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>811</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>795</v>
@@ -18753,10 +20948,10 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>812</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>813</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>20</v>
@@ -18765,16 +20960,16 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>814</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>815</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>816</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>817</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>2000</v>
@@ -18782,7 +20977,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="n">
@@ -18792,16 +20987,16 @@
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>819</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>820</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>821</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>822</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>300</v>
@@ -18809,7 +21004,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="n">
@@ -18819,16 +21014,16 @@
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>814</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>824</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>815</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>825</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>500</v>
@@ -18836,7 +21031,7 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="n">
@@ -18846,16 +21041,16 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>1000</v>
@@ -18863,7 +21058,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="n">
@@ -18873,16 +21068,16 @@
         <v>6</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>829</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>820</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>830</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>600</v>
@@ -18890,7 +21085,7 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="n">
@@ -18900,16 +21095,16 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>832</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>820</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>833</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>834</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>5000</v>
@@ -18917,10 +21112,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>835</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>836</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>8</v>
@@ -18929,16 +21124,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>837</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>838</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>839</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>10000</v>
@@ -18946,10 +21141,10 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>840</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>841</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>15</v>
@@ -18958,16 +21153,16 @@
         <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>1000000</v>
@@ -18975,7 +21170,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B10" s="52" t="s">
         <v>794</v>
@@ -18991,19 +21186,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>843</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>844</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="E11" s="52" t="s">
         <v>845</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="F11" s="53" t="s">
+        <v>819</v>
+      </c>
+      <c r="H11" s="52" t="s">
         <v>846</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>820</v>
-      </c>
-      <c r="H11" s="52" t="s">
-        <v>847</v>
       </c>
       <c r="I11" s="52" t="n">
         <v>200</v>
@@ -19011,17 +21206,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B12" s="52"/>
       <c r="E12" s="53" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F12" s="53" t="s">
+        <v>848</v>
+      </c>
+      <c r="H12" s="52" t="s">
         <v>849</v>
-      </c>
-      <c r="H12" s="52" t="s">
-        <v>850</v>
       </c>
       <c r="I12" s="52" t="n">
         <v>100</v>
@@ -19029,17 +21224,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B13" s="52"/>
       <c r="E13" s="53" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F13" s="53" t="s">
+        <v>848</v>
+      </c>
+      <c r="H13" s="52" t="s">
         <v>849</v>
-      </c>
-      <c r="H13" s="52" t="s">
-        <v>850</v>
       </c>
       <c r="I13" s="52" t="n">
         <v>100</v>
@@ -19047,19 +21242,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
+        <v>852</v>
+      </c>
+      <c r="B14" s="52" t="s">
         <v>853</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="E14" s="53" t="s">
         <v>854</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="F14" s="53" t="s">
+        <v>814</v>
+      </c>
+      <c r="H14" s="52" t="s">
         <v>855</v>
-      </c>
-      <c r="F14" s="53" t="s">
-        <v>815</v>
-      </c>
-      <c r="H14" s="52" t="s">
-        <v>856</v>
       </c>
       <c r="I14" s="52" t="n">
         <v>100</v>
@@ -19067,19 +21262,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
+        <v>856</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>853</v>
+      </c>
+      <c r="E15" s="53" t="s">
         <v>857</v>
       </c>
-      <c r="B15" s="52" t="s">
-        <v>854</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>858</v>
-      </c>
       <c r="F15" s="53" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="H15" s="52" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I15" s="52" t="n">
         <v>100</v>
@@ -19087,19 +21282,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
+        <v>858</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>859</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="E16" s="53" t="s">
         <v>860</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>861</v>
       </c>
       <c r="F16" s="53" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="52" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="I16" s="52" t="n">
         <v>100</v>
@@ -19107,19 +21302,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
+        <v>861</v>
+      </c>
+      <c r="B17" s="52" t="s">
         <v>862</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="E17" s="53" t="s">
         <v>863</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>864</v>
       </c>
       <c r="F17" s="53" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I17" s="52" t="n">
         <v>200</v>
@@ -19127,7 +21322,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>794</v>
@@ -19141,13 +21336,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
+        <v>866</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>867</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="H19" s="52" t="s">
         <v>868</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>869</v>
       </c>
       <c r="I19" s="52" t="n">
         <v>20</v>
@@ -19155,13 +21350,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
+        <v>869</v>
+      </c>
+      <c r="B20" s="52" t="s">
         <v>870</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="H20" s="52" t="s">
         <v>871</v>
-      </c>
-      <c r="H20" s="52" t="s">
-        <v>872</v>
       </c>
       <c r="I20" s="52" t="n">
         <v>100</v>
@@ -19169,13 +21364,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
+        <v>872</v>
+      </c>
+      <c r="B21" s="52" t="s">
         <v>873</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="H21" s="52" t="s">
         <v>874</v>
-      </c>
-      <c r="H21" s="52" t="s">
-        <v>875</v>
       </c>
       <c r="I21" s="52" t="n">
         <v>100</v>
@@ -19183,13 +21378,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
+        <v>875</v>
+      </c>
+      <c r="B22" s="52" t="s">
         <v>876</v>
       </c>
-      <c r="B22" s="52" t="s">
-        <v>877</v>
-      </c>
       <c r="H22" s="52" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I22" s="52" t="n">
         <v>500</v>
@@ -19197,16 +21392,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
+        <v>877</v>
+      </c>
+      <c r="B23" s="52" t="s">
         <v>878</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="F23" s="0" t="s">
         <v>879</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>880</v>
-      </c>
       <c r="H23" s="52" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I23" s="52" t="n">
         <v>100</v>
@@ -19214,16 +21409,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>880</v>
+      </c>
+      <c r="B24" s="52" t="s">
         <v>881</v>
       </c>
-      <c r="B24" s="52" t="s">
-        <v>882</v>
-      </c>
       <c r="F24" s="0" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H24" s="52" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I24" s="52" t="n">
         <v>500</v>
@@ -19231,13 +21426,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
+        <v>882</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>883</v>
       </c>
-      <c r="B25" s="52" t="s">
-        <v>884</v>
-      </c>
       <c r="H25" s="52" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="I25" s="52" t="n">
         <v>1000</v>
@@ -19245,13 +21440,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
+        <v>884</v>
+      </c>
+      <c r="B26" s="52" t="s">
         <v>885</v>
       </c>
-      <c r="B26" s="52" t="s">
-        <v>886</v>
-      </c>
       <c r="H26" s="52" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I26" s="52" t="n">
         <v>4500</v>
@@ -19259,13 +21454,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
+        <v>886</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>887</v>
       </c>
-      <c r="B27" s="52" t="s">
-        <v>888</v>
-      </c>
       <c r="H27" s="52" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I27" s="52" t="n">
         <v>7500</v>
@@ -19273,16 +21468,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
+        <v>888</v>
+      </c>
+      <c r="B28" s="52" t="s">
         <v>889</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="F28" s="0" t="s">
         <v>890</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>891</v>
-      </c>
       <c r="H28" s="52" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I28" s="52" t="n">
         <v>200</v>
@@ -19290,16 +21485,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>891</v>
+      </c>
+      <c r="B29" s="52" t="s">
         <v>892</v>
       </c>
-      <c r="B29" s="52" t="s">
-        <v>893</v>
-      </c>
       <c r="F29" s="0" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="H29" s="52" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I29" s="52" t="n">
         <v>2000</v>
@@ -19307,16 +21502,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
+        <v>893</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>894</v>
       </c>
-      <c r="B30" s="52" t="s">
-        <v>895</v>
-      </c>
       <c r="F30" s="0" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="H30" s="52" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="I30" s="52" t="n">
         <v>5000</v>
@@ -19324,30 +21519,30 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="48" t="s">
+        <v>895</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>897</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>898</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>20</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I32" s="2" t="n">
         <v>50</v>
@@ -19355,16 +21550,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>35</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="I33" s="2" t="n">
         <v>100</v>
@@ -19372,16 +21567,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>40</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I34" s="2" t="n">
         <v>250</v>
@@ -19389,16 +21584,16 @@
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>60</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I35" s="2" t="n">
         <v>500</v>
@@ -19406,13 +21601,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="51" t="s">
+        <v>905</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>906</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="H36" s="52" t="s">
         <v>907</v>
-      </c>
-      <c r="H36" s="52" t="s">
-        <v>908</v>
       </c>
       <c r="I36" s="52" t="n">
         <v>20</v>
@@ -19420,13 +21615,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
+        <v>908</v>
+      </c>
+      <c r="B37" s="52" t="s">
         <v>909</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="H37" s="52" t="s">
         <v>910</v>
-      </c>
-      <c r="H37" s="52" t="s">
-        <v>911</v>
       </c>
       <c r="I37" s="52" t="n">
         <v>40</v>
@@ -19434,13 +21629,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="52" t="s">
+        <v>911</v>
+      </c>
+      <c r="B38" s="52" t="s">
         <v>912</v>
       </c>
-      <c r="B38" s="52" t="s">
-        <v>913</v>
-      </c>
       <c r="H38" s="52" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="I38" s="52" t="n">
         <v>50</v>
@@ -19448,13 +21643,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="52" t="s">
+        <v>913</v>
+      </c>
+      <c r="B39" s="52" t="s">
         <v>914</v>
       </c>
-      <c r="B39" s="52" t="s">
+      <c r="H39" s="52" t="s">
         <v>915</v>
-      </c>
-      <c r="H39" s="52" t="s">
-        <v>916</v>
       </c>
       <c r="I39" s="52" t="n">
         <v>20</v>
@@ -19462,13 +21657,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="52" t="s">
+        <v>916</v>
+      </c>
+      <c r="B40" s="52" t="s">
         <v>917</v>
       </c>
-      <c r="B40" s="52" t="s">
-        <v>918</v>
-      </c>
       <c r="H40" s="52" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="I40" s="52" t="n">
         <v>40</v>
@@ -19493,23 +21688,23 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>918</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>919</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>920</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>921</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>922</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>794</v>
@@ -19523,7 +21718,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>218</v>
@@ -19543,7 +21738,7 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>218</v>
@@ -19563,13 +21758,13 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>5</v>
@@ -19583,13 +21778,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>5</v>
@@ -19603,7 +21798,7 @@
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>218</v>
@@ -19623,13 +21818,13 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>10</v>
@@ -19643,7 +21838,7 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
@@ -19663,19 +21858,19 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.2</v>
@@ -19703,26 +21898,26 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>933</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>934</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>935</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>936</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>807</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>937</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>714</v>
@@ -19733,13 +21928,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>13</v>
@@ -19756,13 +21951,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>12</v>
@@ -19779,7 +21974,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
preparing for vests, and equipment
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3276" uniqueCount="1118">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -4068,7 +4068,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15654,9 +15654,9 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16069,7 +16069,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
   </cols>
@@ -16348,7 +16348,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -16486,7 +16486,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
   </cols>
@@ -16597,7 +16597,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -17135,11 +17135,11 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
   </cols>
@@ -17334,7 +17334,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -18666,7 +18666,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -18978,7 +18978,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -19759,7 +19759,7 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -20758,7 +20758,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
   </cols>
@@ -20908,11 +20908,11 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
   </cols>
@@ -21174,6 +21174,9 @@
       </c>
       <c r="B10" s="52" t="s">
         <v>794</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>806</v>
       </c>
       <c r="E10" s="53"/>
       <c r="F10" s="53"/>
@@ -21691,7 +21694,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
@@ -21901,7 +21904,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">

</xml_diff>

<commit_message>
prepared uniforms, to be read.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,6 +23,7 @@
     <sheet name="zestawy_dajace_premie" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="drobnica" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="gotowe_zestawy" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="mundury" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3276" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3321" uniqueCount="1141">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2515,7 +2516,7 @@
     <t xml:space="preserve">Zintegrowana</t>
   </si>
   <si>
-    <t xml:space="preserve">1A, 4k, 2p</t>
+    <t xml:space="preserve">4k, 2p, 1A</t>
   </si>
   <si>
     <t xml:space="preserve">Klata, Pas</t>
@@ -2569,7 +2570,7 @@
     <t xml:space="preserve">Przeciw wybuchom</t>
   </si>
   <si>
-    <t xml:space="preserve">Całość</t>
+    <t xml:space="preserve">Klata, Pas, Nogi, Ochraniacze, głowa</t>
   </si>
   <si>
     <t xml:space="preserve">2(XXL)</t>
@@ -2707,6 +2708,9 @@
     <t xml:space="preserve">Redukuje obrażenia z odłamków (granaty itd.) o 3. Opcjonalnie można założyć latarkę, oraz jest slot na noktowizor. Dodaj 1 do red, do penetracji średniej.</t>
   </si>
   <si>
+    <t xml:space="preserve">Noktowizor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Noktowizor 1 Generacji</t>
   </si>
   <si>
@@ -2797,7 +2801,7 @@
     <t xml:space="preserve">Ukryta kabura</t>
   </si>
   <si>
-    <t xml:space="preserve">Kabura którą możesz nosić pod ubraniem (ukryć swoją broń +5 do ukrywania)</t>
+    <t xml:space="preserve">Kabura którą możesz nosić pod ubraniem (ukryć swoją broń +5 do ukrywania), ale nie jest najwygodniejsza, oraz dobycie jej jest trudne</t>
   </si>
   <si>
     <t xml:space="preserve">pas nośny</t>
@@ -3413,6 +3417,73 @@
   </si>
   <si>
     <t xml:space="preserve">2040$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ubranie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kamuflaze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tania podróba munduru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leśny, miejski, zimowy, pustynny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tani- po każdym brawurowym ruchu (np. przebijanie się przez krzak) rzuć D6. na 1 się rozrywa i przestaje dawać premię do Uniku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zimnowojenny z demobilu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">niepalny, wytrzymały, kamuflaż</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kontraktowy/ profesjonalny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leśny, miejski, zimowy, pustynny,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pałatka wojskowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciepły, wytrzymały, uniemożliwia szybkie wyciągnięcie przedmiotu z kamizelki (wydłuż czas wszystkich operacji związanych z kamizelką, np. przeładowanie o 2 fazy), Chroni przed deszczem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zwykłe ubranie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wybierz coś sobie popatrz w szafę, np. jeansy z koszulą, lub bluzą i podkoszulkiem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wyglądasz normalnie, cenę weź z prawdziwego świata.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garnitur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czarny, szary, granatowy, biały</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poważny wygląd. Za każdym razem kiedy prowadzisz poważny biznes, i zasiadacie do negocjacji w gabinecie, otrzymujesz premię D6 do Gadany.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gihlie suit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leśny, krzun pustynny,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeśli jesteś za osłoną naturalną (krzakiem), lub leżysz w wysokiej trawie, krzaku etc, i pozostajesz nieruchomy, to zwiększ premię do Uniku z 3 do 6.
+Wyglądasz jak krzak. Jeśli ukrywasz się, masz dodatkowe 3d6 jeśli jesteś w krzaku. Najpierw musisz zdradzić swoja pozycję aby wróg Cię zauważył. Współpracuje jedynie z kamizelką Undershirt, pasami, i szelkami. Wydłuż czasy przeładowania 2-krotnie, chyba że przygotowałeś wcześniej magazynek, i leży on przed tobą.</t>
   </si>
 </sst>
 </file>
@@ -4068,7 +4139,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15654,14 +15725,14 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>3</v>
@@ -15670,13 +15741,13 @@
         <v>794</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>715</v>
@@ -15686,7 +15757,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>5</v>
@@ -15699,7 +15770,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>692</v>
@@ -15709,30 +15780,30 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="52" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="E3" s="52" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>10</v>
@@ -15748,46 +15819,46 @@
         <v>855</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="52" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="E5" s="52" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="E6" s="52" t="n">
         <v>10</v>
@@ -15796,79 +15867,79 @@
         <v>816</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="E7" s="52" t="n">
         <v>50</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>961</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>965</v>
+      </c>
+      <c r="D8" s="52" t="s">
         <v>963</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>960</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>964</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>962</v>
       </c>
       <c r="E8" s="52" t="n">
         <v>5</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="E9" s="52" t="n">
         <v>3</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="G9" s="52" t="s">
         <v>692</v>
@@ -15878,13 +15949,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>18</v>
@@ -15893,7 +15964,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>698</v>
@@ -15903,22 +15974,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="E11" s="52" t="n">
         <v>5</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>685</v>
@@ -16069,26 +16140,26 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>638</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>794</v>
@@ -16105,22 +16176,22 @@
         <v>750</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>685</v>
@@ -16128,97 +16199,97 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>794</v>
@@ -16232,20 +16303,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>2</v>
@@ -16256,74 +16327,74 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>997</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>996</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>1000</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
   </sheetData>
@@ -16348,23 +16419,23 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>643</v>
@@ -16372,7 +16443,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.5</v>
@@ -16387,12 +16458,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -16404,12 +16475,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="0" t="n">
@@ -16419,12 +16490,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C5" s="52" t="n">
         <v>1</v>
@@ -16433,12 +16504,12 @@
         <v>2</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C6" s="52" t="n">
         <v>0.5</v>
@@ -16447,12 +16518,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C7" s="52" t="n">
         <v>1</v>
@@ -16461,7 +16532,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
     </row>
   </sheetData>
@@ -16486,20 +16557,20 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>715</v>
@@ -16507,27 +16578,27 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="D3" s="52" t="s">
         <v>804</v>
@@ -16535,41 +16606,41 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="D6" s="52" t="s">
         <v>804</v>
@@ -16597,14 +16668,14 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>714</v>
@@ -16615,38 +16686,38 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>855</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>855</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>855</v>
@@ -16657,10 +16728,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>855</v>
@@ -16671,10 +16742,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>871</v>
@@ -16685,13 +16756,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>706</v>
@@ -16699,13 +16770,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="D8" s="52" t="s">
         <v>706</v>
@@ -16713,13 +16784,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B9" s="52" t="s">
         <v>1045</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>1044</v>
-      </c>
       <c r="C9" s="52" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>706</v>
@@ -16727,24 +16798,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>826</v>
@@ -16755,13 +16826,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>706</v>
@@ -16769,13 +16840,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D13" s="52" t="s">
         <v>701</v>
@@ -16783,13 +16854,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>706</v>
@@ -16797,13 +16868,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>706</v>
@@ -16811,13 +16882,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>701</v>
@@ -16825,24 +16896,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>714</v>
@@ -16853,10 +16924,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>826</v>
@@ -16867,13 +16938,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>706</v>
@@ -16881,10 +16952,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>826</v>
@@ -16895,13 +16966,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="D22" s="52" t="s">
         <v>706</v>
@@ -16909,27 +16980,27 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>826</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D24" s="52" t="s">
         <v>701</v>
@@ -16937,13 +17008,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>701</v>
@@ -16951,10 +17022,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>826</v>
@@ -16965,10 +17036,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B27" s="52" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>871</v>
@@ -16979,10 +17050,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>826</v>
@@ -16993,27 +17064,27 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B29" s="52" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B30" s="52" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D30" s="52" t="s">
         <v>701</v>
@@ -17021,10 +17092,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>826</v>
@@ -17035,13 +17106,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>798</v>
@@ -17049,41 +17120,41 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="52" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="52" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>804</v>
@@ -17091,10 +17162,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="52" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>826</v>
@@ -17105,13 +17176,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="D37" s="52" t="s">
         <v>701</v>
@@ -17139,20 +17210,20 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>643</v>
@@ -17160,13 +17231,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>798</v>
@@ -17174,58 +17245,58 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17311,6 +17382,190 @@
       <c r="B20" s="53"/>
       <c r="C20" s="53"/>
       <c r="D20" s="53"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>638</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>794</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>714</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="52" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B2" s="52" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>821</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B3" s="52" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B4" s="52" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B5" s="52" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>816</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="52" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>961</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>821</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="52" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="52" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B8" s="52" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>821</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>985</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -17334,7 +17589,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -18666,7 +18921,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -18978,7 +19233,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -19759,7 +20014,7 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -20758,7 +21013,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
   </cols>
@@ -20908,11 +21163,11 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
   </cols>
@@ -21417,6 +21672,9 @@
       <c r="B24" s="52" t="s">
         <v>881</v>
       </c>
+      <c r="E24" s="0" t="s">
+        <v>882</v>
+      </c>
       <c r="F24" s="0" t="s">
         <v>879</v>
       </c>
@@ -21429,10 +21687,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="H25" s="52" t="s">
         <v>833</v>
@@ -21443,10 +21701,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="H26" s="52" t="s">
         <v>821</v>
@@ -21457,10 +21715,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B27" s="52" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="H27" s="52" t="s">
         <v>816</v>
@@ -21471,13 +21729,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="H28" s="52" t="s">
         <v>816</v>
@@ -21488,13 +21746,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>892</v>
+      </c>
+      <c r="B29" s="52" t="s">
+        <v>893</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>891</v>
-      </c>
-      <c r="B29" s="52" t="s">
-        <v>892</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>890</v>
       </c>
       <c r="H29" s="52" t="s">
         <v>821</v>
@@ -21505,13 +21763,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B30" s="52" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="H30" s="52" t="s">
         <v>833</v>
@@ -21522,27 +21780,27 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="48" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>20</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>816</v>
@@ -21553,13 +21811,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>35</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>824</v>
@@ -21570,13 +21828,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>40</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>821</v>
@@ -21587,16 +21845,16 @@
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>60</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="I35" s="2" t="n">
         <v>500</v>
@@ -21604,13 +21862,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="51" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>906</v>
+        <v>907</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="H36" s="52" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="I36" s="52" t="n">
         <v>20</v>
@@ -21618,13 +21879,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="H37" s="52" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="I37" s="52" t="n">
         <v>40</v>
@@ -21632,13 +21893,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="52" t="s">
+        <v>912</v>
+      </c>
+      <c r="B38" s="52" t="s">
+        <v>913</v>
+      </c>
+      <c r="H38" s="52" t="s">
         <v>911</v>
-      </c>
-      <c r="B38" s="52" t="s">
-        <v>912</v>
-      </c>
-      <c r="H38" s="52" t="s">
-        <v>910</v>
       </c>
       <c r="I38" s="52" t="n">
         <v>50</v>
@@ -21646,13 +21907,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="52" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="H39" s="52" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="I39" s="52" t="n">
         <v>20</v>
@@ -21660,13 +21921,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="52" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="H40" s="52" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="I40" s="52" t="n">
         <v>40</v>
@@ -21694,20 +21955,20 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>794</v>
@@ -21721,7 +21982,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>218</v>
@@ -21741,7 +22002,7 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>218</v>
@@ -21761,13 +22022,13 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>5</v>
@@ -21781,13 +22042,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>5</v>
@@ -21801,7 +22062,7 @@
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>218</v>
@@ -21821,13 +22082,13 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>10</v>
@@ -21841,7 +22102,7 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
@@ -21861,19 +22122,19 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.2</v>
@@ -21904,23 +22165,23 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>806</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>714</v>
@@ -21931,13 +22192,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>13</v>
@@ -21954,13 +22215,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>12</v>
@@ -21977,7 +22238,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
Done some testing, and finaly update base is not as primitive, as it was.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1139">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2475,9 +2475,6 @@
   </si>
   <si>
     <t xml:space="preserve">200$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">szpej</t>
   </si>
   <si>
     <t xml:space="preserve">Max_Unik</t>
@@ -4136,7 +4133,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15722,14 +15719,14 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>3</v>
@@ -15738,13 +15735,13 @@
         <v>794</v>
       </c>
       <c r="D1" s="52" t="s">
+        <v>947</v>
+      </c>
+      <c r="E1" s="52" t="s">
         <v>948</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="F1" s="52" t="s">
         <v>949</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>950</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>715</v>
@@ -15754,7 +15751,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>5</v>
@@ -15767,7 +15764,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>692</v>
@@ -15777,30 +15774,30 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="52" t="s">
+        <v>953</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>954</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>955</v>
       </c>
       <c r="E3" s="52" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>10</v>
@@ -15813,130 +15810,130 @@
         <v>5</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="52" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E5" s="52" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
+        <v>961</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>962</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>963</v>
       </c>
       <c r="E6" s="52" t="n">
         <v>10</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>965</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="C7" s="52" t="s">
         <v>966</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>967</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>968</v>
       </c>
       <c r="E7" s="52" t="n">
         <v>50</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>968</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>965</v>
+      </c>
+      <c r="C8" s="52" t="s">
         <v>969</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>966</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>970</v>
-      </c>
       <c r="D8" s="52" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E8" s="52" t="n">
         <v>5</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>971</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>965</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>972</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>966</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>973</v>
-      </c>
       <c r="D9" s="52" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E9" s="52" t="n">
         <v>3</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G9" s="52" t="s">
         <v>692</v>
@@ -15946,13 +15943,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>18</v>
@@ -15961,7 +15958,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>698</v>
@@ -15971,22 +15968,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>975</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>965</v>
+      </c>
+      <c r="C11" s="52" t="s">
         <v>976</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>966</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>977</v>
-      </c>
       <c r="D11" s="52" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E11" s="52" t="n">
         <v>5</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>685</v>
@@ -16137,26 +16134,26 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>638</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>794</v>
@@ -16173,22 +16170,22 @@
         <v>750</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>981</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>982</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>983</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>966</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>984</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>685</v>
@@ -16196,97 +16193,97 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>985</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>986</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>987</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>984</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>991</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>992</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>993</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>966</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>995</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>996</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>997</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>794</v>
@@ -16300,20 +16297,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>1002</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>2</v>
@@ -16324,74 +16321,74 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="G8" s="54" t="s">
-        <v>1004</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>1005</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>1006</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
   </sheetData>
@@ -16416,23 +16413,23 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>1008</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="0" t="s">
         <v>1009</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>1010</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1011</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>643</v>
@@ -16440,7 +16437,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.5</v>
@@ -16455,12 +16452,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -16472,12 +16469,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="0" t="n">
@@ -16487,12 +16484,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C5" s="52" t="n">
         <v>1</v>
@@ -16501,12 +16498,12 @@
         <v>2</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C6" s="52" t="n">
         <v>0.5</v>
@@ -16515,12 +16512,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C7" s="52" t="n">
         <v>1</v>
@@ -16529,7 +16526,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
   </sheetData>
@@ -16554,20 +16551,20 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>715</v>
@@ -16575,13 +16572,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1021</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="52" t="s">
         <v>1022</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>1023</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>804</v>
@@ -16589,13 +16586,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1024</v>
       </c>
-      <c r="B3" s="52" t="s">
-        <v>1025</v>
-      </c>
       <c r="C3" s="52" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D3" s="52" t="s">
         <v>804</v>
@@ -16603,41 +16600,41 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1026</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1027</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>1028</v>
-      </c>
       <c r="D4" s="52" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1029</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>1030</v>
-      </c>
       <c r="C5" s="52" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1031</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>1032</v>
-      </c>
       <c r="C6" s="52" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D6" s="52" t="s">
         <v>804</v>
@@ -16665,14 +16662,14 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1033</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>1034</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>714</v>
@@ -16683,41 +16680,41 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1035</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="52" t="s">
+        <v>854</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>1036</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>855</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>706</v>
@@ -16725,13 +16722,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D5" s="52" t="s">
         <v>689</v>
@@ -16739,13 +16736,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1041</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>1042</v>
-      </c>
       <c r="C6" s="52" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D6" s="52" t="s">
         <v>706</v>
@@ -16753,13 +16750,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>1043</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>1044</v>
-      </c>
       <c r="C7" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>706</v>
@@ -16767,13 +16764,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B8" s="52" t="s">
         <v>1045</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>1046</v>
-      </c>
       <c r="C8" s="52" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D8" s="52" t="s">
         <v>706</v>
@@ -16781,13 +16778,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>1047</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>1048</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>706</v>
@@ -16795,27 +16792,27 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>1049</v>
       </c>
-      <c r="B10" s="52" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>1050</v>
-      </c>
       <c r="D10" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>1051</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>1052</v>
-      </c>
       <c r="C11" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D11" s="52" t="s">
         <v>706</v>
@@ -16823,13 +16820,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>706</v>
@@ -16837,13 +16834,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B13" s="52" t="s">
         <v>1054</v>
       </c>
-      <c r="B13" s="52" t="s">
-        <v>1055</v>
-      </c>
       <c r="C13" s="52" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D13" s="52" t="s">
         <v>701</v>
@@ -16851,13 +16848,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>1056</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>1057</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>706</v>
@@ -16865,13 +16862,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C15" s="52" t="s">
         <v>1058</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>1059</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>706</v>
@@ -16879,13 +16876,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>1060</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="C16" s="52" t="s">
         <v>1061</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>1062</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>701</v>
@@ -16893,24 +16890,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D17" s="52" t="s">
         <v>1063</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>1057</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>1064</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>714</v>
@@ -16921,13 +16918,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>1066</v>
       </c>
-      <c r="B19" s="52" t="s">
-        <v>1067</v>
-      </c>
       <c r="C19" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D19" s="52" t="s">
         <v>689</v>
@@ -16935,13 +16932,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>1068</v>
-      </c>
-      <c r="B20" s="52" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>1069</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>706</v>
@@ -16949,13 +16946,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D21" s="52" t="s">
         <v>706</v>
@@ -16963,13 +16960,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D22" s="52" t="s">
         <v>706</v>
@@ -16977,27 +16974,27 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B24" s="52" t="s">
         <v>1073</v>
       </c>
-      <c r="B24" s="52" t="s">
-        <v>1074</v>
-      </c>
       <c r="C24" s="52" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D24" s="52" t="s">
         <v>701</v>
@@ -17005,13 +17002,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>1075</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="C25" s="52" t="s">
         <v>1076</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>1077</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>701</v>
@@ -17019,13 +17016,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D26" s="52" t="s">
         <v>804</v>
@@ -17033,13 +17030,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>1079</v>
       </c>
-      <c r="B27" s="52" t="s">
-        <v>1080</v>
-      </c>
       <c r="C27" s="52" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D27" s="52" t="s">
         <v>701</v>
@@ -17047,13 +17044,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D28" s="52" t="s">
         <v>689</v>
@@ -17061,27 +17058,27 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B29" s="52" t="s">
         <v>1082</v>
       </c>
-      <c r="B29" s="52" t="s">
-        <v>1083</v>
-      </c>
       <c r="C29" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>1084</v>
       </c>
-      <c r="B30" s="52" t="s">
-        <v>1085</v>
-      </c>
       <c r="C30" s="52" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D30" s="52" t="s">
         <v>701</v>
@@ -17089,13 +17086,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C31" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D31" s="52" t="s">
         <v>804</v>
@@ -17103,13 +17100,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B32" s="52" t="s">
         <v>1087</v>
       </c>
-      <c r="B32" s="52" t="s">
-        <v>1088</v>
-      </c>
       <c r="C32" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>798</v>
@@ -17117,41 +17114,41 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="52" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B33" s="52" t="s">
         <v>1089</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="C33" s="52" t="s">
         <v>1090</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="D33" s="52" t="s">
         <v>1091</v>
-      </c>
-      <c r="D33" s="52" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="52" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B35" s="52" t="s">
         <v>1094</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="C35" s="52" t="s">
         <v>1095</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>1096</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>804</v>
@@ -17159,13 +17156,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="52" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>1097</v>
       </c>
-      <c r="B36" s="52" t="s">
-        <v>1098</v>
-      </c>
       <c r="C36" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D36" s="52" t="s">
         <v>685</v>
@@ -17173,13 +17170,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B37" s="52" t="s">
         <v>1060</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="C37" s="52" t="s">
         <v>1061</v>
-      </c>
-      <c r="C37" s="52" t="s">
-        <v>1062</v>
       </c>
       <c r="D37" s="52" t="s">
         <v>701</v>
@@ -17207,20 +17204,20 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1099</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>1100</v>
-      </c>
       <c r="C1" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>643</v>
@@ -17228,13 +17225,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1101</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>1102</v>
-      </c>
       <c r="C2" s="52" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>798</v>
@@ -17242,58 +17239,58 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1103</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="C3" s="52" t="s">
         <v>1104</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="D3" s="52" t="s">
         <v>1105</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1107</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1108</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="D4" s="52" t="s">
         <v>1109</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1111</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="C5" s="52" t="s">
         <v>1112</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="D5" s="52" t="s">
         <v>1113</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>1114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1115</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="C6" s="52" t="s">
         <v>1116</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1117</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17402,17 +17399,17 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>638</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>794</v>
@@ -17426,19 +17423,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="52" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>1122</v>
       </c>
-      <c r="D2" s="52" t="s">
-        <v>1123</v>
-      </c>
       <c r="E2" s="52" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F2" s="52" t="s">
         <v>701</v>
@@ -17446,19 +17443,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B3" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>685</v>
@@ -17466,19 +17463,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>798</v>
@@ -17486,19 +17483,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F5" s="52" t="s">
         <v>685</v>
@@ -17506,19 +17503,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>965</v>
+      </c>
+      <c r="C6" s="52" t="s">
         <v>1130</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>966</v>
-      </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1131</v>
       </c>
-      <c r="D6" s="52" t="s">
-        <v>1132</v>
-      </c>
       <c r="E6" s="52" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>685</v>
@@ -17526,42 +17523,42 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>1133</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>1134</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="E7" s="52" t="s">
         <v>1135</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>1136</v>
-      </c>
       <c r="F7" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="52" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>1138</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>1139</v>
-      </c>
       <c r="E8" s="52" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
   </sheetData>
@@ -17586,7 +17583,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -18918,7 +18915,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -19230,7 +19227,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
@@ -20011,7 +20008,7 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -21010,7 +21007,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
   </cols>
@@ -21160,36 +21157,36 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>805</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>806</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>807</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>808</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>809</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>810</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>795</v>
@@ -21200,10 +21197,10 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>811</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>812</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>20</v>
@@ -21212,16 +21209,16 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>813</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>815</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>816</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>2000</v>
@@ -21229,7 +21226,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="n">
@@ -21239,16 +21236,16 @@
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>818</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>819</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>820</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>821</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>300</v>
@@ -21256,7 +21253,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="n">
@@ -21266,16 +21263,16 @@
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>813</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>823</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>814</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>824</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>500</v>
@@ -21283,7 +21280,7 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="n">
@@ -21293,16 +21290,16 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>1000</v>
@@ -21310,7 +21307,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="n">
@@ -21320,16 +21317,16 @@
         <v>6</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>828</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>819</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>829</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>600</v>
@@ -21337,7 +21334,7 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="n">
@@ -21347,16 +21344,16 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>831</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>819</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>832</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>833</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>5000</v>
@@ -21364,10 +21361,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>834</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>835</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>8</v>
@@ -21376,16 +21373,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>836</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>837</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>838</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>10000</v>
@@ -21393,10 +21390,10 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>839</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>840</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>15</v>
@@ -21405,16 +21402,16 @@
         <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>1000000</v>
@@ -21422,13 +21419,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B10" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E10" s="53"/>
       <c r="F10" s="53"/>
@@ -21441,19 +21438,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>842</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>843</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="E11" s="52" t="s">
         <v>844</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="F11" s="53" t="s">
+        <v>818</v>
+      </c>
+      <c r="H11" s="52" t="s">
         <v>845</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>819</v>
-      </c>
-      <c r="H11" s="52" t="s">
-        <v>846</v>
       </c>
       <c r="I11" s="52" t="n">
         <v>200</v>
@@ -21461,17 +21458,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B12" s="52"/>
       <c r="E12" s="53" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F12" s="53" t="s">
+        <v>847</v>
+      </c>
+      <c r="H12" s="52" t="s">
         <v>848</v>
-      </c>
-      <c r="H12" s="52" t="s">
-        <v>849</v>
       </c>
       <c r="I12" s="52" t="n">
         <v>100</v>
@@ -21479,17 +21476,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B13" s="52"/>
       <c r="E13" s="53" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F13" s="53" t="s">
+        <v>847</v>
+      </c>
+      <c r="H13" s="52" t="s">
         <v>848</v>
-      </c>
-      <c r="H13" s="52" t="s">
-        <v>849</v>
       </c>
       <c r="I13" s="52" t="n">
         <v>100</v>
@@ -21497,19 +21494,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
+        <v>851</v>
+      </c>
+      <c r="B14" s="52" t="s">
         <v>852</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="E14" s="53" t="s">
         <v>853</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="F14" s="53" t="s">
+        <v>813</v>
+      </c>
+      <c r="H14" s="52" t="s">
         <v>854</v>
-      </c>
-      <c r="F14" s="53" t="s">
-        <v>814</v>
-      </c>
-      <c r="H14" s="52" t="s">
-        <v>855</v>
       </c>
       <c r="I14" s="52" t="n">
         <v>100</v>
@@ -21517,19 +21514,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
+        <v>855</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>852</v>
+      </c>
+      <c r="E15" s="53" t="s">
         <v>856</v>
       </c>
-      <c r="B15" s="52" t="s">
-        <v>853</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>857</v>
-      </c>
       <c r="F15" s="53" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="H15" s="52" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I15" s="52" t="n">
         <v>100</v>
@@ -21537,19 +21534,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
+        <v>857</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>858</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="E16" s="53" t="s">
         <v>859</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>860</v>
       </c>
       <c r="F16" s="53" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="52" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I16" s="52" t="n">
         <v>100</v>
@@ -21557,19 +21554,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
+        <v>860</v>
+      </c>
+      <c r="B17" s="52" t="s">
         <v>861</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="E17" s="53" t="s">
         <v>862</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>863</v>
       </c>
       <c r="F17" s="53" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="I17" s="52" t="n">
         <v>200</v>
@@ -21577,7 +21574,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>794</v>
@@ -21591,16 +21588,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
+        <v>865</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>866</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="F19" s="0" t="s">
         <v>867</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="H19" s="52" t="s">
         <v>868</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>869</v>
       </c>
       <c r="I19" s="52" t="n">
         <v>20</v>
@@ -21608,16 +21605,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
+        <v>869</v>
+      </c>
+      <c r="B20" s="52" t="s">
         <v>870</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="F20" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="H20" s="52" t="s">
         <v>871</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>868</v>
-      </c>
-      <c r="H20" s="52" t="s">
-        <v>872</v>
       </c>
       <c r="I20" s="52" t="n">
         <v>100</v>
@@ -21625,16 +21622,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
+        <v>872</v>
+      </c>
+      <c r="B21" s="52" t="s">
         <v>873</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="F21" s="0" t="s">
         <v>874</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="H21" s="52" t="s">
         <v>875</v>
-      </c>
-      <c r="H21" s="52" t="s">
-        <v>876</v>
       </c>
       <c r="I21" s="52" t="n">
         <v>100</v>
@@ -21642,16 +21639,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
+        <v>876</v>
+      </c>
+      <c r="B22" s="52" t="s">
         <v>877</v>
       </c>
-      <c r="B22" s="52" t="s">
-        <v>878</v>
-      </c>
       <c r="F22" s="0" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H22" s="52" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="I22" s="52" t="n">
         <v>500</v>
@@ -21659,16 +21656,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
+        <v>878</v>
+      </c>
+      <c r="B23" s="52" t="s">
         <v>879</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="F23" s="0" t="s">
         <v>880</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>881</v>
-      </c>
       <c r="H23" s="52" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I23" s="52" t="n">
         <v>100</v>
@@ -21676,19 +21673,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>881</v>
+      </c>
+      <c r="B24" s="52" t="s">
         <v>882</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="E24" s="0" t="s">
         <v>883</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>884</v>
-      </c>
       <c r="F24" s="0" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="H24" s="52" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I24" s="52" t="n">
         <v>500</v>
@@ -21696,13 +21693,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
+        <v>884</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>885</v>
       </c>
-      <c r="B25" s="52" t="s">
-        <v>886</v>
-      </c>
       <c r="H25" s="52" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="I25" s="52" t="n">
         <v>1000</v>
@@ -21710,13 +21707,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
+        <v>886</v>
+      </c>
+      <c r="B26" s="52" t="s">
         <v>887</v>
       </c>
-      <c r="B26" s="52" t="s">
-        <v>888</v>
-      </c>
       <c r="H26" s="52" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I26" s="52" t="n">
         <v>4500</v>
@@ -21724,13 +21721,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
+        <v>888</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>889</v>
       </c>
-      <c r="B27" s="52" t="s">
-        <v>890</v>
-      </c>
       <c r="H27" s="52" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I27" s="52" t="n">
         <v>7500</v>
@@ -21738,16 +21735,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
+        <v>890</v>
+      </c>
+      <c r="B28" s="52" t="s">
         <v>891</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="F28" s="0" t="s">
         <v>892</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>893</v>
-      </c>
       <c r="H28" s="52" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I28" s="52" t="n">
         <v>200</v>
@@ -21755,16 +21752,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>893</v>
+      </c>
+      <c r="B29" s="52" t="s">
         <v>894</v>
       </c>
-      <c r="B29" s="52" t="s">
-        <v>895</v>
-      </c>
       <c r="F29" s="0" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H29" s="52" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I29" s="52" t="n">
         <v>2000</v>
@@ -21772,16 +21769,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
+        <v>895</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>896</v>
       </c>
-      <c r="B30" s="52" t="s">
-        <v>897</v>
-      </c>
       <c r="F30" s="0" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H30" s="52" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="I30" s="52" t="n">
         <v>5000</v>
@@ -21789,30 +21786,30 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="48" t="s">
+        <v>897</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>899</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>900</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>20</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I32" s="2" t="n">
         <v>50</v>
@@ -21820,16 +21817,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>35</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="I33" s="2" t="n">
         <v>100</v>
@@ -21837,16 +21834,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>40</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I34" s="2" t="n">
         <v>250</v>
@@ -21854,16 +21851,16 @@
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>60</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="I35" s="2" t="n">
         <v>500</v>
@@ -21871,16 +21868,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="51" t="s">
+        <v>907</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>908</v>
-      </c>
-      <c r="B36" s="52" t="s">
-        <v>909</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H36" s="52" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I36" s="52" t="n">
         <v>20</v>
@@ -21888,16 +21885,16 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
+        <v>910</v>
+      </c>
+      <c r="B37" s="52" t="s">
         <v>911</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="F37" s="0" t="s">
         <v>912</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="H37" s="52" t="s">
         <v>913</v>
-      </c>
-      <c r="H37" s="52" t="s">
-        <v>914</v>
       </c>
       <c r="I37" s="52" t="n">
         <v>40</v>
@@ -21905,16 +21902,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="52" t="s">
+        <v>914</v>
+      </c>
+      <c r="B38" s="52" t="s">
         <v>915</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="F38" s="0" t="s">
         <v>916</v>
       </c>
-      <c r="F38" s="0" t="s">
-        <v>917</v>
-      </c>
       <c r="H38" s="52" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="I38" s="52" t="n">
         <v>50</v>
@@ -21922,16 +21919,16 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="52" t="s">
+        <v>917</v>
+      </c>
+      <c r="B39" s="52" t="s">
         <v>918</v>
       </c>
-      <c r="B39" s="52" t="s">
+      <c r="F39" s="0" t="s">
         <v>919</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="H39" s="52" t="s">
         <v>920</v>
-      </c>
-      <c r="H39" s="52" t="s">
-        <v>921</v>
       </c>
       <c r="I39" s="52" t="n">
         <v>20</v>
@@ -21939,16 +21936,16 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="52" t="s">
+        <v>921</v>
+      </c>
+      <c r="B40" s="52" t="s">
         <v>922</v>
       </c>
-      <c r="B40" s="52" t="s">
-        <v>923</v>
-      </c>
       <c r="F40" s="0" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="H40" s="52" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I40" s="52" t="n">
         <v>40</v>
@@ -21976,20 +21973,20 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>923</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>924</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>925</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>926</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>927</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>794</v>
@@ -22003,7 +22000,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>218</v>
@@ -22023,7 +22020,7 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>218</v>
@@ -22043,13 +22040,13 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>5</v>
@@ -22063,13 +22060,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>5</v>
@@ -22083,7 +22080,7 @@
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>218</v>
@@ -22103,13 +22100,13 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>10</v>
@@ -22123,7 +22120,7 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
@@ -22143,19 +22140,19 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.2</v>
@@ -22186,23 +22183,23 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>938</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>939</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>940</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>941</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>806</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>942</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>714</v>
@@ -22213,13 +22210,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>13</v>
@@ -22236,13 +22233,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>12</v>
@@ -22259,7 +22256,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
some cosmetics refactor, also sterted adding first aid kits.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1138">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2592,9 +2592,6 @@
   </si>
   <si>
     <t xml:space="preserve">Szelki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3A</t>
   </si>
   <si>
     <t xml:space="preserve">0,6kg</t>
@@ -4133,14 +4130,16 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.45"/>
@@ -15719,14 +15718,16 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>3</v>
@@ -15735,13 +15736,13 @@
         <v>794</v>
       </c>
       <c r="D1" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="E1" s="52" t="s">
         <v>947</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="F1" s="52" t="s">
         <v>948</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>949</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>715</v>
@@ -15751,7 +15752,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>5</v>
@@ -15764,7 +15765,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>692</v>
@@ -15774,30 +15775,30 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="52" t="s">
+        <v>952</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>953</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>954</v>
       </c>
       <c r="E3" s="52" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>10</v>
@@ -15810,49 +15811,49 @@
         <v>5</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="52" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E5" s="52" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
+        <v>960</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>961</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>962</v>
       </c>
       <c r="E6" s="52" t="n">
         <v>10</v>
@@ -15861,79 +15862,79 @@
         <v>815</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>964</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="C7" s="52" t="s">
         <v>965</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>966</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>967</v>
       </c>
       <c r="E7" s="52" t="n">
         <v>50</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>967</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="C8" s="52" t="s">
         <v>968</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>965</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>969</v>
-      </c>
       <c r="D8" s="52" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="E8" s="52" t="n">
         <v>5</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>970</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>971</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>965</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>972</v>
-      </c>
       <c r="D9" s="52" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="E9" s="52" t="n">
         <v>3</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G9" s="52" t="s">
         <v>692</v>
@@ -15943,13 +15944,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>18</v>
@@ -15958,7 +15959,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>698</v>
@@ -15968,22 +15969,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>974</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="C11" s="52" t="s">
         <v>975</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>965</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>976</v>
-      </c>
       <c r="D11" s="52" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E11" s="52" t="n">
         <v>5</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>685</v>
@@ -16134,26 +16135,28 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>638</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>794</v>
@@ -16170,22 +16173,22 @@
         <v>750</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>980</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>981</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>982</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>965</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>983</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>685</v>
@@ -16193,97 +16196,97 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>984</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>985</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>986</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>983</v>
-      </c>
-      <c r="H3" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>989</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>990</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>991</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>992</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>993</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>965</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>995</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>996</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>794</v>
@@ -16297,20 +16300,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>1000</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>1001</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>2</v>
@@ -16321,74 +16324,74 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="G8" s="54" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>1003</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>1004</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>1005</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
   </sheetData>
@@ -16413,23 +16416,26 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>1007</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="0" t="s">
         <v>1008</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>1009</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1010</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>643</v>
@@ -16437,7 +16443,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.5</v>
@@ -16452,12 +16458,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -16469,12 +16475,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="0" t="n">
@@ -16484,12 +16490,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C5" s="52" t="n">
         <v>1</v>
@@ -16498,12 +16504,12 @@
         <v>2</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C6" s="52" t="n">
         <v>0.5</v>
@@ -16512,12 +16518,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C7" s="52" t="n">
         <v>1</v>
@@ -16526,7 +16532,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
   </sheetData>
@@ -16551,20 +16557,21 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>715</v>
@@ -16572,13 +16579,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1020</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="52" t="s">
         <v>1021</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>1022</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>804</v>
@@ -16586,10 +16593,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1023</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>1024</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>815</v>
@@ -16600,41 +16607,41 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1025</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1026</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>1027</v>
-      </c>
       <c r="D4" s="52" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1028</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>1029</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>832</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1030</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>1031</v>
-      </c>
       <c r="C6" s="52" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D6" s="52" t="s">
         <v>804</v>
@@ -16662,14 +16669,17 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1032</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>1033</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>714</v>
@@ -16680,41 +16690,41 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1034</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="52" t="s">
+        <v>853</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>1035</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>854</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>1036</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>706</v>
@@ -16722,13 +16732,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D5" s="52" t="s">
         <v>689</v>
@@ -16736,13 +16746,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1040</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>1041</v>
-      </c>
       <c r="C6" s="52" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D6" s="52" t="s">
         <v>706</v>
@@ -16750,13 +16760,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>1043</v>
-      </c>
       <c r="C7" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>706</v>
@@ -16764,13 +16774,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B8" s="52" t="s">
         <v>1044</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>1045</v>
-      </c>
       <c r="C8" s="52" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D8" s="52" t="s">
         <v>706</v>
@@ -16778,13 +16788,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>1046</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>1047</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>706</v>
@@ -16792,24 +16802,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>1048</v>
       </c>
-      <c r="B10" s="52" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>1049</v>
-      </c>
       <c r="D10" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>1050</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>1051</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>825</v>
@@ -16820,13 +16830,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>706</v>
@@ -16834,13 +16844,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B13" s="52" t="s">
         <v>1053</v>
       </c>
-      <c r="B13" s="52" t="s">
-        <v>1054</v>
-      </c>
       <c r="C13" s="52" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D13" s="52" t="s">
         <v>701</v>
@@ -16848,13 +16858,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>1055</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>1056</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>706</v>
@@ -16862,13 +16872,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C15" s="52" t="s">
         <v>1057</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>1058</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>706</v>
@@ -16876,13 +16886,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>1059</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="C16" s="52" t="s">
         <v>1060</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>1061</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>701</v>
@@ -16890,24 +16900,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D17" s="52" t="s">
         <v>1062</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>1056</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>1063</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>714</v>
@@ -16918,10 +16928,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>1065</v>
-      </c>
-      <c r="B19" s="52" t="s">
-        <v>1066</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>825</v>
@@ -16932,13 +16942,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>1067</v>
-      </c>
-      <c r="B20" s="52" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>1068</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>706</v>
@@ -16946,10 +16956,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>825</v>
@@ -16960,13 +16970,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D22" s="52" t="s">
         <v>706</v>
@@ -16974,27 +16984,27 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>825</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B24" s="52" t="s">
         <v>1072</v>
       </c>
-      <c r="B24" s="52" t="s">
-        <v>1073</v>
-      </c>
       <c r="C24" s="52" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D24" s="52" t="s">
         <v>701</v>
@@ -17002,13 +17012,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>1074</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="C25" s="52" t="s">
         <v>1075</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>1076</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>701</v>
@@ -17016,10 +17026,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>825</v>
@@ -17030,13 +17040,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>1078</v>
       </c>
-      <c r="B27" s="52" t="s">
-        <v>1079</v>
-      </c>
       <c r="C27" s="52" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D27" s="52" t="s">
         <v>701</v>
@@ -17044,10 +17054,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>825</v>
@@ -17058,27 +17068,27 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B29" s="52" t="s">
         <v>1081</v>
       </c>
-      <c r="B29" s="52" t="s">
-        <v>1082</v>
-      </c>
       <c r="C29" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>1083</v>
       </c>
-      <c r="B30" s="52" t="s">
-        <v>1084</v>
-      </c>
       <c r="C30" s="52" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D30" s="52" t="s">
         <v>701</v>
@@ -17086,10 +17096,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>825</v>
@@ -17100,13 +17110,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B32" s="52" t="s">
         <v>1086</v>
       </c>
-      <c r="B32" s="52" t="s">
-        <v>1087</v>
-      </c>
       <c r="C32" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>798</v>
@@ -17114,41 +17124,41 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="52" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B33" s="52" t="s">
         <v>1088</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="C33" s="52" t="s">
         <v>1089</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="D33" s="52" t="s">
         <v>1090</v>
-      </c>
-      <c r="D33" s="52" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="52" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B35" s="52" t="s">
         <v>1093</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="C35" s="52" t="s">
         <v>1094</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>1095</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>804</v>
@@ -17156,10 +17166,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="52" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>1096</v>
-      </c>
-      <c r="B36" s="52" t="s">
-        <v>1097</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>825</v>
@@ -17170,13 +17180,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B37" s="52" t="s">
         <v>1059</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="C37" s="52" t="s">
         <v>1060</v>
-      </c>
-      <c r="C37" s="52" t="s">
-        <v>1061</v>
       </c>
       <c r="D37" s="52" t="s">
         <v>701</v>
@@ -17204,20 +17214,21 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1098</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>1099</v>
-      </c>
       <c r="C1" s="52" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>643</v>
@@ -17225,13 +17236,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1100</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>1101</v>
-      </c>
       <c r="C2" s="52" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>798</v>
@@ -17239,58 +17250,58 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1102</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="C3" s="52" t="s">
         <v>1103</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="D3" s="52" t="s">
         <v>1104</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>1105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1106</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1107</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="D4" s="52" t="s">
         <v>1108</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1110</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="C5" s="52" t="s">
         <v>1111</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="D5" s="52" t="s">
         <v>1112</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1114</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="C6" s="52" t="s">
         <v>1115</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1116</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17399,17 +17410,17 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>638</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>794</v>
@@ -17423,16 +17434,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="52" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>1121</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>1122</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>820</v>
@@ -17443,19 +17454,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B3" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>685</v>
@@ -17463,19 +17474,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>798</v>
@@ -17483,16 +17494,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E5" s="52" t="s">
         <v>815</v>
@@ -17503,16 +17514,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="C6" s="52" t="s">
         <v>1129</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>965</v>
-      </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1130</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>1131</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>820</v>
@@ -17523,42 +17534,42 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>1132</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>1133</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="E7" s="52" t="s">
         <v>1134</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="52" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="516.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="52" t="s">
         <v>1135</v>
-      </c>
-      <c r="F7" s="52" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="52" t="s">
-        <v>1136</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="52" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>1137</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1138</v>
       </c>
       <c r="E8" s="52" t="s">
         <v>820</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
   </sheetData>
@@ -17583,7 +17594,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -18190,7 +18204,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
         <v>666</v>
       </c>
@@ -18915,7 +18929,10 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
@@ -18946,7 +18963,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
         <v>682</v>
       </c>
@@ -19227,11 +19244,13 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="9" style="0" width="11.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20008,10 +20027,11 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="11.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20306,7 +20326,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>773</v>
       </c>
@@ -20335,7 +20355,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>176</v>
       </c>
@@ -20361,7 +20381,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>775</v>
       </c>
@@ -20387,7 +20407,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>776</v>
       </c>
@@ -20491,7 +20511,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>331</v>
       </c>
@@ -20517,7 +20537,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>465</v>
       </c>
@@ -20543,7 +20563,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>186</v>
       </c>
@@ -20569,7 +20589,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>438</v>
       </c>
@@ -20595,7 +20615,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>434</v>
       </c>
@@ -20621,7 +20641,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>782</v>
       </c>
@@ -20647,7 +20667,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>412</v>
       </c>
@@ -20673,7 +20693,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>438</v>
       </c>
@@ -20699,7 +20719,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>783</v>
       </c>
@@ -20725,7 +20745,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>429</v>
       </c>
@@ -20751,7 +20771,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>375</v>
       </c>
@@ -20777,7 +20797,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>150</v>
       </c>
@@ -20806,7 +20826,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>66</v>
       </c>
@@ -20835,7 +20855,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>463</v>
       </c>
@@ -20864,7 +20884,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>785</v>
       </c>
@@ -20893,7 +20913,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>788</v>
       </c>
@@ -20922,7 +20942,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>526</v>
       </c>
@@ -20951,7 +20971,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>209</v>
       </c>
@@ -20980,7 +21000,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
         <v>766</v>
       </c>
@@ -21007,9 +21027,11 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="6" style="0" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21157,13 +21179,14 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21444,13 +21467,13 @@
         <v>843</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="F11" s="53" t="s">
         <v>818</v>
       </c>
       <c r="H11" s="52" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="I11" s="52" t="n">
         <v>200</v>
@@ -21458,17 +21481,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B12" s="52"/>
       <c r="E12" s="53" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="F12" s="53" t="s">
+        <v>846</v>
+      </c>
+      <c r="H12" s="52" t="s">
         <v>847</v>
-      </c>
-      <c r="H12" s="52" t="s">
-        <v>848</v>
       </c>
       <c r="I12" s="52" t="n">
         <v>100</v>
@@ -21476,17 +21499,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B13" s="52"/>
       <c r="E13" s="53" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F13" s="53" t="s">
+        <v>846</v>
+      </c>
+      <c r="H13" s="52" t="s">
         <v>847</v>
-      </c>
-      <c r="H13" s="52" t="s">
-        <v>848</v>
       </c>
       <c r="I13" s="52" t="n">
         <v>100</v>
@@ -21494,19 +21517,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
+        <v>850</v>
+      </c>
+      <c r="B14" s="52" t="s">
         <v>851</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="E14" s="53" t="s">
         <v>852</v>
-      </c>
-      <c r="E14" s="53" t="s">
-        <v>853</v>
       </c>
       <c r="F14" s="53" t="s">
         <v>813</v>
       </c>
       <c r="H14" s="52" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="I14" s="52" t="n">
         <v>100</v>
@@ -21514,19 +21537,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
+        <v>854</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>851</v>
+      </c>
+      <c r="E15" s="53" t="s">
         <v>855</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>852</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>856</v>
       </c>
       <c r="F15" s="53" t="s">
         <v>813</v>
       </c>
       <c r="H15" s="52" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="I15" s="52" t="n">
         <v>100</v>
@@ -21534,19 +21557,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
+        <v>856</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>857</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="E16" s="53" t="s">
         <v>858</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>859</v>
       </c>
       <c r="F16" s="53" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="52" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="I16" s="52" t="n">
         <v>100</v>
@@ -21554,19 +21577,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
+        <v>859</v>
+      </c>
+      <c r="B17" s="52" t="s">
         <v>860</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="E17" s="53" t="s">
         <v>861</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>862</v>
       </c>
       <c r="F17" s="53" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="I17" s="52" t="n">
         <v>200</v>
@@ -21574,7 +21597,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>794</v>
@@ -21588,16 +21611,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
+        <v>864</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>865</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="F19" s="0" t="s">
         <v>866</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="H19" s="52" t="s">
         <v>867</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>868</v>
       </c>
       <c r="I19" s="52" t="n">
         <v>20</v>
@@ -21605,16 +21628,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
+        <v>868</v>
+      </c>
+      <c r="B20" s="52" t="s">
         <v>869</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="F20" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="H20" s="52" t="s">
         <v>870</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>867</v>
-      </c>
-      <c r="H20" s="52" t="s">
-        <v>871</v>
       </c>
       <c r="I20" s="52" t="n">
         <v>100</v>
@@ -21622,16 +21645,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="B21" s="52" t="s">
         <v>872</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="F21" s="0" t="s">
         <v>873</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="H21" s="52" t="s">
         <v>874</v>
-      </c>
-      <c r="H21" s="52" t="s">
-        <v>875</v>
       </c>
       <c r="I21" s="52" t="n">
         <v>100</v>
@@ -21639,13 +21662,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
+        <v>875</v>
+      </c>
+      <c r="B22" s="52" t="s">
         <v>876</v>
       </c>
-      <c r="B22" s="52" t="s">
-        <v>877</v>
-      </c>
       <c r="F22" s="0" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H22" s="52" t="s">
         <v>825</v>
@@ -21656,13 +21679,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
+        <v>877</v>
+      </c>
+      <c r="B23" s="52" t="s">
         <v>878</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="F23" s="0" t="s">
         <v>879</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>880</v>
       </c>
       <c r="H23" s="52" t="s">
         <v>820</v>
@@ -21673,16 +21696,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>880</v>
+      </c>
+      <c r="B24" s="52" t="s">
         <v>881</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="E24" s="0" t="s">
         <v>882</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>883</v>
-      </c>
       <c r="F24" s="0" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H24" s="52" t="s">
         <v>820</v>
@@ -21693,10 +21716,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
+        <v>883</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>884</v>
-      </c>
-      <c r="B25" s="52" t="s">
-        <v>885</v>
       </c>
       <c r="H25" s="52" t="s">
         <v>832</v>
@@ -21707,10 +21730,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
+        <v>885</v>
+      </c>
+      <c r="B26" s="52" t="s">
         <v>886</v>
-      </c>
-      <c r="B26" s="52" t="s">
-        <v>887</v>
       </c>
       <c r="H26" s="52" t="s">
         <v>820</v>
@@ -21721,10 +21744,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
+        <v>887</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>888</v>
-      </c>
-      <c r="B27" s="52" t="s">
-        <v>889</v>
       </c>
       <c r="H27" s="52" t="s">
         <v>815</v>
@@ -21735,13 +21758,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
+        <v>889</v>
+      </c>
+      <c r="B28" s="52" t="s">
         <v>890</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="F28" s="0" t="s">
         <v>891</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>892</v>
       </c>
       <c r="H28" s="52" t="s">
         <v>815</v>
@@ -21752,13 +21775,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>892</v>
+      </c>
+      <c r="B29" s="52" t="s">
         <v>893</v>
       </c>
-      <c r="B29" s="52" t="s">
-        <v>894</v>
-      </c>
       <c r="F29" s="0" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H29" s="52" t="s">
         <v>820</v>
@@ -21769,13 +21792,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
+        <v>894</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>895</v>
       </c>
-      <c r="B30" s="52" t="s">
-        <v>896</v>
-      </c>
       <c r="F30" s="0" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H30" s="52" t="s">
         <v>832</v>
@@ -21786,27 +21809,27 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="48" t="s">
+        <v>896</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>897</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>899</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>20</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>815</v>
@@ -21817,13 +21840,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>35</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>823</v>
@@ -21834,13 +21857,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>40</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>820</v>
@@ -21851,16 +21874,16 @@
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>60</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="I35" s="2" t="n">
         <v>500</v>
@@ -21868,16 +21891,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="51" t="s">
+        <v>906</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>907</v>
-      </c>
-      <c r="B36" s="52" t="s">
-        <v>908</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H36" s="52" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I36" s="52" t="n">
         <v>20</v>
@@ -21885,16 +21908,16 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
+        <v>909</v>
+      </c>
+      <c r="B37" s="52" t="s">
         <v>910</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="F37" s="0" t="s">
         <v>911</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="H37" s="52" t="s">
         <v>912</v>
-      </c>
-      <c r="H37" s="52" t="s">
-        <v>913</v>
       </c>
       <c r="I37" s="52" t="n">
         <v>40</v>
@@ -21902,16 +21925,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="52" t="s">
+        <v>913</v>
+      </c>
+      <c r="B38" s="52" t="s">
         <v>914</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="F38" s="0" t="s">
         <v>915</v>
       </c>
-      <c r="F38" s="0" t="s">
-        <v>916</v>
-      </c>
       <c r="H38" s="52" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="I38" s="52" t="n">
         <v>50</v>
@@ -21919,16 +21942,16 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="52" t="s">
+        <v>916</v>
+      </c>
+      <c r="B39" s="52" t="s">
         <v>917</v>
       </c>
-      <c r="B39" s="52" t="s">
+      <c r="F39" s="0" t="s">
         <v>918</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="H39" s="52" t="s">
         <v>919</v>
-      </c>
-      <c r="H39" s="52" t="s">
-        <v>920</v>
       </c>
       <c r="I39" s="52" t="n">
         <v>20</v>
@@ -21936,16 +21959,16 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="52" t="s">
+        <v>920</v>
+      </c>
+      <c r="B40" s="52" t="s">
         <v>921</v>
       </c>
-      <c r="B40" s="52" t="s">
-        <v>922</v>
-      </c>
       <c r="F40" s="0" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="H40" s="52" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I40" s="52" t="n">
         <v>40</v>
@@ -21973,20 +21996,23 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>922</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>924</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>925</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>926</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>794</v>
@@ -22000,7 +22026,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>218</v>
@@ -22020,7 +22046,7 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>218</v>
@@ -22040,13 +22066,13 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>5</v>
@@ -22060,13 +22086,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>5</v>
@@ -22080,7 +22106,7 @@
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>218</v>
@@ -22100,13 +22126,13 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>10</v>
@@ -22120,7 +22146,7 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
@@ -22140,19 +22166,19 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.2</v>
@@ -22183,23 +22209,26 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>937</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>938</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>939</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>940</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>805</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>714</v>
@@ -22210,13 +22239,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>13</v>
@@ -22233,13 +22262,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>12</v>
@@ -22256,7 +22285,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
Roll to hit for granades Done.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1137">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2895,9 +2895,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ciężka Militarna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apteczka</t>
   </si>
   <si>
     <t xml:space="preserve">zajmowane_miejsce</t>
@@ -15714,8 +15711,8 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15727,7 +15724,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>945</v>
+        <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>3</v>
@@ -15736,13 +15733,13 @@
         <v>794</v>
       </c>
       <c r="D1" s="52" t="s">
+        <v>945</v>
+      </c>
+      <c r="E1" s="52" t="s">
         <v>946</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="F1" s="52" t="s">
         <v>947</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>948</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>715</v>
@@ -15752,7 +15749,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>5</v>
@@ -15765,7 +15762,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>692</v>
@@ -15775,14 +15772,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="52" t="s">
+        <v>951</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>952</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>953</v>
       </c>
       <c r="E3" s="52" t="n">
         <v>1</v>
@@ -15791,14 +15788,14 @@
         <v>908</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>10</v>
@@ -15814,21 +15811,21 @@
         <v>853</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="52" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E5" s="52" t="n">
         <v>1</v>
@@ -15837,23 +15834,23 @@
         <v>919</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
+        <v>959</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>960</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>961</v>
       </c>
       <c r="E6" s="52" t="n">
         <v>10</v>
@@ -15862,23 +15859,23 @@
         <v>815</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>962</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>963</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="C7" s="52" t="s">
         <v>964</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>965</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>966</v>
       </c>
       <c r="E7" s="52" t="n">
         <v>50</v>
@@ -15887,23 +15884,23 @@
         <v>912</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>966</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="C8" s="52" t="s">
         <v>967</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>964</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>968</v>
-      </c>
       <c r="D8" s="52" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E8" s="52" t="n">
         <v>5</v>
@@ -15912,23 +15909,23 @@
         <v>908</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>969</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>970</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>964</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>971</v>
-      </c>
       <c r="D9" s="52" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E9" s="52" t="n">
         <v>3</v>
@@ -15944,13 +15941,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>18</v>
@@ -15959,7 +15956,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>698</v>
@@ -15969,16 +15966,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>973</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="C11" s="52" t="s">
         <v>974</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>964</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>975</v>
-      </c>
       <c r="D11" s="52" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E11" s="52" t="n">
         <v>5</v>
@@ -16144,19 +16141,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>638</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>794</v>
@@ -16173,22 +16170,22 @@
         <v>750</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>979</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>980</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>981</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>964</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>982</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>685</v>
@@ -16196,97 +16193,97 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>983</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>984</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>986</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>987</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>982</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>989</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>990</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>991</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>992</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>964</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>993</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>995</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>794</v>
@@ -16300,20 +16297,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>999</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>1000</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>2</v>
@@ -16324,74 +16321,74 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>987</v>
-      </c>
-      <c r="G8" s="54" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>1003</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>1004</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
   </sheetData>
@@ -16426,16 +16423,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>1006</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="0" t="s">
         <v>1007</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>1008</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1009</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>643</v>
@@ -16443,7 +16440,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.5</v>
@@ -16458,12 +16455,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -16475,12 +16472,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="0" t="n">
@@ -16490,12 +16487,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C5" s="52" t="n">
         <v>1</v>
@@ -16504,12 +16501,12 @@
         <v>2</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C6" s="52" t="n">
         <v>0.5</v>
@@ -16518,12 +16515,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C7" s="52" t="n">
         <v>1</v>
@@ -16532,7 +16529,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
   </sheetData>
@@ -16565,13 +16562,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>715</v>
@@ -16579,13 +16576,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1019</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="52" t="s">
         <v>1020</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>1021</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>804</v>
@@ -16593,10 +16590,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1022</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>1023</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>815</v>
@@ -16607,38 +16604,38 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1024</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1025</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>1026</v>
-      </c>
       <c r="D4" s="52" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1027</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>1028</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>832</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1029</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>1030</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>905</v>
@@ -16676,10 +16673,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1031</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>1032</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>714</v>
@@ -16690,38 +16687,38 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1033</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>1034</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>853</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>853</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>853</v>
@@ -16732,10 +16729,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>853</v>
@@ -16746,10 +16743,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1039</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>1040</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>870</v>
@@ -16760,13 +16757,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>1041</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>1042</v>
-      </c>
       <c r="C7" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>706</v>
@@ -16774,10 +16771,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B8" s="52" t="s">
         <v>1043</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>1044</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>919</v>
@@ -16788,13 +16785,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>1045</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>1046</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>706</v>
@@ -16802,24 +16799,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>1047</v>
       </c>
-      <c r="B10" s="52" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>1048</v>
-      </c>
       <c r="D10" s="52" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>1049</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>1050</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>825</v>
@@ -16830,13 +16827,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>706</v>
@@ -16844,10 +16841,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B13" s="52" t="s">
         <v>1052</v>
-      </c>
-      <c r="B13" s="52" t="s">
-        <v>1053</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>912</v>
@@ -16858,13 +16855,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>1054</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>1055</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>706</v>
@@ -16872,13 +16869,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C15" s="52" t="s">
         <v>1056</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>1057</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>706</v>
@@ -16886,13 +16883,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>1058</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="C16" s="52" t="s">
         <v>1059</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>1060</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>701</v>
@@ -16900,24 +16897,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D17" s="52" t="s">
         <v>1061</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>1062</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>714</v>
@@ -16928,10 +16925,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>1064</v>
-      </c>
-      <c r="B19" s="52" t="s">
-        <v>1065</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>825</v>
@@ -16942,13 +16939,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>1066</v>
-      </c>
-      <c r="B20" s="52" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>1067</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>706</v>
@@ -16956,10 +16953,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>825</v>
@@ -16970,13 +16967,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D22" s="52" t="s">
         <v>706</v>
@@ -16984,24 +16981,24 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>825</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B24" s="52" t="s">
         <v>1071</v>
-      </c>
-      <c r="B24" s="52" t="s">
-        <v>1072</v>
       </c>
       <c r="C24" s="52" t="s">
         <v>912</v>
@@ -17012,13 +17009,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>1073</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="C25" s="52" t="s">
         <v>1074</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>1075</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>701</v>
@@ -17026,10 +17023,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>825</v>
@@ -17040,10 +17037,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>1077</v>
-      </c>
-      <c r="B27" s="52" t="s">
-        <v>1078</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>870</v>
@@ -17054,10 +17051,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>825</v>
@@ -17068,24 +17065,24 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B29" s="52" t="s">
         <v>1080</v>
       </c>
-      <c r="B29" s="52" t="s">
-        <v>1081</v>
-      </c>
       <c r="C29" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>1082</v>
-      </c>
-      <c r="B30" s="52" t="s">
-        <v>1083</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>912</v>
@@ -17096,10 +17093,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>825</v>
@@ -17110,13 +17107,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B32" s="52" t="s">
         <v>1085</v>
       </c>
-      <c r="B32" s="52" t="s">
-        <v>1086</v>
-      </c>
       <c r="C32" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>798</v>
@@ -17124,41 +17121,41 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="52" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B33" s="52" t="s">
         <v>1087</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="C33" s="52" t="s">
         <v>1088</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="D33" s="52" t="s">
         <v>1089</v>
-      </c>
-      <c r="D33" s="52" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="52" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B35" s="52" t="s">
         <v>1092</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="C35" s="52" t="s">
         <v>1093</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>1094</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>804</v>
@@ -17166,10 +17163,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="52" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>1095</v>
-      </c>
-      <c r="B36" s="52" t="s">
-        <v>1096</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>825</v>
@@ -17180,13 +17177,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B37" s="52" t="s">
         <v>1058</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="C37" s="52" t="s">
         <v>1059</v>
-      </c>
-      <c r="C37" s="52" t="s">
-        <v>1060</v>
       </c>
       <c r="D37" s="52" t="s">
         <v>701</v>
@@ -17222,13 +17219,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1097</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>1098</v>
-      </c>
       <c r="C1" s="52" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>643</v>
@@ -17236,13 +17233,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1099</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>1100</v>
-      </c>
       <c r="C2" s="52" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>798</v>
@@ -17250,58 +17247,58 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1101</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="C3" s="52" t="s">
         <v>1102</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="D3" s="52" t="s">
         <v>1103</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>1104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1105</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1106</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="D4" s="52" t="s">
         <v>1107</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>1108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1109</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="C5" s="52" t="s">
         <v>1110</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="D5" s="52" t="s">
         <v>1111</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1113</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="C6" s="52" t="s">
         <v>1114</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1115</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17414,13 +17411,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>638</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>794</v>
@@ -17434,16 +17431,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="52" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>1120</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>1121</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>820</v>
@@ -17454,19 +17451,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B3" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>685</v>
@@ -17474,19 +17471,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>798</v>
@@ -17494,16 +17491,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="E5" s="52" t="s">
         <v>815</v>
@@ -17514,16 +17511,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="C6" s="52" t="s">
         <v>1128</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>964</v>
-      </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1129</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>1130</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>820</v>
@@ -17534,42 +17531,42 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>1131</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>1132</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="E7" s="52" t="s">
         <v>1133</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>1134</v>
-      </c>
       <c r="F7" s="52" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="516.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="52" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>1136</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1137</v>
       </c>
       <c r="E8" s="52" t="s">
         <v>820</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
   </sheetData>
@@ -18925,8 +18922,8 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21179,7 +21176,7 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
preparing for finally moving to something bigger, and user use.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3323" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3325" uniqueCount="1133">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -4115,7 +4115,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15703,7 +15703,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
@@ -16120,7 +16120,7 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
@@ -16401,7 +16401,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>
@@ -16542,7 +16542,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
@@ -16654,7 +16654,7 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>
@@ -17199,7 +17199,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
@@ -17395,7 +17395,7 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -17579,7 +17579,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -18914,7 +18914,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -19229,7 +19229,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.98"/>
@@ -20012,7 +20012,7 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -21012,7 +21012,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
@@ -21164,11 +21164,11 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
@@ -21977,11 +21977,11 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>
@@ -22122,6 +22122,9 @@
       <c r="D7" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>810</v>
+      </c>
       <c r="F7" s="2" t="n">
         <v>2.2</v>
       </c>
@@ -22141,6 +22144,9 @@
       </c>
       <c r="D8" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>834</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>10</v>
@@ -22194,7 +22200,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>

</xml_diff>

<commit_message>
started some testing, but still not fully implemented.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3325" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3325" uniqueCount="1132">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2814,9 +2814,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ten jest dla broni której masa jest większa niż 7Kg. Umożliwia wygodne (jak na taką kobyłę) przenoszenie broni. Możesz dzięki temu mieć wolne ręce a broń Ci wisi na boku i łatwo Ci ją szybko chwycić (1 faza). Zajmuje slot na plecach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wkłady</t>
   </si>
   <si>
     <t xml:space="preserve">różne_rozmiary</t>
@@ -15721,13 +15718,13 @@
         <v>794</v>
       </c>
       <c r="D1" s="52" t="s">
+        <v>940</v>
+      </c>
+      <c r="E1" s="52" t="s">
         <v>941</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="F1" s="52" t="s">
         <v>942</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>943</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>715</v>
@@ -15737,7 +15734,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>5</v>
@@ -15750,7 +15747,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>692</v>
@@ -15760,14 +15757,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="52" t="s">
+        <v>946</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>947</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>948</v>
       </c>
       <c r="E3" s="52" t="n">
         <v>1</v>
@@ -15776,14 +15773,14 @@
         <v>904</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>10</v>
@@ -15799,21 +15796,21 @@
         <v>849</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="52" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E5" s="52" t="n">
         <v>1</v>
@@ -15822,23 +15819,23 @@
         <v>915</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
+        <v>954</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>955</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>956</v>
       </c>
       <c r="E6" s="52" t="n">
         <v>10</v>
@@ -15847,23 +15844,23 @@
         <v>815</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>957</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>958</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="C7" s="52" t="s">
         <v>959</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>960</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>961</v>
       </c>
       <c r="E7" s="52" t="n">
         <v>50</v>
@@ -15872,23 +15869,23 @@
         <v>908</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>961</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>958</v>
+      </c>
+      <c r="C8" s="52" t="s">
         <v>962</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>959</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>963</v>
-      </c>
       <c r="D8" s="52" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E8" s="52" t="n">
         <v>5</v>
@@ -15897,23 +15894,23 @@
         <v>904</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>964</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>958</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>965</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>959</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>966</v>
-      </c>
       <c r="D9" s="52" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E9" s="52" t="n">
         <v>3</v>
@@ -15929,13 +15926,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>18</v>
@@ -15944,7 +15941,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>698</v>
@@ -15954,16 +15951,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>968</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>958</v>
+      </c>
+      <c r="C11" s="52" t="s">
         <v>969</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>959</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>970</v>
-      </c>
       <c r="D11" s="52" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E11" s="52" t="n">
         <v>5</v>
@@ -16129,19 +16126,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>638</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>794</v>
@@ -16158,22 +16155,22 @@
         <v>750</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>975</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>976</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>959</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>977</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>685</v>
@@ -16181,97 +16178,97 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>978</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>979</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>980</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>981</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>982</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>977</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>984</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>985</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>986</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>959</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>988</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>989</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>990</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>794</v>
@@ -16285,20 +16282,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>995</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>2</v>
@@ -16309,74 +16306,74 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>996</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>982</v>
-      </c>
-      <c r="G8" s="54" t="s">
-        <v>997</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>998</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>999</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
   </sheetData>
@@ -16411,16 +16408,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>1001</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="0" t="s">
         <v>1002</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>1003</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1004</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>643</v>
@@ -16428,7 +16425,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.5</v>
@@ -16443,12 +16440,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -16460,12 +16457,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="0" t="n">
@@ -16475,12 +16472,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C5" s="52" t="n">
         <v>1</v>
@@ -16489,12 +16486,12 @@
         <v>2</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C6" s="52" t="n">
         <v>0.5</v>
@@ -16503,12 +16500,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C7" s="52" t="n">
         <v>1</v>
@@ -16517,7 +16514,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
   </sheetData>
@@ -16550,13 +16547,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>715</v>
@@ -16564,13 +16561,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1014</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="52" t="s">
         <v>1015</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>1016</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>804</v>
@@ -16578,10 +16575,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1017</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>1018</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>815</v>
@@ -16592,38 +16589,38 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1019</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1020</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>1021</v>
-      </c>
       <c r="D4" s="52" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1022</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>1023</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>829</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1024</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>1025</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>901</v>
@@ -16661,10 +16658,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1026</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>1027</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>714</v>
@@ -16675,38 +16672,38 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1028</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>1029</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>849</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>849</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>849</v>
@@ -16717,10 +16714,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>849</v>
@@ -16731,10 +16728,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1034</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>1035</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>866</v>
@@ -16745,13 +16742,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>1036</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>1037</v>
-      </c>
       <c r="C7" s="52" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>706</v>
@@ -16759,10 +16756,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B8" s="52" t="s">
         <v>1038</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>1039</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>915</v>
@@ -16773,13 +16770,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>1040</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>1041</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>706</v>
@@ -16787,24 +16784,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="B10" s="52" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>1043</v>
-      </c>
       <c r="D10" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>1044</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>1045</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>824</v>
@@ -16815,13 +16812,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>706</v>
@@ -16829,10 +16826,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B13" s="52" t="s">
         <v>1047</v>
-      </c>
-      <c r="B13" s="52" t="s">
-        <v>1048</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>908</v>
@@ -16843,13 +16840,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>1049</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>1050</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>706</v>
@@ -16857,13 +16854,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C15" s="52" t="s">
         <v>1051</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>1052</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>706</v>
@@ -16871,13 +16868,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>1053</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="C16" s="52" t="s">
         <v>1054</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>1055</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>701</v>
@@ -16885,24 +16882,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D17" s="52" t="s">
         <v>1056</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>1050</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>1057</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>714</v>
@@ -16913,10 +16910,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>1059</v>
-      </c>
-      <c r="B19" s="52" t="s">
-        <v>1060</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>824</v>
@@ -16927,13 +16924,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>1061</v>
-      </c>
-      <c r="B20" s="52" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>1062</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>706</v>
@@ -16941,10 +16938,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>824</v>
@@ -16955,13 +16952,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D22" s="52" t="s">
         <v>706</v>
@@ -16969,24 +16966,24 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>824</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B24" s="52" t="s">
         <v>1066</v>
-      </c>
-      <c r="B24" s="52" t="s">
-        <v>1067</v>
       </c>
       <c r="C24" s="52" t="s">
         <v>908</v>
@@ -16997,13 +16994,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>1068</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="C25" s="52" t="s">
         <v>1069</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>1070</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>701</v>
@@ -17011,10 +17008,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>824</v>
@@ -17025,10 +17022,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>1072</v>
-      </c>
-      <c r="B27" s="52" t="s">
-        <v>1073</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>866</v>
@@ -17039,10 +17036,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>824</v>
@@ -17053,24 +17050,24 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B29" s="52" t="s">
         <v>1075</v>
       </c>
-      <c r="B29" s="52" t="s">
-        <v>1076</v>
-      </c>
       <c r="C29" s="52" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>1077</v>
-      </c>
-      <c r="B30" s="52" t="s">
-        <v>1078</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>908</v>
@@ -17081,10 +17078,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>824</v>
@@ -17095,13 +17092,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B32" s="52" t="s">
         <v>1080</v>
       </c>
-      <c r="B32" s="52" t="s">
-        <v>1081</v>
-      </c>
       <c r="C32" s="52" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>798</v>
@@ -17109,41 +17106,41 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="52" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B33" s="52" t="s">
         <v>1082</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="C33" s="52" t="s">
         <v>1083</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="D33" s="52" t="s">
         <v>1084</v>
-      </c>
-      <c r="D33" s="52" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="52" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B35" s="52" t="s">
         <v>1087</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="C35" s="52" t="s">
         <v>1088</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>1089</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>804</v>
@@ -17151,10 +17148,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="52" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>1090</v>
-      </c>
-      <c r="B36" s="52" t="s">
-        <v>1091</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>824</v>
@@ -17165,13 +17162,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B37" s="52" t="s">
         <v>1053</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="C37" s="52" t="s">
         <v>1054</v>
-      </c>
-      <c r="C37" s="52" t="s">
-        <v>1055</v>
       </c>
       <c r="D37" s="52" t="s">
         <v>701</v>
@@ -17207,13 +17204,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1092</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>1093</v>
-      </c>
       <c r="C1" s="52" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>643</v>
@@ -17221,13 +17218,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>1094</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>1095</v>
-      </c>
       <c r="C2" s="52" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>798</v>
@@ -17235,58 +17232,58 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>1096</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="C3" s="52" t="s">
         <v>1097</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="D3" s="52" t="s">
         <v>1098</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>1100</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C4" s="52" t="s">
         <v>1101</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="D4" s="52" t="s">
         <v>1102</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>1104</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="C5" s="52" t="s">
         <v>1105</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="D5" s="52" t="s">
         <v>1106</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>1108</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="C6" s="52" t="s">
         <v>1109</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1110</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17399,13 +17396,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>638</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>794</v>
@@ -17419,16 +17416,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="52" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>1115</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>1116</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>819</v>
@@ -17439,19 +17436,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B3" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>685</v>
@@ -17459,19 +17456,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>798</v>
@@ -17479,16 +17476,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E5" s="52" t="s">
         <v>815</v>
@@ -17499,16 +17496,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>958</v>
+      </c>
+      <c r="C6" s="52" t="s">
         <v>1123</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>959</v>
-      </c>
-      <c r="C6" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>1124</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>1125</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>819</v>
@@ -17519,42 +17516,42 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>1126</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>1127</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="E7" s="52" t="s">
         <v>1128</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>1129</v>
-      </c>
       <c r="F7" s="52" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="516.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="52" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>1131</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1132</v>
       </c>
       <c r="E8" s="52" t="s">
         <v>819</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -21978,7 +21975,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21988,16 +21985,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>918</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>919</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>920</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>921</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>794</v>
@@ -22011,7 +22008,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>218</v>
@@ -22031,7 +22028,7 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>218</v>
@@ -22051,13 +22048,13 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>5</v>
@@ -22071,13 +22068,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>5</v>
@@ -22091,7 +22088,7 @@
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>218</v>
@@ -22111,13 +22108,13 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>10</v>
@@ -22134,7 +22131,7 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
@@ -22157,19 +22154,19 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.2</v>
@@ -22207,19 +22204,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>932</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>933</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>934</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>935</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>805</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>714</v>
@@ -22230,13 +22227,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>13</v>
@@ -22253,13 +22250,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>12</v>
@@ -22276,7 +22273,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
bugfix and uniforms ready without camouflage.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3325" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1129">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2858,9 +2858,6 @@
     <t xml:space="preserve">zwiększa wytrzymałość o 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Tarcze</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mod_Unik</t>
   </si>
   <si>
@@ -2972,9 +2969,6 @@
     <t xml:space="preserve">Na 2 godziny redukuje kary z ran do 0 (nie same rany, ale tylko kary do testów z nich wynikające). Skorzystanie wymaga 2 rang w Dyscyplinie Naukowej Medycyna.</t>
   </si>
   <si>
-    <t xml:space="preserve">Radia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Szyfrowanie</t>
   </si>
   <si>
@@ -3137,9 +3131,6 @@
     <t xml:space="preserve">Zawiera śpiwór, menaszki, i wszystko czego potrzebujesz aby rozpalić ogień, i zrobić na nim żarcie, jeśli jakieś upolujesz, (pamiętaj nie masz tego wiele). Za każde 200$ dodaj premię +1 do przyrządzania jedzenia oraz rozbijanie obozu, oraz dodatkowy kilogram masy, a za każde dodatkowe 4 kilogramy dodaj slot zajmowany. Maksymalna premia +10.</t>
   </si>
   <si>
-    <t xml:space="preserve">Użytkowe</t>
-  </si>
-  <si>
     <t xml:space="preserve">objętość</t>
   </si>
   <si>
@@ -3335,9 +3326,6 @@
     <t xml:space="preserve">1 slot,</t>
   </si>
   <si>
-    <t xml:space="preserve">Gotowe_zestawy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Opis</t>
   </si>
   <si>
@@ -3395,9 +3383,6 @@
     <t xml:space="preserve">2040$</t>
   </si>
   <si>
-    <t xml:space="preserve">ubranie</t>
-  </si>
-  <si>
     <t xml:space="preserve">kamuflaze</t>
   </si>
   <si>
@@ -3407,7 +3392,7 @@
     <t xml:space="preserve">leśny, miejski, zimowy, pustynny</t>
   </si>
   <si>
-    <t xml:space="preserve">tani- po każdym brawurowym ruchu (np. przebijanie się przez krzak) rzuć D6. na 1 się rozrywa i przestaje dawać premię do Uniku</t>
+    <t xml:space="preserve">kamuflaż, tani- po każdym brawurowym ruchu (np. przebijanie się przez krzak) rzuć D6. na 1 się rozrywa i przestaje dawać premię do Uniku</t>
   </si>
   <si>
     <t xml:space="preserve">zimnowojenny z demobilu</t>
@@ -3416,12 +3401,15 @@
     <t xml:space="preserve">niepalny, wytrzymały, kamuflaż</t>
   </si>
   <si>
-    <t xml:space="preserve">kontraktowy/ profesjonalny</t>
+    <t xml:space="preserve">kontraktowy</t>
   </si>
   <si>
     <t xml:space="preserve">leśny, miejski, zimowy, pustynny,</t>
   </si>
   <si>
+    <t xml:space="preserve">profesjonalny</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pałatka wojskowa</t>
   </si>
   <si>
@@ -3455,8 +3443,11 @@
     <t xml:space="preserve">Leśny, pustynny,</t>
   </si>
   <si>
-    <t xml:space="preserve">Jeśli jesteś za osłoną naturalną (krzakiem), lub leżysz w wysokiej trawie, krzaku etc, i pozostajesz nieruchomy, to zwiększ premię do Uniku z 3 do 6.
+    <t xml:space="preserve">kamuflaż, Jeśli jesteś za osłoną naturalną (krzakiem), lub leżysz w wysokiej trawie, krzaku etc, i pozostajesz nieruchomy, to zwiększ premię do Uniku z 3 do 6.
 Wyglądasz jak krzak. Jeśli ukrywasz się, masz dodatkowe 3d6 jeśli jesteś w krzaku. Najpierw musisz zdradzić swoja pozycję aby wróg Cię zauważył. Współpracuje jedynie z kamizelką Undershirt, pasami, i szelkami. Wydłuż czasy przeładowania 2-krotnie, chyba że przygotowałeś wcześniej magazynek, i leży on przed tobą.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                 78//////7</t>
   </si>
 </sst>
 </file>
@@ -4108,8 +4099,8 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15697,7 +15688,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15718,13 +15709,13 @@
         <v>794</v>
       </c>
       <c r="D1" s="52" t="s">
+        <v>939</v>
+      </c>
+      <c r="E1" s="52" t="s">
         <v>940</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="F1" s="52" t="s">
         <v>941</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>942</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>715</v>
@@ -15734,7 +15725,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>5</v>
@@ -15747,7 +15738,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>692</v>
@@ -15757,14 +15748,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="52" t="s">
+        <v>945</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>946</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>947</v>
       </c>
       <c r="E3" s="52" t="n">
         <v>1</v>
@@ -15773,14 +15764,14 @@
         <v>904</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>10</v>
@@ -15796,21 +15787,21 @@
         <v>849</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="52" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="E5" s="52" t="n">
         <v>1</v>
@@ -15819,23 +15810,23 @@
         <v>915</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
+        <v>953</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>954</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>955</v>
       </c>
       <c r="E6" s="52" t="n">
         <v>10</v>
@@ -15844,23 +15835,23 @@
         <v>815</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>956</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>957</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="C7" s="52" t="s">
         <v>958</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>959</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>960</v>
       </c>
       <c r="E7" s="52" t="n">
         <v>50</v>
@@ -15869,23 +15860,23 @@
         <v>908</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>960</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>957</v>
+      </c>
+      <c r="C8" s="52" t="s">
         <v>961</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>958</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>962</v>
-      </c>
       <c r="D8" s="52" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E8" s="52" t="n">
         <v>5</v>
@@ -15894,23 +15885,23 @@
         <v>904</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>957</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>964</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>958</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>965</v>
-      </c>
       <c r="D9" s="52" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E9" s="52" t="n">
         <v>3</v>
@@ -15926,13 +15917,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>18</v>
@@ -15941,7 +15932,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>698</v>
@@ -15951,16 +15942,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
+        <v>967</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>957</v>
+      </c>
+      <c r="C11" s="52" t="s">
         <v>968</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>958</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>969</v>
-      </c>
       <c r="D11" s="52" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="E11" s="52" t="n">
         <v>5</v>
@@ -16114,7 +16105,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16126,19 +16117,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>970</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>638</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>794</v>
@@ -16155,22 +16146,22 @@
         <v>750</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>685</v>
@@ -16178,97 +16169,97 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>977</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>978</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>979</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>980</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>981</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>976</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>983</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>984</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>794</v>
@@ -16282,20 +16273,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>2</v>
@@ -16306,74 +16297,74 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
   </sheetData>
@@ -16394,8 +16385,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16408,16 +16399,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>998</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>999</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>1000</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="E1" s="2" t="s">
         <v>1001</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1003</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>643</v>
@@ -16425,7 +16416,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.5</v>
@@ -16440,12 +16431,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -16457,12 +16448,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="0" t="n">
@@ -16472,12 +16463,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="C5" s="52" t="n">
         <v>1</v>
@@ -16486,12 +16477,12 @@
         <v>2</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C6" s="52" t="n">
         <v>0.5</v>
@@ -16500,12 +16491,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="C7" s="52" t="n">
         <v>1</v>
@@ -16514,7 +16505,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
   </sheetData>
@@ -16547,13 +16538,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>715</v>
@@ -16561,13 +16552,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C2" s="52" t="s">
         <v>1013</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>1014</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>1015</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>804</v>
@@ -16575,10 +16566,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>815</v>
@@ -16589,38 +16580,38 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C4" s="52" t="s">
         <v>1018</v>
       </c>
-      <c r="B4" s="52" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>1020</v>
-      </c>
       <c r="D4" s="52" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>829</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>901</v>
@@ -16648,7 +16639,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16658,10 +16649,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>714</v>
@@ -16672,38 +16663,38 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>849</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>849</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>849</v>
@@ -16714,10 +16705,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>849</v>
@@ -16728,10 +16719,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>866</v>
@@ -16742,13 +16733,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>706</v>
@@ -16756,10 +16747,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>915</v>
@@ -16770,13 +16761,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>706</v>
@@ -16784,24 +16775,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>824</v>
@@ -16812,13 +16803,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>706</v>
@@ -16826,10 +16817,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>908</v>
@@ -16840,13 +16831,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>706</v>
@@ -16854,13 +16845,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>706</v>
@@ -16868,13 +16859,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>701</v>
@@ -16882,24 +16873,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>714</v>
@@ -16910,10 +16901,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>824</v>
@@ -16924,13 +16915,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>706</v>
@@ -16938,10 +16929,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>824</v>
@@ -16952,13 +16943,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="D22" s="52" t="s">
         <v>706</v>
@@ -16966,24 +16957,24 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>824</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="C24" s="52" t="s">
         <v>908</v>
@@ -16994,13 +16985,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>701</v>
@@ -17008,10 +16999,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>824</v>
@@ -17022,10 +17013,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="B27" s="52" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>866</v>
@@ -17036,10 +17027,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>824</v>
@@ -17050,24 +17041,24 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="B29" s="52" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="B30" s="52" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>908</v>
@@ -17078,10 +17069,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>824</v>
@@ -17092,13 +17083,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>798</v>
@@ -17106,41 +17097,41 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="52" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C33" s="52" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D33" s="52" t="s">
         <v>1081</v>
-      </c>
-      <c r="B33" s="52" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C33" s="52" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D33" s="52" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="52" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>804</v>
@@ -17148,10 +17139,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="52" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>824</v>
@@ -17162,13 +17153,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="D37" s="52" t="s">
         <v>701</v>
@@ -17193,7 +17184,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17204,13 +17195,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1091</v>
+        <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>643</v>
@@ -17218,13 +17209,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>798</v>
@@ -17232,58 +17223,58 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17386,23 +17377,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1111</v>
+        <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>638</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>794</v>
@@ -17416,16 +17407,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>819</v>
@@ -17436,19 +17427,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1116</v>
+        <v>1111</v>
       </c>
       <c r="B3" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1117</v>
+        <v>1112</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>685</v>
@@ -17456,19 +17447,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1118</v>
+        <v>1113</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1119</v>
+        <v>1114</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1117</v>
+        <v>1112</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>798</v>
@@ -17476,39 +17467,39 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1119</v>
+        <v>1114</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1121</v>
+        <v>1112</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>815</v>
+        <v>1013</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>685</v>
+        <v>798</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>958</v>
+        <v>1116</v>
+      </c>
+      <c r="B6" s="52" t="n">
+        <v>4</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1123</v>
+        <v>1114</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1124</v>
+        <v>1117</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>685</v>
@@ -17516,42 +17507,67 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B7" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>819</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="52" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B8" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="52" t="s">
         <v>1125</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="52" t="s">
+      <c r="B9" s="52" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>1126</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D9" s="2" t="s">
         <v>1127</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E9" s="52" t="s">
+        <v>819</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
         <v>1128</v>
-      </c>
-      <c r="F7" s="52" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="516.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="52" t="s">
-        <v>1129</v>
-      </c>
-      <c r="B8" s="52" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1131</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>819</v>
-      </c>
-      <c r="F8" s="52" t="s">
-        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -21974,7 +21990,7 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -22194,7 +22210,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22204,19 +22220,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>932</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>933</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>934</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>805</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>714</v>
@@ -22227,7 +22243,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>5</v>
@@ -22250,13 +22266,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>12</v>
@@ -22273,7 +22289,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
added test about reloading.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1128">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -3399,9 +3399,6 @@
   </si>
   <si>
     <t xml:space="preserve">niepalny, wytrzymały, kamuflaż</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kontraktowy</t>
   </si>
   <si>
     <t xml:space="preserve">leśny, miejski, zimowy, pustynny,</t>
@@ -16385,7 +16382,7 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -17379,7 +17376,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -17447,13 +17444,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1113</v>
+        <v>957</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>1112</v>
@@ -17467,13 +17464,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D5" s="52" t="s">
         <v>1112</v>
@@ -17487,16 +17484,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>815</v>
@@ -17507,16 +17504,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B7" s="52" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="52" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D7" s="52" t="s">
         <v>1119</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>1120</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>819</v>
@@ -17527,19 +17524,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="52" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D8" s="52" t="s">
         <v>1122</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="E8" s="52" t="s">
         <v>1123</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>1124</v>
       </c>
       <c r="F8" s="52" t="s">
         <v>947</v>
@@ -17547,16 +17544,16 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B9" s="52" t="n">
         <v>3</v>
       </c>
       <c r="C9" s="52" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>1126</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1127</v>
       </c>
       <c r="E9" s="52" t="s">
         <v>819</v>
@@ -17567,7 +17564,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more tests about reloading.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1129">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -3399,6 +3399,9 @@
   </si>
   <si>
     <t xml:space="preserve">niepalny, wytrzymały, kamuflaż</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kontraktowy</t>
   </si>
   <si>
     <t xml:space="preserve">leśny, miejski, zimowy, pustynny,</t>
@@ -4100,7 +4103,7 @@
       <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15688,11 +15691,9 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16105,11 +16106,9 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16386,10 +16385,7 @@
       <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -16527,10 +16523,9 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16639,10 +16634,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -17184,10 +17176,9 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17377,10 +17368,10 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -17444,13 +17435,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>957</v>
+        <v>1113</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>1112</v>
@@ -17464,13 +17455,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="D5" s="52" t="s">
         <v>1112</v>
@@ -17484,16 +17475,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>815</v>
@@ -17504,16 +17495,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B7" s="52" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>819</v>
@@ -17524,19 +17515,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="F8" s="52" t="s">
         <v>947</v>
@@ -17544,16 +17535,16 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="B9" s="52" t="n">
         <v>3</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="E9" s="52" t="s">
         <v>819</v>
@@ -17564,7 +17555,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
     </row>
   </sheetData>
@@ -17589,7 +17580,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -18924,7 +18915,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -19239,7 +19230,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.98"/>
@@ -20022,7 +20013,7 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -21022,7 +21013,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
@@ -21178,10 +21169,9 @@
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21991,10 +21981,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
@@ -22210,10 +22197,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">

</xml_diff>

<commit_message>
apteczki i leczenie zrobione.
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="1130">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -2877,6 +2877,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ciężka Militarna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b             </t>
   </si>
   <si>
     <t xml:space="preserve">zajmowane_miejsce</t>
@@ -4099,11 +4102,11 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E213" activeCellId="0" sqref="E213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -15691,9 +15694,11 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15707,13 +15712,13 @@
         <v>794</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>715</v>
@@ -15723,7 +15728,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>5</v>
@@ -15736,7 +15741,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>692</v>
@@ -15746,14 +15751,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="52" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E3" s="52" t="n">
         <v>1</v>
@@ -15762,14 +15767,14 @@
         <v>904</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>10</v>
@@ -15785,21 +15790,21 @@
         <v>849</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="52" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E5" s="52" t="n">
         <v>1</v>
@@ -15808,23 +15813,23 @@
         <v>915</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="E6" s="52" t="n">
         <v>10</v>
@@ -15833,23 +15838,23 @@
         <v>815</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="E7" s="52" t="n">
         <v>50</v>
@@ -15858,23 +15863,23 @@
         <v>908</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
+        <v>961</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>958</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>962</v>
+      </c>
+      <c r="D8" s="52" t="s">
         <v>960</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>957</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>961</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>959</v>
       </c>
       <c r="E8" s="52" t="n">
         <v>5</v>
@@ -15883,23 +15888,23 @@
         <v>904</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="E9" s="52" t="n">
         <v>3</v>
@@ -15915,13 +15920,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>18</v>
@@ -15930,7 +15935,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>698</v>
@@ -15940,16 +15945,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E11" s="52" t="n">
         <v>5</v>
@@ -16106,9 +16111,11 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16119,13 +16126,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>638</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>794</v>
@@ -16142,22 +16149,22 @@
         <v>750</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>685</v>
@@ -16165,97 +16172,97 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>794</v>
@@ -16269,20 +16276,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>2</v>
@@ -16293,74 +16300,74 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>993</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>992</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>997</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>996</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
   </sheetData>
@@ -16385,23 +16392,26 @@
       <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>643</v>
@@ -16409,7 +16419,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.5</v>
@@ -16424,12 +16434,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -16441,12 +16451,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="0" t="n">
@@ -16456,12 +16466,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C5" s="52" t="n">
         <v>1</v>
@@ -16470,12 +16480,12 @@
         <v>2</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C6" s="52" t="n">
         <v>0.5</v>
@@ -16484,12 +16494,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C7" s="52" t="n">
         <v>1</v>
@@ -16498,7 +16508,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
   </sheetData>
@@ -16523,20 +16533,21 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>715</v>
@@ -16544,13 +16555,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>804</v>
@@ -16558,10 +16569,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>815</v>
@@ -16572,38 +16583,38 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>829</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>901</v>
@@ -16634,14 +16645,17 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>714</v>
@@ -16652,38 +16666,38 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>849</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>849</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>849</v>
@@ -16694,10 +16708,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>849</v>
@@ -16708,10 +16722,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>866</v>
@@ -16722,13 +16736,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>706</v>
@@ -16736,10 +16750,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>915</v>
@@ -16750,13 +16764,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B9" s="52" t="s">
         <v>1036</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>1035</v>
-      </c>
       <c r="C9" s="52" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>706</v>
@@ -16764,24 +16778,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>824</v>
@@ -16792,13 +16806,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>706</v>
@@ -16806,10 +16820,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="52" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>908</v>
@@ -16820,13 +16834,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="52" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>706</v>
@@ -16834,13 +16848,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>706</v>
@@ -16848,13 +16862,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="52" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>701</v>
@@ -16862,24 +16876,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>714</v>
@@ -16890,10 +16904,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>824</v>
@@ -16904,13 +16918,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>706</v>
@@ -16918,10 +16932,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>824</v>
@@ -16932,13 +16946,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="D22" s="52" t="s">
         <v>706</v>
@@ -16946,24 +16960,24 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>824</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C24" s="52" t="s">
         <v>908</v>
@@ -16974,13 +16988,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>701</v>
@@ -16988,10 +17002,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>824</v>
@@ -17002,10 +17016,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="52" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B27" s="52" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>866</v>
@@ -17016,10 +17030,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>824</v>
@@ -17030,24 +17044,24 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B29" s="52" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B30" s="52" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>908</v>
@@ -17058,10 +17072,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>824</v>
@@ -17072,13 +17086,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>798</v>
@@ -17086,41 +17100,41 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="52" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="52" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>804</v>
@@ -17128,10 +17142,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="52" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>824</v>
@@ -17142,13 +17156,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D37" s="52" t="s">
         <v>701</v>
@@ -17176,9 +17190,10 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17186,10 +17201,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>643</v>
@@ -17197,13 +17212,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>798</v>
@@ -17211,58 +17226,58 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17367,11 +17382,11 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -17381,7 +17396,7 @@
         <v>638</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="D1" s="52" t="s">
         <v>794</v>
@@ -17395,16 +17410,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>819</v>
@@ -17415,19 +17430,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B3" s="52" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>685</v>
@@ -17435,19 +17450,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>798</v>
@@ -17455,19 +17470,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="F5" s="52" t="s">
         <v>798</v>
@@ -17475,16 +17490,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>4</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>815</v>
@@ -17495,16 +17510,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B7" s="52" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>819</v>
@@ -17515,47 +17530,47 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="527.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B9" s="52" t="n">
         <v>3</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="E9" s="52" t="s">
         <v>819</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
   </sheetData>
@@ -17580,7 +17595,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -18915,7 +18930,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -19230,7 +19245,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.98"/>
@@ -20013,7 +20028,7 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -21013,7 +21028,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
@@ -21165,13 +21180,14 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21981,7 +21997,10 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
@@ -22191,13 +22210,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
@@ -22289,6 +22311,11 @@
       </c>
       <c r="G4" s="2" t="n">
         <v>15000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="s">
+        <v>939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wydawanie i dostawanie kasy
</commit_message>
<xml_diff>
--- a/TabelaBroni.xlsx
+++ b/TabelaBroni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="bron" sheetId="1" state="visible" r:id="rId2"/>
@@ -4102,11 +4102,11 @@
   </sheetPr>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E213" activeCellId="0" sqref="E213"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.56"/>
@@ -4125,7 +4125,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="16" style="0" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15694,7 +15694,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
@@ -16111,7 +16111,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
@@ -16388,11 +16388,11 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>
@@ -16533,7 +16533,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
@@ -16645,7 +16645,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>
@@ -17190,7 +17190,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
@@ -17386,7 +17386,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
@@ -17591,11 +17591,11 @@
   </sheetPr>
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -18930,7 +18930,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.98"/>
   </cols>
@@ -19241,11 +19241,11 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.98"/>
@@ -20028,7 +20028,7 @@
       <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -21028,7 +21028,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
@@ -21184,7 +21184,7 @@
       <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="11.61"/>
@@ -21997,7 +21997,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>
@@ -22216,7 +22216,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.61"/>
   </cols>

</xml_diff>